<commit_message>
Refactored expandclause SPARQL generation as became too complex
</commit_message>
<xml_diff>
--- a/odata2sparql.v4/src/test/resources/GetTests.xlsx
+++ b/odata2sparql.v4/src/test/resources/GetTests.xlsx
@@ -3287,7 +3287,7 @@
     <t xml:space="preserve">V2.3</t>
   </si>
   <si>
-    <t xml:space="preserve">$filter=contains('SEVES',subjectId)</t>
+    <t xml:space="preserve">$filter=contains('10664',subjectId)</t>
   </si>
   <si>
     <t xml:space="preserve">V2.4</t>
@@ -3598,8 +3598,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H47" activeCellId="0" sqref="H47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F187" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H218" activeCellId="0" sqref="H218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added support for lambdaAll
</commit_message>
<xml_diff>
--- a/odata2sparql.v4/src/test/resources/GetTests.xlsx
+++ b/odata2sparql.v4/src/test/resources/GetTests.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="717">
   <si>
     <t xml:space="preserve">Group</t>
   </si>
@@ -95,354 +95,6 @@
   </si>
   <si>
     <t xml:space="preserve">$expand=rdf_facts($expand=rdf_terms,rdf_property)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource(rdf_facts(rdf_property(),rdf_terms()))/$entity","comment":null,"label":"OrderDetail-10250-51","subjectId":"NWD~OrderDetail-10250-51","rdf_facts":[{"comment":null,"label":null,"propertyId":"rdfs~label","subjectId":"NWD~OrderDetail-10250-51-4f75ce12336ab89a4edebd807cd62265","rdf_property":{"comment":"","label":"label","subjectId":"rdfs~label"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"OrderDetail-10250-51","resourceId":null,"subjectId":"NWD~OrderDetail-10250-51-4f75ce12336ab89a4edebd807cd62265-311f0cc52cba0a21070961879f9173c8"}]},{"comment":null,"label":null,"propertyId":"northwind~discount","subjectId":"NWD~OrderDetail-10250-51-560ff6ef546ba93e36c161c0d4dce072","rdf_property":{"comment":"","label":"discount","subjectId":"northwind~discount"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"0.15","resourceId":null,"subjectId":"NWD~OrderDetail-10250-51-560ff6ef546ba93e36c161c0d4dce072-9ffc7a03c1959674fa8c0a7369460097"}]},{"comment":null,"label":null,"propertyId":"northwind~order","subjectId":"NWD~OrderDetail-10250-51-7849cdb0ec5319c5c3c71d9bff0672b0","rdf_property":{"comment":"","label":"is part of order","subjectId":"northwind~order"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/Order-10250","resourceId":null,"subjectId":"NWD~OrderDetail-10250-51-7849cdb0ec5319c5c3c71d9bff0672b0-b6b2d84f8259c3db3fb89c10ce920509"}]},{"comment":null,"label":null,"propertyId":"northwind~product","subjectId":"NWD~OrderDetail-10250-51-9f79a810fc71f8d74ecbb8bb013bed9c","rdf_property":{"comment":"","label":"includes product","subjectId":"northwind~product"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/Product-51","resourceId":null,"subjectId":"NWD~OrderDetail-10250-51-9f79a810fc71f8d74ecbb8bb013bed9c-46a5bfba2bbe33d1a6e41ac2f23216b1"}]},{"comment":null,"label":null,"propertyId":"northwind~quantity","subjectId":"NWD~OrderDetail-10250-51-9fc1ed06938066abace0a241064b728b","rdf_property":{"comment":"","label":"quantity","subjectId":"northwind~quantity"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"35","resourceId":null,"subjectId":"NWD~OrderDetail-10250-51-9fc1ed06938066abace0a241064b728b-1c383cd30b7c298ab50293adfecb7b18"}]},{"comment":null,"label":null,"propertyId":"rdf~type","subjectId":"NWD~OrderDetail-10250-51-c74e2b735dd8dc85ad0ee3510c33925f","rdf_property":{"comment":"","label":"type","subjectId":"rdf~type"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/model/OrderDetail","resourceId":null,"subjectId":"NWD~OrderDetail-10250-51-c74e2b735dd8dc85ad0ee3510c33925f-1c1c9eee9ed5045311df73136e39de22"}]},{"comment":null,"label":null,"propertyId":"northwind~orderDetailUnitPrice","subjectId":"NWD~OrderDetail-10250-51-f42cdd44e43333f6f7b46b4988d2a2f6","rdf_property":{"comment":"","label":"unit price","subjectId":"northwind~orderDetailUnitPrice"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"42.4","resourceId":null,"subjectId":"NWD~OrderDetail-10250-51-f42cdd44e43333f6f7b46b4988d2a2f6-8a622231ebe8e6ec3b0e654c589717d3"}]}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource/facts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rdfs_Resource('NWD~OrderDetail-10250-51')/rdf_facts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource('NWD~OrderDetail-10250-51')/rdf_facts","value":[{"comment":null,"label":"discount","propertyId":null,"subjectId":"northwind~discount"},{"comment":null,"label":"is part of order","propertyId":null,"subjectId":"northwind~order"},{"comment":null,"label":"unit price","propertyId":null,"subjectId":"northwind~orderDetailUnitPrice"},{"comment":null,"label":"includes product","propertyId":null,"subjectId":"northwind~product"},{"comment":null,"label":"quantity","propertyId":null,"subjectId":"northwind~quantity"},{"comment":null,"label":null,"propertyId":null,"subjectId":"rdfs~label"},{"comment":null,"label":null,"propertyId":null,"subjectId":"rdf~type"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource/facts,expandTermsProperty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$expand=rdf_terms,rdf_property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource('NWD~OrderDetail-10250-51')/rdf_facts(rdf_property(),rdf_terms())","value":[{"comment":"","label":"discount","propertyId":"northwind~discount","subjectId":"northwind~discount","rdf_property":{"comment":"","label":"discount","subjectId":"northwind~discount"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"0.15","resourceId":null,"subjectId":"northwind~discount-9ffc7a03c1959674fa8c0a7369460097"}]},{"comment":"","label":"is part of order","propertyId":"northwind~order","subjectId":"northwind~order","rdf_property":{"comment":"","label":"is part of order","subjectId":"northwind~order"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/Order-10250","resourceId":null,"subjectId":"northwind~order-b6b2d84f8259c3db3fb89c10ce920509"}]},{"comment":"","label":"unit price","propertyId":"northwind~orderDetailUnitPrice","subjectId":"northwind~orderDetailUnitPrice","rdf_property":{"comment":"","label":"unit price","subjectId":"northwind~orderDetailUnitPrice"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"42.4","resourceId":null,"subjectId":"northwind~orderDetailUnitPrice-8a622231ebe8e6ec3b0e654c589717d3"}]},{"comment":"","label":"includes product","propertyId":"northwind~product","subjectId":"northwind~product","rdf_property":{"comment":"","label":"includes product","subjectId":"northwind~product"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/Product-51","resourceId":null,"subjectId":"northwind~product-46a5bfba2bbe33d1a6e41ac2f23216b1"}]},{"comment":"","label":"quantity","propertyId":"northwind~quantity","subjectId":"northwind~quantity","rdf_property":{"comment":"","label":"quantity","subjectId":"northwind~quantity"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"35","resourceId":null,"subjectId":"northwind~quantity-1c383cd30b7c298ab50293adfecb7b18"}]},{"comment":"","label":"label","propertyId":"rdfs~label","subjectId":"rdfs~label","rdf_property":{"comment":"","label":"label","subjectId":"rdfs~label"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"OrderDetail-10250-51","resourceId":null,"subjectId":"rdfs~label-311f0cc52cba0a21070961879f9173c8"}]},{"comment":"","label":"type","propertyId":"rdf~type","subjectId":"rdf~type","rdf_property":{"comment":"","label":"type","subjectId":"rdf~type"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/model/OrderDetail","resourceId":null,"subjectId":"rdf~type-1c1c9eee9ed5045311df73136e39de22"}]}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource/fact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rdfs_Resource('NWD~OrderDetail-10250-51')/rdf_facts('northwind~product')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource/$entity","comment":null,"label":"includes product","propertyId":null,"subjectId":"northwind~product"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource/fact,expandTermsProperty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource(rdf_property(),rdf_terms())/$entity","comment":"","label":"includes product","propertyId":"northwind~product","subjectId":"northwind~product","rdf_property":{"comment":"","label":"includes product","subjectId":"northwind~product"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/Product-51","resourceId":null,"subjectId":"northwind~product-46a5bfba2bbe33d1a6e41ac2f23216b1"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource/fact/terms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rdfs_Resource('NWD~OrderDetail-10250-51')/rdf_facts('northwind~product')/rdf_terms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource('NWD~OrderDetail-10250-51')/rdf_facts('northwind~product')/rdf_terms","value":[{"comment":null,"label":"Product-51","rdf_literal":"Product-51","rdf_object":"Product-51","resourceId":"","subjectId":"NWD~Product-51"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rdfs_Resource('NWD~Employee-2')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource/$entity","comment":null,"label":"Employee-2","subjectId":"NWD~Employee-2"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource,expandIsObjectOf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$expand=rdf_isObjectOf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource(rdf_isObjectOf())/$entity","comment":null,"label":"Employee-2","subjectId":"NWD~Employee-2","rdf_isObjectOf":[{"comment":null,"isPropertyOfId":null,"label":null,"subjectId":"northwind~employee-183be8a27387eafb4f11fc9e9ea98950"},{"comment":null,"isPropertyOfId":null,"label":null,"subjectId":"northwind~reportsTo-183be8a27387eafb4f11fc9e9ea98950"},{"comment":null,"isPropertyOfId":null,"label":null,"subjectId":"rdf~subject-183be8a27387eafb4f11fc9e9ea98950"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource,expandIsObjectOfSubject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$expand=rdf_isObjectOf($expand=rdf_isPropertyOf,rdf_subjects)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Too large</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource/isObjectofs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rdfs_Resource('NWD~Employee-2')/rdf_isObjectOf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource('NWD~Employee-2')/rdf_isObjectOf","value":[{"comment":null,"isPropertyOfId":null,"label":"is managed by","subjectId":"northwind~employee"},{"comment":null,"isPropertyOfId":null,"label":"reports to employee","subjectId":"northwind~reportsTo"},{"comment":null,"isPropertyOfId":null,"label":null,"subjectId":"rdf~subject"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource/isObjectofs,expandSubjectsProperty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$expand=rdf_subjects,rdf_isPropertyOf&amp;$top=2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource('NWD~Employee-2')/rdf_isObjectOf(rdf_isPropertyOf(),rdf_subjects())","value":[{"comment":null,"isPropertyOfId":"northwind~reportsTo","label":"reports to employee","subjectId":"northwind~reportsTo","rdf_isPropertyOf":{"comment":null,"label":"reports to employee","subjectId":"northwind~reportsTo"},"rdf_subjects":[{"comment":null,"label":"Employee-1","subjectId":"NWD~Employee-1"},{"comment":null,"label":"Employee-8","subjectId":"NWD~Employee-8"}]}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource/isObjectof</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rdfs_Resource('NWD~Employee-2')/rdf_isObjectOf('northwind~reportsTo')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource/$entity","comment":null,"isPropertyOfId":null,"label":"reports to employee","subjectId":"northwind~reportsTo"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource/isObjectof,expandSubjects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$expand=rdf_subjects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource(rdf_subjects())/$entity","comment":null,"isPropertyOfId":null,"label":"reports to employee","subjectId":"northwind~reportsTo","rdf_subjects":[{"comment":null,"label":"Employee-1","subjectId":"NWD~Employee-1"},{"comment":null,"label":"Employee-3","subjectId":"NWD~Employee-3"},{"comment":null,"label":"Employee-4","subjectId":"NWD~Employee-4"},{"comment":null,"label":"Employee-5","subjectId":"NWD~Employee-5"},{"comment":null,"label":"Employee-8","subjectId":"NWD~Employee-8"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource/isObjectof/subjects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rdfs_Resource('NWD~Employee-2')/rdf_isObjectOf('northwind~reportsTo')/rdf_subjects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource('NWD~Employee-2')/rdf_isObjectOf('northwind~reportsTo')/rdf_subjects","value":[{"comment":null,"label":"Employee-1","subjectId":"NWD~Employee-1"},{"comment":null,"label":"Employee-3","subjectId":"NWD~Employee-3"},{"comment":null,"label":"Employee-4","subjectId":"NWD~Employee-4"},{"comment":null,"label":"Employee-5","subjectId":"NWD~Employee-5"},{"comment":null,"label":"Employee-8","subjectId":"NWD~Employee-8"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Segmentpaths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Path1.EntitySet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$top=5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee","value":[{"birthDate":"1968-12-08","comment":null,"employeeAddress":"507 - 20th Ave. E.\\nApt. 2A","employeeCity":"Seattle","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98122","employeeSalary":null,"employer":null,"extension":"5467","favorite":null,"firstName":"Nancy","hireDate":"2012-05-01","homePhone":"(206) 555-9857","label":"Employee-1","lastName":"Davolio","lat":47.6234778,"lat_long":"47.6234778,-122.3063220","long":-122.306322,"notes":"Education includes a BA in psychology from Colorado State University in 1970. She also completed The Art of the Cold Call. Nancy is a member of Toastmasters International.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-1","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Ms."},{"birthDate":"1972-02-19","comment":null,"employeeAddress":"908 W. Capital Way","employeeCity":"Tacoma","employeeCountry":"USA","employeeLinkedIn":"https://www.linkedin.com/in/peterjohnlawrence/","employeePostalCode":"98401","employeeSalary":null,"employer":null,"extension":"3457","favorite":null,"firstName":"Andrew","hireDate":"2012-08-14","homePhone":"(206) 555-9482","label":"Employee-2","lastName":"Fuller","lat":38.972057,"lat_long":"38.9720570,-77.0268860","long":-77.026886,"notes":"Andrew received his BTS commercial in 1974 and a Ph.D. in international marketing from the University of Dallas in 1981. He is fluent in French and Italian and reads German. He joined the company as a sales representative, was promoted to sales manager in January 1992 and to vice president of sales in March 1993. Andrew is a member of the Sales Management Roundtable, the Seattle Chamber of Commerce, and the Pacific Rim Importers Association.","photo":"http://accweb/emmployees/fuller.bmp","regionDescription":null,"reportsToId":null,"reportsToNotation":null,"subjectId":"NWD~Employee-2","territoryNotation":null,"title":"Vice President, Sales","titleOfCourtesy":"Dr."},{"birthDate":"1975-03-04","comment":null,"employeeAddress":"14 Garrett Hill","employeeCity":"London","employeeCountry":"UK","employeeLinkedIn":null,"employeePostalCode":"SW1 8JR","employeeSalary":null,"employer":null,"extension":"3453","favorite":null,"firstName":"Steven","hireDate":"2013-10-17","homePhone":"(71) 555-4848","label":"Employee-5","lastName":"Buchanan","lat":51.5239508,"lat_long":"51.5239508,-0.0944701","long":-0.0944701,"notes":"Steven Buchanan graduated from St. Andrews University, Scotland, with a BSC degree in 1976. Upon joining the company as a sales representative in 1992, he spent 6 months in an orientation program at the Seattle office and then returned to his permanent post in London. He was promoted to sales manager in March 1993. Mr. Buchanan has completed the courses Successful Telemarketing and International Sales Management. He is fluent in French.","photo":"http://accweb/emmployees/buchanan.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-5","territoryNotation":null,"title":"Sales Manager","titleOfCourtesy":"Mr."},{"birthDate":"1978-01-09","comment":null,"employeeAddress":"4726 - 11th Ave. N.E.","employeeCity":"Seattle","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98105","employeeSalary":null,"employer":null,"extension":"2344","favorite":null,"firstName":"Laura","hireDate":"2014-03-05","homePhone":"(206) 555-1189","label":"Employee-8","lastName":"Callahan","lat":47.6641642,"lat_long":"47.6641642,-122.3160149","long":-122.3160149,"notes":"Laura received a BA in psychology from the University of Washington. She has also completed a course in business French. She reads and writes French.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-8","territoryNotation":null,"title":"Inside Sales Coordinator","titleOfCourtesy":"Ms."},{"birthDate":"1986-01-27","comment":null,"employeeAddress":"7 Houndstooth Rd.","employeeCity":"London","employeeCountry":"UK","employeeLinkedIn":null,"employeePostalCode":"WG2 7LT","employeeSalary":null,"employer":null,"extension":"452","favorite":null,"firstName":"Anne","hireDate":"2014-11-15","homePhone":"(71) 555-4444","label":"Employee-9","lastName":"Dodsworth","lat":51.5073509,"lat_long":"51.5073509,-0.1277583","long":-0.1277583,"notes":"Anne has a BA degree in English from St. Lawrence College. She is fluent in French and German.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-5","reportsToNotation":null,"subjectId":"NWD~Employee-9","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Ms."}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Path1.Entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee('NWD~Employee-2')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee/$entity","birthDate":"1972-02-19","comment":null,"employeeAddress":"908 W. Capital Way","employeeCity":"Tacoma","employeeCountry":"USA","employeeLinkedIn":"https://www.linkedin.com/in/peterjohnlawrence/","employeePostalCode":"98401","employeeSalary":null,"employer":null,"extension":"3457","favorite":null,"firstName":"Andrew","hireDate":"2012-08-14","homePhone":"(206) 555-9482","label":"Employee-2","lastName":"Fuller","lat":38.972057,"lat_long":"38.9720570,-77.0268860","long":-77.026886,"notes":"Andrew received his BTS commercial in 1974 and a Ph.D. in international marketing from the University of Dallas in 1981. He is fluent in French and Italian and reads German. He joined the company as a sales representative, was promoted to sales manager in January 1992 and to vice president of sales in March 1993. Andrew is a member of the Sales Management Roundtable, the Seattle Chamber of Commerce, and the Pacific Rim Importers Association.","photo":"http://accweb/emmployees/fuller.bmp","regionDescription":null,"reportsToId":null,"reportsToNotation":null,"subjectId":"NWD~Employee-2","territoryNotation":null,"title":"Vice President, Sales","titleOfCourtesy":"Dr."}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Path2.EntitySet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$select=subjectId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~Employee-2')/managesOrder(subjectId)","value":[{"subjectId":"NWD~Order-10265"},{"subjectId":"NWD~Order-10277"},{"subjectId":"NWD~Order-10280"},{"subjectId":"NWD~Order-10295"},{"subjectId":"NWD~Order-10300"},{"subjectId":"NWD~Order-10307"},{"subjectId":"NWD~Order-10312"},{"subjectId":"NWD~Order-10313"},{"subjectId":"NWD~Order-10327"},{"subjectId":"NWD~Order-10339"},{"subjectId":"NWD~Order-10345"},{"subjectId":"NWD~Order-10368"},{"subjectId":"NWD~Order-10379"},{"subjectId":"NWD~Order-10388"},{"subjectId":"NWD~Order-10392"},{"subjectId":"NWD~Order-10398"},{"subjectId":"NWD~Order-10404"},{"subjectId":"NWD~Order-10407"},{"subjectId":"NWD~Order-10414"},{"subjectId":"NWD~Order-10422"},{"subjectId":"NWD~Order-10457"},{"subjectId":"NWD~Order-10462"},{"subjectId":"NWD~Order-10471"},{"subjectId":"NWD~Order-10478"},{"subjectId":"NWD~Order-10487"},{"subjectId":"NWD~Order-10502"},{"subjectId":"NWD~Order-10515"},{"subjectId":"NWD~Order-10516"},{"subjectId":"NWD~Order-10541"},{"subjectId":"NWD~Order-10552"},{"subjectId":"NWD~Order-10553"},{"subjectId":"NWD~Order-10556"},{"subjectId":"NWD~Order-10561"},{"subjectId":"NWD~Order-10563"},{"subjectId":"NWD~Order-10583"},{"subjectId":"NWD~Order-10588"},{"subjectId":"NWD~Order-10595"},{"subjectId":"NWD~Order-10615"},{"subjectId":"NWD~Order-10620"},{"subjectId":"NWD~Order-10657"},{"subjectId":"NWD~Order-10663"},{"subjectId":"NWD~Order-10669"},{"subjectId":"NWD~Order-10673"},{"subjectId":"NWD~Order-10676"},{"subjectId":"NWD~Order-10683"},{"subjectId":"NWD~Order-10686"},{"subjectId":"NWD~Order-10691"},{"subjectId":"NWD~Order-10727"},{"subjectId":"NWD~Order-10734"},{"subjectId":"NWD~Order-10737"},{"subjectId":"NWD~Order-10738"},{"subjectId":"NWD~Order-10752"},{"subjectId":"NWD~Order-10780"},{"subjectId":"NWD~Order-10781"},{"subjectId":"NWD~Order-10787"},{"subjectId":"NWD~Order-10798"},{"subjectId":"NWD~Order-10805"},{"subjectId":"NWD~Order-10808"},{"subjectId":"NWD~Order-10810"},{"subjectId":"NWD~Order-10815"},{"subjectId":"NWD~Order-10819"},{"subjectId":"NWD~Order-10832"},{"subjectId":"NWD~Order-10846"},{"subjectId":"NWD~Order-10858"},{"subjectId":"NWD~Order-10865"},{"subjectId":"NWD~Order-10912"},{"subjectId":"NWD~Order-10915"},{"subjectId":"NWD~Order-10919"},{"subjectId":"NWD~Order-10939"},{"subjectId":"NWD~Order-10949"},{"subjectId":"NWD~Order-10967"},{"subjectId":"NWD~Order-10971"},{"subjectId":"NWD~Order-10982"},{"subjectId":"NWD~Order-10983"},{"subjectId":"NWD~Order-10985"},{"subjectId":"NWD~Order-10989"},{"subjectId":"NWD~Order-10990"},{"subjectId":"NWD~Order-10994"},{"subjectId":"NWD~Order-11000"},{"subjectId":"NWD~Order-11001"},{"subjectId":"NWD~Order-11005"},{"subjectId":"NWD~Order-11009"},{"subjectId":"NWD~Order-11010"},{"subjectId":"NWD~Order-11013"},{"subjectId":"NWD~Order-11014"},{"subjectId":"NWD~Order-11015"},{"subjectId":"NWD~Order-11020"},{"subjectId":"NWD~Order-11028"},{"subjectId":"NWD~Order-11032"},{"subjectId":"NWD~Order-11035"},{"subjectId":"NWD~Order-11042"},{"subjectId":"NWD~Order-11053"},{"subjectId":"NWD~Order-11059"},{"subjectId":"NWD~Order-11060"},{"subjectId":"NWD~Order-11070"},{"subjectId":"NWD~Order-11073"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Path2.Entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee('NWD~Employee-5')/reportsTo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~Employee-5')/reportsTo/$entity","birthDate":"1972-02-19","comment":null,"employeeAddress":"908 W. Capital Way","employeeCity":"Tacoma","employeeCountry":"USA","employeeLinkedIn":"https://www.linkedin.com/in/peterjohnlawrence/","employeePostalCode":"98401","employeeSalary":null,"employer":null,"extension":"3457","favorite":null,"firstName":"Andrew","hireDate":"2012-08-14","homePhone":"(206) 555-9482","label":"Employee-2","lastName":"Fuller","lat":38.972057,"lat_long":"38.9720570,-77.0268860","long":-77.026886,"notes":"Andrew received his BTS commercial in 1974 and a Ph.D. in international marketing from the University of Dallas in 1981. He is fluent in French and Italian and reads German. He joined the company as a sales representative, was promoted to sales manager in January 1992 and to vice president of sales in March 1993. Andrew is a member of the Sales Management Roundtable, the Seattle Chamber of Commerce, and the Pacific Rim Importers Association.","photo":"http://accweb/emmployees/fuller.bmp","regionDescription":null,"reportsToId":null,"reportsToNotation":null,"subjectId":"NWD~Employee-2","territoryNotation":null,"title":"Vice President, Sales","titleOfCourtesy":"Dr."}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee/$entity","comment":null,"customerId":"NWD~Customer-BLONP","customerNotation":null,"employeeId":"NWD~Employee-2","employeeNotation":null,"freight":55.279999,"label":"Order-10265","lat":48.5835085,"lat_long":"48.5835085,7.7446960","long":7.744696,"orderDate":"2016-07-25T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-08-22T00:00:00Z","shipAddress":"24, place Kléber","shipCity":"Strasbourg","shipCountry":"France","shipName":"Blondel père et fils","shipPostalCode":"67000","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2016-08-12T00:00:00Z","subjectId":"NWD~Order-10265"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Path3.EntitySet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail","value":[{"comment":null,"discount":0.0,"label":"OrderDetail-10265-17","orderDetailUnitPrice":31.2,"orderId":"NWD~Order-10265","orderNotation":null,"productId":"NWD~Product-17","productNotation":null,"quantity":30,"subjectId":"NWD~OrderDetail-10265-17"},{"comment":null,"discount":0.0,"label":"OrderDetail-10265-70","orderDetailUnitPrice":12.0,"orderId":"NWD~Order-10265","orderNotation":null,"productId":"NWD~Product-70","productNotation":null,"quantity":20,"subjectId":"NWD~OrderDetail-10265-70"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Path3.Entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/customer/$entity","comment":null,"customerAddress":"24, place Kléber","customerCity":"Strasbourg","customerCompanyName":"Blondesddsl père et fils","customerContactName":"Frédérique Citeaux","customerContactTitle":"Marketing Manager","customerCountry":"France","customerFax":"88.60.15.32","customerPhone":"88.60.15.31","customerPostalCode":"67000","customerWebsite":null,"label":"Blondesddsl père et fils","lat":48.5835085,"lat_long":"48.5835085,7.7446960","long":7.744696,"regionDescription":null,"subjectId":"NWD~Customer-BLONP"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail('NWD~OrderDetail-10265-17')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee/$entity","comment":null,"discount":0.0,"label":"OrderDetail-10265-17","orderDetailUnitPrice":31.2,"orderId":"NWD~Order-10265","orderNotation":null,"productId":"NWD~Product-17","productNotation":null,"quantity":30,"subjectId":"NWD~OrderDetail-10265-17"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Path4.Entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail('NWD~OrderDetail-10265-17')/product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail('NWD~OrderDetail-10265-17')/product/$entity","categoryId":"NWD~Category-6","categoryNotation":null,"comment":null,"discontinued":true,"label":"Product-17","productName":"Alice Mutton","productUnitPrice":39.0,"quantityPerUnit":"20 - 1 kg tins","reorderLevel":0,"subjectId":"NWD~Product-17","supplierId":"NWD~Supplier-7","supplierNotation":null,"unitCommission":null,"unitsInStock":0,"unitsOnOrder":0}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Path5.Entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail('NWD~OrderDetail-10265-17')/product/supplier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail('NWD~OrderDetail-10265-17')/product/supplier/$entity","comment":null,"homePage":null,"label":"Supplier-7","lat":-37.741888,"lat_long":"-37.7418880,144.9475730","long":144.947573,"regionDescription":null,"subjectId":"NWD~Supplier-7","supplierAddress":"74 Rose St. Moonie Ponds","supplierCity":"Melbourne","supplierCompanyName":"Pavlova, Ltd.","supplierContactName":"Ian Devling","supplierContactTitle":"Marketing Manager","supplierCountry":"Australia","supplierFax":null,"supplierHomePage":null,"supplierPhone":"(03) 444-2343","supplierPostalCode":"3058"}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Path6.Entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail('NWD~OrderDetail-10265-17')/product/supplier/suppliesProduct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail('NWD~OrderDetail-10265-17')/product/supplier/suppliesProduct","value":[{"categoryId":"NWD~Category-3","categoryNotation":null,"comment":null,"discontinued":false,"label":"Product-16","productName":"Pavlova","productUnitPrice":17.45,"quantityPerUnit":"32 - 500 g boxes","reorderLevel":10,"subjectId":"NWD~Product-16","supplierId":"NWD~Supplier-7","supplierNotation":null,"unitCommission":null,"unitsInStock":29,"unitsOnOrder":0},{"categoryId":"NWD~Category-6","categoryNotation":null,"comment":null,"discontinued":true,"label":"Product-17","productName":"Alice Mutton","productUnitPrice":39.0,"quantityPerUnit":"20 - 1 kg tins","reorderLevel":0,"subjectId":"NWD~Product-17","supplierId":"NWD~Supplier-7","supplierNotation":null,"unitCommission":null,"unitsInStock":0,"unitsOnOrder":0},{"categoryId":"NWD~Category-8","categoryNotation":null,"comment":null,"discontinued":false,"label":"Product-18","productName":"Carnarvon Tigers","productUnitPrice":62.5,"quantityPerUnit":"16 kg pkg.","reorderLevel":0,"subjectId":"NWD~Product-18","supplierId":"NWD~Supplier-7","supplierNotation":null,"unitCommission":null,"unitsInStock":42,"unitsOnOrder":0},{"categoryId":"NWD~Category-2","categoryNotation":null,"comment":null,"discontinued":false,"label":"Product-63","productName":"Vegie-spread","productUnitPrice":43.9,"quantityPerUnit":"15 - 625 g jars","reorderLevel":5,"subjectId":"NWD~Product-63","supplierId":"NWD~Supplier-7","supplierNotation":null,"unitCommission":null,"unitsInStock":24,"unitsOnOrder":0},{"categoryId":"NWD~Category-1","categoryNotation":null,"comment":null,"discontinued":false,"label":"Product-70","productName":"Outback Lager","productUnitPrice":15.0,"quantityPerUnit":"24 - 355 ml bottles","reorderLevel":30,"subjectId":"NWD~Product-70","supplierId":"NWD~Supplier-7","supplierNotation":null,"unitCommission":null,"unitsInStock":15,"unitsOnOrder":10}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProxyOLGAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">olgap_ShortestPath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODATA2SPARQL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service=%27tfl%27&amp;start=londontube~Euston&amp;end=londontube~Baker_Street&amp;propertyPath=%27(tfl~connectsFrom)!(rdf~type%7Ctfl~connectsTo)%5E!(rdf~type%7Ctfl~hasStationInZone%7Ctfl~hasStationOnLine%7Ctfl~connectsFrom)%5E(rdf~type)%27&amp;maxPath=8&amp;$orderby=edge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_ShortestPath","value":[{"direct":true,"edge":1,"maxPath":null,"object":"londontube~Kings_Cross_St._Pancras","property":"tfl~connectsFrom","propertyPath":null,"subject":"londontube~Euston"},{"direct":true,"edge":2,"maxPath":null,"object":"londontube~Euston_Square","property":"tfl~connectsFrom","propertyPath":null,"subject":"londontube~Kings_Cross_St._Pancras"},{"direct":false,"edge":3,"maxPath":null,"object":"londontube~Great_Portland_Street","property":"tfl~connectsFrom","propertyPath":null,"subject":"londontube~Euston_Square"},{"direct":false,"edge":4,"maxPath":null,"object":"londontube~Baker_Street","property":"tfl~connectsFrom","propertyPath":null,"subject":"londontube~Great_Portland_Street"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service=%22tfl%22&amp;start=londontube~Goldhawk_Road&amp;end=londontube~Tower_Hill&amp;propertyPath=%22!(rdf~type%7Ctfl~connectsFrom%7Ctfl~onLine%7Ctfl~inZone)%5E!(rdf~type%7Ctfl~hasStationInZone%7Ctfl~hasStationOnLine)%22&amp;maxPath=20&amp;$select=direct,object,property,subject&amp;$expand=olgap_object($select=label),olgap_subject($select=label),olgap_property($select=label,subjectId)&amp;$orderby=edge&amp;bidirectional=true&amp;$skip=0&amp;$top=20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_ShortestPath(direct,object,property,subject,olgap_object(label,subjectId),olgap_property(label,subjectId),olgap_subject(label,subjectId))","value":[{"direct":true,"object":"londontube~Shepherds_Bush_Market","property":"tfl~connectsTo","subject":"londontube~Goldhawk_Road","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Shepherds_Bush_Market')","label":"Shepherds Bush Market","subjectId":"londontube~Shepherds_Bush_Market"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Goldhawk_Road')","label":"Goldhawk Road","subjectId":"londontube~Goldhawk_Road"}},{"direct":true,"object":"londontube~Wood_Lane","property":"tfl~connectsTo","subject":"londontube~Shepherds_Bush_Market","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Wood_Lane')","label":"Wood Lane","subjectId":"londontube~Wood_Lane"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Shepherds_Bush_Market')","label":"Shepherds Bush Market","subjectId":"londontube~Shepherds_Bush_Market"}},{"direct":true,"object":"londontube~Latimer_Road","property":"tfl~connectsTo","subject":"londontube~Wood_Lane","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Latimer_Road')","label":"Latimer Road","subjectId":"londontube~Latimer_Road"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Wood_Lane')","label":"Wood Lane","subjectId":"londontube~Wood_Lane"}},{"direct":true,"object":"londontube~Ladbroke_Grove","property":"tfl~connectsTo","subject":"londontube~Latimer_Road","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Ladbroke_Grove')","label":"Ladbroke Grove","subjectId":"londontube~Ladbroke_Grove"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Latimer_Road')","label":"Latimer Road","subjectId":"londontube~Latimer_Road"}},{"direct":true,"object":"londontube~Westbourne_Park","property":"tfl~connectsTo","subject":"londontube~Ladbroke_Grove","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Westbourne_Park')","label":"Westbourne Park","subjectId":"londontube~Westbourne_Park"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Ladbroke_Grove')","label":"Ladbroke Grove","subjectId":"londontube~Ladbroke_Grove"}},{"direct":true,"object":"londontube~Royal_Oak","property":"tfl~connectsTo","subject":"londontube~Westbourne_Park","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Royal_Oak')","label":"Royal Oak","subjectId":"londontube~Royal_Oak"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Westbourne_Park')","label":"Westbourne Park","subjectId":"londontube~Westbourne_Park"}},{"direct":true,"object":"londontube~Paddington","property":"tfl~connectsTo","subject":"londontube~Royal_Oak","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Paddington')","label":"Paddington","subjectId":"londontube~Paddington"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Royal_Oak')","label":"Royal Oak","subjectId":"londontube~Royal_Oak"}},{"direct":true,"object":"londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29","property":"tfl~connectsTo","subject":"londontube~Paddington","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29')","label":"Edgware Road (Circle/District/Hammersmith and City)","subjectId":"londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Paddington')","label":"Paddington","subjectId":"londontube~Paddington"}},{"direct":true,"object":"londontube~Baker_Street","property":"tfl~connectsTo","subject":"londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Baker_Street')","label":"Baker Street","subjectId":"londontube~Baker_Street"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29')","label":"Edgware Road (Circle/District/Hammersmith and City)","subjectId":"londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29"}},{"direct":true,"object":"londontube~Bond_Street","property":"tfl~connectsTo","subject":"londontube~Baker_Street","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Bond_Street')","label":"Bond Street","subjectId":"londontube~Bond_Street"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Baker_Street')","label":"Baker Street","subjectId":"londontube~Baker_Street"}},{"direct":true,"object":"londontube~Green_Park","property":"tfl~connectsTo","subject":"londontube~Bond_Street","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Green_Park')","label":"Green Park","subjectId":"londontube~Green_Park"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Bond_Street')","label":"Bond Street","subjectId":"londontube~Bond_Street"}},{"direct":true,"object":"londontube~Westminster","property":"tfl~connectsTo","subject":"londontube~Green_Park","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Westminster')","label":"Westminster","subjectId":"londontube~Westminster"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Green_Park')","label":"Green Park","subjectId":"londontube~Green_Park"}},{"direct":true,"object":"londontube~Waterloo","property":"tfl~connectsTo","subject":"londontube~Westminster","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Waterloo')","label":"Waterloo","subjectId":"londontube~Waterloo"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Westminster')","label":"Westminster","subjectId":"londontube~Westminster"}},{"direct":true,"object":"londontube~Bank","property":"tfl~connectsTo","subject":"londontube~Waterloo","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Bank')","label":"Bank","subjectId":"londontube~Bank"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Waterloo')","label":"Waterloo","subjectId":"londontube~Waterloo"}},{"direct":false,"object":"londontube~Liverpool_Street","property":"tfl~connectsTo","subject":"londontube~Bank","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Liverpool_Street')","label":"Liverpool Street","subjectId":"londontube~Liverpool_Street"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Bank')","label":"Bank","subjectId":"londontube~Bank"}},{"direct":false,"object":"londontube~Aldgate","property":"tfl~connectsTo","subject":"londontube~Liverpool_Street","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Aldgate')","label":"Aldgate","subjectId":"londontube~Aldgate"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Liverpool_Street')","label":"Liverpool Street","subjectId":"londontube~Liverpool_Street"}},{"direct":true,"object":"londontube~Tower_Hill","property":"tfl~connectsTo","subject":"londontube~Aldgate","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Tower_Hill')","label":"Tower Hill","subjectId":"londontube~Tower_Hill"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Aldgate')","label":"Aldgate","subjectId":"londontube~Aldgate"}}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service=%27northwind%27&amp;start=NWD~Customer-PRINI&amp;end=NWD~Product-29&amp;propertyPath=%27!(rdf~type)%5E!(rdf~type)%27&amp;maxPath=15&amp;$orderby=edge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_ShortestPath","value":[{"direct":false,"edge":1,"maxPath":null,"object":"NWD~Order-11007","property":"northwind~customer","propertyPath":null,"subject":"NWD~Customer-PRINI"},{"direct":false,"edge":2,"maxPath":null,"object":"NWD~OrderDetail-11007-29","property":"northwind~order","propertyPath":null,"subject":"NWD~Order-11007"},{"direct":true,"edge":3,"maxPath":null,"object":"NWD~Product-29","property":"northwind~product","propertyPath":null,"subject":"NWD~OrderDetail-11007-29"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service=%27northwind%27&amp;start=NWD~Order-10477&amp;end=NWD~Order-10491&amp;propertyPath=%27!(rdf~type)%5E!(rdf~type)%27&amp;maxPath=15&amp;$orderby=edge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_ShortestPath","value":[{"direct":true,"edge":1,"maxPath":null,"object":"NWD~Employee-5","property":"northwind~employee","propertyPath":null,"subject":"NWD~Order-10477"},{"direct":true,"edge":2,"maxPath":null,"object":"NWD~Employee-2","property":"northwind~reportsTo","propertyPath":null,"subject":"NWD~Employee-5"},{"direct":false,"edge":3,"maxPath":null,"object":"NWD~Employee-8","property":"northwind~reportsTo","propertyPath":null,"subject":"NWD~Employee-2"},{"direct":false,"edge":4,"maxPath":null,"object":"NWD~Order-10491","property":"northwind~employee","propertyPath":null,"subject":"NWD~Employee-8"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">olgap_Triangles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service=%27tfl%27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_Triangles","value":[{"triangles":2491,"trianglesService":"j0~tfl"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">olgap_DegreeDistribution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service=%27tfl%27&amp;$orderby=degree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_DegreeDistribution","value":[{"count":3827,"degree":1,"degreeDistributionService":"UNDEF"},{"count":701,"degree":2,"degreeDistributionService":"UNDEF"},{"count":4,"degree":3,"degreeDistributionService":"UNDEF"},{"count":17,"degree":4,"degreeDistributionService":"UNDEF"},{"count":6,"degree":5,"degreeDistributionService":"UNDEF"},{"count":2,"degree":7,"degreeDistributionService":"UNDEF"},{"count":3,"degree":9,"degreeDistributionService":"UNDEF"},{"count":3,"degree":11,"degreeDistributionService":"UNDEF"},{"count":1,"degree":13,"degreeDistributionService":"UNDEF"},{"count":1,"degree":14,"degreeDistributionService":"UNDEF"},{"count":37,"degree":16,"degreeDistributionService":"UNDEF"},{"count":334,"degree":18,"degreeDistributionService":"UNDEF"},{"count":76,"degree":20,"degreeDistributionService":"UNDEF"},{"count":1,"degree":21,"degreeDistributionService":"UNDEF"},{"count":34,"degree":22,"degreeDistributionService":"UNDEF"},{"count":80,"degree":24,"degreeDistributionService":"UNDEF"},{"count":30,"degree":26,"degreeDistributionService":"UNDEF"},{"count":2,"degree":27,"degreeDistributionService":"UNDEF"},{"count":13,"degree":28,"degreeDistributionService":"UNDEF"},{"count":2,"degree":29,"degreeDistributionService":"UNDEF"},{"count":12,"degree":30,"degreeDistributionService":"UNDEF"},{"count":7,"degree":32,"degreeDistributionService":"UNDEF"},{"count":5,"degree":34,"degreeDistributionService":"UNDEF"},{"count":3,"degree":36,"degreeDistributionService":"UNDEF"},{"count":3,"degree":38,"degreeDistributionService":"UNDEF"},{"count":2,"degree":42,"degreeDistributionService":"UNDEF"},{"count":1,"degree":44,"degreeDistributionService":"UNDEF"},{"count":2,"degree":45,"degreeDistributionService":"UNDEF"},{"count":1,"degree":48,"degreeDistributionService":"UNDEF"},{"count":1,"degree":49,"degreeDistributionService":"UNDEF"},{"count":1,"degree":50,"degreeDistributionService":"UNDEF"},{"count":1,"degree":52,"degreeDistributionService":"UNDEF"},{"count":1,"degree":53,"degreeDistributionService":"UNDEF"},{"count":1,"degree":57,"degreeDistributionService":"UNDEF"},{"count":1,"degree":61,"degreeDistributionService":"UNDEF"},{"count":1,"degree":67,"degreeDistributionService":"UNDEF"},{"count":1,"degree":69,"degreeDistributionService":"UNDEF"},{"count":1,"degree":73,"degreeDistributionService":"UNDEF"},{"count":1,"degree":81,"degreeDistributionService":"UNDEF"},{"count":1,"degree":91,"degreeDistributionService":"UNDEF"},{"count":1,"degree":93,"degreeDistributionService":"UNDEF"},{"count":1,"degree":101,"degreeDistributionService":"UNDEF"},{"count":1,"degree":103,"degreeDistributionService":"UNDEF"},{"count":1,"degree":107,"degreeDistributionService":"UNDEF"},{"count":1,"degree":109,"degreeDistributionService":"UNDEF"},{"count":1,"degree":123,"degreeDistributionService":"UNDEF"},{"count":1,"degree":137,"degreeDistributionService":"UNDEF"},{"count":1,"degree":145,"degreeDistributionService":"UNDEF"},{"count":1,"degree":163,"degreeDistributionService":"UNDEF"},{"count":1,"degree":203,"degreeDistributionService":"UNDEF"},{"count":1,"degree":215,"degreeDistributionService":"UNDEF"},{"count":1,"degree":225,"degreeDistributionService":"UNDEF"},{"count":1,"degree":299,"degreeDistributionService":"UNDEF"},{"count":1,"degree":305,"degreeDistributionService":"UNDEF"},{"count":1,"degree":353,"degreeDistributionService":"UNDEF"},{"count":1,"degree":1295,"degreeDistributionService":"UNDEF"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">olgap_Eccentricity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service=%27tfl%27&amp;subject=londontube~Baker_Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">olgap_ConnectedComponents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">olgap_PageRank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProxySearch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">search_EntitySearch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service=%22northwind%22&amp;string=%22isabel%20AND%20portugal%22&amp;$orderby=entity&amp;$select=entity,formattedValue,type&amp;$expand=search_entity($select=label,subjectId)&amp;$skip=0&amp;$top=20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#search_EntitySearch(entity,formattedValue,type,search_entity(label,subjectId))","value":[{"entity":"NWD~Customer-PRINI","formattedValue":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;company name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;label:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;contact name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Isabel&lt;/B&gt; de Castro&lt;/td&gt;&lt;/tr&gt;","type":"northwind~Customer","search_entity":{"label":"Princesa Isabel Vinhos","subjectId":"NWD~Customer-PRINI"}},{"entity":"NWD~Order-10336","formattedValue":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;ship name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","type":"northwind~Order","search_entity":{"label":"Order-10336","subjectId":"NWD~Order-10336"}},{"entity":"NWD~Order-10397","formattedValue":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;ship name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","type":"northwind~Order","search_entity":{"label":"Order-10397","subjectId":"NWD~Order-10397"}},{"entity":"NWD~Order-10433","formattedValue":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;ship name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","type":"northwind~Order","search_entity":{"label":"Order-10433","subjectId":"NWD~Order-10433"}},{"entity":"NWD~Order-10477","formattedValue":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;ship name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","type":"northwind~Order","search_entity":{"label":"Order-10477","subjectId":"NWD~Order-10477"}},{"entity":"NWD~Order-11007","formattedValue":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;ship name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","type":"northwind~Order","search_entity":{"label":"Order-11007","subjectId":"NWD~Order-11007"}}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">search_LinkedSearch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service=%22northwind%22&amp;subjectA=NWD~Customer-ANTON&amp;stringB=%22Geitost%22&amp;$select=entityA,entityB,formattedValueB,i10,i21,i32,i43,i54,i65,node1,node2,node3,node4,node5,p01,p12,p23,p34,p45,p56,type1,type2,type3,type4,type5,typeA,typeB&amp;$skip=0&amp;$top=3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#search_LinkedSearch(entityA,entityB,formattedValueB,i10,i21,i32,i43,i54,i65,node1,node2,node3,node4,node5,p01,p12,p23,p34,p45,p56,type1,type2,type3,type4,type5,typeA,typeB)","value":[{"entityA":"NWD~Customer-ANTON","entityB":"NWD~Product-33","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;product name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Geitost&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","i10":"northwind~customer","i21":"UNDEF","i32":"northwind~customer","i43":"northwind~order","i54":"UNDEF","i65":"UNDEF","node1":"NWD~Order-10365","node2":"NWD~Customer-ANTON","node3":"NWD~Order-10677","node4":"NWD~OrderDetail-10677-33","node5":"UNDEF","p01":"UNDEF","p12":"northwind~customer","p23":"UNDEF","p34":"UNDEF","p45":"northwind~product","p56":"UNDEF","type1":"northwind~Order","type2":"northwind~Customer","type3":"northwind~Order","type4":"northwind~OrderDetail","type5":"UNDEF","typeA":"UNDEF","typeB":"northwind~Product"},{"entityA":"NWD~Customer-ANTON","entityB":"NWD~Product-33","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;product name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Geitost&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","i10":"northwind~customer","i21":"UNDEF","i32":"northwind~customer","i43":"northwind~order","i54":"UNDEF","i65":"UNDEF","node1":"NWD~Order-10365","node2":"NWD~Customer-ANTON","node3":"NWD~Order-10682","node4":"NWD~OrderDetail-10682-33","node5":"UNDEF","p01":"UNDEF","p12":"northwind~customer","p23":"UNDEF","p34":"UNDEF","p45":"northwind~product","p56":"UNDEF","type1":"northwind~Order","type2":"northwind~Customer","type3":"northwind~Order","type4":"northwind~OrderDetail","type5":"UNDEF","typeA":"UNDEF","typeB":"northwind~Product"},{"entityA":"NWD~Customer-ANTON","entityB":"NWD~Product-33","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;product name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Geitost&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","i10":"northwind~customer","i21":"UNDEF","i32":"UNDEF","i43":"northwind~orderRegion","i54":"northwind~order","i65":"UNDEF","node1":"NWD~Order-10365","node2":"NWD~Employee-3","node3":"NWD~Region-4306a04670067b5b27e766335d3d40fa","node4":"NWD~Order-10269","node5":"NWD~OrderDetail-10269-33","p01":"UNDEF","p12":"northwind~employee","p23":"northwind~employeeRegion","p34":"UNDEF","p45":"UNDEF","p56":"northwind~product","type1":"northwind~Order","type2":"northwind~Employee","type3":"northwind~Region","type4":"northwind~Order","type5":"northwind~OrderDetail","typeA":"UNDEF","typeB":"northwind~Product"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">search_PathSearch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service=%22northwind%22&amp;subjectA=NWD~Customer-ANTON&amp;stringB=%22Geitost%22&amp;propertyPath=%27!(rdf~type)%5E!(rdf~type)%27&amp;maxPath=20&amp;$select=entityA,entityB,formattedValueB,edge,subject,property,direct,object&amp;$top=1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#search_PathSearch(direct,edge,entityA,entityB,formattedValueB,object,property,subject,typeA,typeB)","value":[{"@odata.id":"search_PathSearch(entityA='NWD~Customer-ANTON',entityB='NWD~Product-33',object='NWD~OrderDetail-10682-33',property='northwind~order',subject='NWD~Order-10682',typeA='UNDEF',typeB='northwind~Product')","direct":false,"edge":2,"entityA":"NWD~Customer-ANTON","entityB":"NWD~Product-33","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;product name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Geitost&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","object":"NWD~OrderDetail-10682-33","property":"northwind~order","subject":"NWD~Order-10682","typeA":"UNDEF","typeB":"northwind~Product"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">search_LinkedEntitySearch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service=%22northwind%22&amp;stringA=%22isabel%22&amp;stringB=%22portugal%22&amp;$select=entityA,entityB,formattedValueA,formattedValueB,i10,i21,i32,i43,i54,i65,node1,node2,node3,node4,node5,p01,p12,p23,p34,p45,p56,type1,type2,type3,type4,type5,typeA,typeB&amp;$skip=0&amp;$top=3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#search_LinkedEntitySearch(entityA,entityB,formattedValueA,formattedValueB,i10,i21,i32,i43,i54,i65,node1,node2,node3,node4,node5,p01,p12,p23,p34,p45,p56,type1,type2,type3,type4,type5,typeA,typeB)","value":[{"entityA":"NWD~Customer-PRINI","entityB":"NWD~Order-11007","formattedValueA":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;company name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","i10":"northwind~customer","i21":"UNDEF","i32":"northwind~customer","i43":"UNDEF","i54":"northwind~customer","i65":"UNDEF","node1":"NWD~Order-10336","node2":"NWD~Customer-PRINI","node3":"NWD~Order-10336","node4":"NWD~Customer-PRINI","node5":"UNDEF","p01":"UNDEF","p12":"northwind~customer","p23":"UNDEF","p34":"northwind~customer","p45":"UNDEF","p56":"UNDEF","type1":"northwind~Order","type2":"northwind~Customer","type3":"northwind~Order","type4":"northwind~Customer","type5":"UNDEF","typeA":"northwind~Customer","typeB":"northwind~Order"},{"entityA":"NWD~Customer-PRINI","entityB":"NWD~Order-11007","formattedValueA":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;company name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","i10":"northwind~customer","i21":"UNDEF","i32":"northwind~customer","i43":"UNDEF","i54":"UNDEF","i65":"UNDEF","node1":"NWD~Order-10336","node2":"NWD~Customer-PRINI","node3":"UNDEF","node4":"UNDEF","node5":"UNDEF","p01":"UNDEF","p12":"northwind~customer","p23":"UNDEF","p34":"UNDEF","p45":"UNDEF","p56":"UNDEF","type1":"northwind~Order","type2":"northwind~Customer","type3":"UNDEF","type4":"UNDEF","type5":"UNDEF","typeA":"northwind~Customer","typeB":"northwind~Order"},{"entityA":"NWD~Customer-PRINI","entityB":"NWD~Order-11007","formattedValueA":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;company name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","i10":"northwind~customer","i21":"UNDEF","i32":"UNDEF","i43":"UNDEF","i54":"UNDEF","i65":"UNDEF","node1":"UNDEF","node2":"UNDEF","node3":"UNDEF","node4":"UNDEF","node5":"UNDEF","p01":"UNDEF","p12":"UNDEF","p23":"UNDEF","p34":"UNDEF","p45":"UNDEF","p56":"UNDEF","type1":"UNDEF","type2":"UNDEF","type3":"UNDEF","type4":"UNDEF","type5":"UNDEF","typeA":"northwind~Customer","typeB":"northwind~Order"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">search_PathEntitySearch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service=%22northwind%22&amp;stringA=%22isabel%22&amp;stringB=%22portugal%22&amp;propertyPath=%27!(rdf~type)%5E!(rdf~type)%27&amp;maxPath=20&amp;$select=entityA,formattedValueA,entityB,formattedValueB,edge,subject,property,direct,object&amp;$top=1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#search_PathEntitySearch(direct,edge,entityA,entityB,formattedValueA,formattedValueB,object,property,subject,typeA,typeB)","value":[{"@odata.id":"search_PathEntitySearch(entityA='NWD~Order-10477',entityB='NWD~Order-10491',object='NWD~Employee-2',property='northwind~reportsTo',subject='NWD~Employee-5',typeA='northwind~Order',typeB='northwind~Order')","direct":true,"edge":2,"entityA":"NWD~Order-10477","entityB":"NWD~Order-10491","formattedValueA":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","object":"NWD~Employee-2","property":"northwind~reportsTo","subject":"NWD~Employee-5","typeA":"northwind~Order","typeB":"northwind~Order"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProxyContextmenu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contextmenu_Count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service=%22northwind%22&amp;subject=NWD~OrderDetail-10255-16&amp;$select=count,property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#contextmenu_Count(count,entity,property)","value":[{"@odata.id":"contextmenu_Count(entity='NWD~OrderDetail-10255-16',property='northwind~product')","count":1,"entity":"NWD~OrderDetail-10255-16","property":"northwind~product"},{"@odata.id":"contextmenu_Count(entity='NWD~OrderDetail-10255-16',property='northwind~order')","count":1,"entity":"NWD~OrderDetail-10255-16","property":"northwind~order"},{"@odata.id":"contextmenu_Count(entity='NWD~OrderDetail-10255-16',property='rdf~type')","count":1,"entity":"NWD~OrderDetail-10255-16","property":"rdf~type"}]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contextmenu_Types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service=%22northwind%22&amp;subject=NWD~OrderDetail-10255-16</t>
   </si>
   <si>
     <r>
@@ -452,7 +104,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#contextmenu_</t>
+      <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource(rdf_facts(rdf_property(),rdf_terms()))/$entity","comment":null,"label":"OrderDetail-10250-51","subjectId":"NWD~OrderDetail-10250-51","rdf_facts":[{"comment":null,"label":null,"propertyId":"rdfs~label","subjectId":"NWD~OrderDetail-10250-51-4f75ce12336ab89a4edebd807cd62265","rdf_property":{"comment":"","label":"label","subjectId":"rdfs~label"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":</t>
     </r>
     <r>
       <rPr>
@@ -460,16 +112,582 @@
         <color rgb="FFFF0000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Types","value":[{"entity":"NWD~OrderDetail-10255-16","type":"rdfs~Resource"},{"entity":"NWD~OrderDetail-10255-16","type":"northwind~OrderDetail</t>
+      <t xml:space="preserve">"OrderDetail-10250-51","rdf_object":"OrderDetail-10250-51","resourceId":null,"subjectId":"NWD~OrderDetail-10250-51-4f75ce12336ab89a4edebd807cd62265-311f0cc52cba0a21070961879f9173c8"}]},{"comment":null,"label":null,"propertyId":"northwind~discount","subjectId":"NWD~OrderDetail-10250-51-560ff6ef546ba93e36c161c0d4dce072","rdf_property":{"comment":"","label":"discount","subjectId":"northwind~discount"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":"0.15","rdf_object":"0.15","resourceId":null,"subjectId":"NWD~OrderDetail-10250-51-560ff6ef546ba93e36c161c0d4dce072-9ffc7a03c1959674fa8c0a7369460097"}]},{"comment":null,"label":null,"propertyId":"northwind~order","subjectId":"NWD~OrderDetail-10250-51-7849cdb0ec5319c5c3c71d9bff0672b0","rdf_property":{"comment":"","label":"is part of order","subjectId":"northwind~order"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/Order-10250","resourceId":"NWD~Order-10250","subjectId":"NWD~OrderDetail-10250-51-7849cdb0ec5319c5c3c71d9bff0672b0-b6b2d84f8259c3db3fb89c10ce920509"}]},{"comment":null,"label":null,"propertyId":"northwind~product","subjectId":"NWD~OrderDetail-10250-51-9f79a810fc71f8d74ecbb8bb013bed9c","rdf_property":{"comment":"","label":"includes product","subjectId":"northwind~product"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/Product-51","resourceId":"NWD~Product-51","subjectId":"NWD~OrderDetail-10250-51-9f79a810fc71f8d74ecbb8bb013bed9c-46a5bfba2bbe33d1a6e41ac2f23216b1"}]},{"comment":null,"label":null,"propertyId":"northwind~quantity","subjectId":"NWD~OrderDetail-10250-51-9fc1ed06938066abace0a241064b728b","rdf_property":{"comment":"","label":"quantity","subjectId":"northwind~quantity"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":"35","rdf_object":"35","resourceId":null,"subjectId":"NWD~OrderDetail-10250-51-9fc1ed06938066abace0a241064b728b-1c383cd30b7c298ab50293adfecb7b18"}]},{"comment":null,"label":null,"propertyId":"rdf~type","subjectId":"NWD~OrderDetail-10250-51-c74e2b735dd8dc85ad0ee3510c33925f","rdf_property":{"comment":"","label":"type","subjectId":"rdf~type"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/model/OrderDetail","resourceId":"northwind~OrderDetail","subjectId":"NWD~OrderDetail-10250-51-c74e2b735dd8dc85ad0ee3510c33925f-1c1c9eee9ed5045311df73136e39de22"}]},{"comment":null,"label":null,"propertyId":"northwind~orderDetailUnitPrice","subjectId":"NWD~OrderDetail-10250-51-f42cdd44e43333f6f7b46b4988d2a2f6","rdf_property":{"comment":"","label":"unit price","subjectId":"northwind~orderDetailUnitPrice"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":"42.4"</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Consolas"/>
         <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">,"rdf_object":"42.4","resourceId":null,"subjectId":"NWD~OrderDetail-10250-51-f42cdd44e43333f6f7b46b4988d2a2f6-8a622231ebe8e6ec3b0e654c589717d3"}]}]}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource/facts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdfs_Resource('NWD~OrderDetail-10250-51')/rdf_facts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource('NWD~OrderDetail-10250-51')/rdf_facts","value":[{"comment":null,"label":"discount","propertyId":null,"subjectId":"northwind~discount"},{"comment":null,"label":"is part of order","propertyId":null,"subjectId":"northwind~order"},{"comment":null,"label":"unit price","propertyId":null,"subjectId":"northwind~orderDetailUnitPrice"},{"comment":null,"label":"includes product","propertyId":null,"subjectId":"northwind~product"},{"comment":null,"label":"quantity","propertyId":null,"subjectId":"northwind~quantity"},{"comment":null,"label":null,"propertyId":null,"subjectId":"rdfs~label"},{"comment":null,"label":null,"propertyId":null,"subjectId":"rdf~type"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource/facts,expandTermsProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$expand=rdf_terms,rdf_property</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource('NWD~OrderDetail-10250-51')/rdf_facts(rdf_property(),rdf_terms())","value":[{"comment":"","label":"discount","propertyId":"northwind~discount","subjectId":"northwind~discount","rdf_property":{"comment":"","label":"discount","subjectId":"northwind~discount"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">"0.15","rdf_object":"0.15","resourceId":null,"subjectId":"northwind~discount-9ffc7a03c1959674fa8c0a7369460097"}]},{"comment":"","label":"is part of order","propertyId":"northwind~order","subjectId":"northwind~order","rdf_property":{"comment":"","label":"is part of order","subjectId":"northwind~order"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/Order-10250","resourceId":"NWD~Order-10250","subjectId":"northwind~order-b6b2d84f8259c3db3fb89c10ce920509"}]},{"comment":"","label":"unit price","propertyId":"northwind~orderDetailUnitPrice","subjectId":"northwind~orderDetailUnitPrice","rdf_property":{"comment":"","label":"unit price","subjectId":"northwind~orderDetailUnitPrice"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":"42.4","rdf_object":"42.4","resourceId":null,"subjectId":"northwind~orderDetailUnitPrice-8a622231ebe8e6ec3b0e654c589717d3"}]},{"comment":"","label":"includes product","propertyId":"northwind~product","subjectId":"northwind~product","rdf_property":{"comment":"","label":"includes product","subjectId":"northwind~product"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/Product-51","resourceId":"NWD~Product-51","subjectId":"northwind~product-46a5bfba2bbe33d1a6e41ac2f23216b1"}]},{"comment":"","label":"quantity","propertyId":"northwind~quantity","subjectId":"northwind~quantity","rdf_property":{"comment":"","label":"quantity","subjectId":"northwind~quantity"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":"35","rdf_object":"35","resourceId":null,"subjectId":"northwind~quantity-1c383cd30b7c298ab50293adfecb7b18"}]},{"comment":"","label":"label","propertyId":"rdfs~label","subjectId":"rdfs~label","rdf_property":{"comment":"","label":"label","subjectId":"rdfs~label"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":"OrderDetail-10250-51","rdf_object":"OrderDetail-10250-51","resourceId":null,"subjectId":"rdfs~label-311f0cc52cba0a21070961879f9173c8"}]},{"comment":"","label":"type","propertyId":"rdf~type","subjectId":"rdf~type","rdf_property":{"comment":"","label":"type","subjectId":"rdf~type"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/model/OrderDetail","resourceId":"northwind~OrderDetail"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">,"subjectId":"rdf~type-1c1c9eee9ed5045311df73136e39de22"}]}]}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource/fact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdfs_Resource('NWD~OrderDetail-10250-51')/rdf_facts('northwind~product')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource/$entity","comment":null,"label":"includes product","propertyId":null,"subjectId":"northwind~product"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource/fact,expandTermsProperty</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource(rdf_property(),rdf_terms())/$entity","comment":"","label":"includes product","propertyId":"northwind~product","subjectId":"northwind~product","rdf_property":{"comment":"","label":"includes product","subjectId":"northwind~product"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/Product-51","resourceId":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">"NWD~Product-51"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">,"subjectId":"northwind~product-46a5bfba2bbe33d1a6e41ac2f23216b1"}]}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource/fact/terms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdfs_Resource('NWD~OrderDetail-10250-51')/rdf_facts('northwind~product')/rdf_terms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource('NWD~OrderDetail-10250-51')/rdf_facts('northwind~product')/rdf_terms","value":[{"comment":null,"label":"Product-51","rdf_literal":"Product-51","rdf_object":"Product-51","resourceId":"","subjectId":"NWD~Product-51"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdfs_Resource('NWD~Employee-2')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource/$entity","comment":null,"label":"Employee-2","subjectId":"NWD~Employee-2"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource,expandIsObjectOf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$expand=rdf_isObjectOf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource(rdf_isObjectOf())/$entity","comment":null,"label":"Employee-2","subjectId":"NWD~Employee-2","rdf_isObjectOf":[{"comment":null,"isPropertyOfId":null,"label":null,"subjectId":"northwind~employee-183be8a27387eafb4f11fc9e9ea98950"},{"comment":null,"isPropertyOfId":null,"label":null,"subjectId":"northwind~reportsTo-183be8a27387eafb4f11fc9e9ea98950"},{"comment":null,"isPropertyOfId":null,"label":null,"subjectId":"rdf~subject-183be8a27387eafb4f11fc9e9ea98950"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource,expandIsObjectOfSubject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$expand=rdf_isObjectOf($expand=rdf_isPropertyOf,rdf_subjects)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Too large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource/isObjectofs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdfs_Resource('NWD~Employee-2')/rdf_isObjectOf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource('NWD~Employee-2')/rdf_isObjectOf","value":[{"comment":null,"isPropertyOfId":null,"label":"is managed by","subjectId":"northwind~employee"},{"comment":null,"isPropertyOfId":null,"label":"reports to employee","subjectId":"northwind~reportsTo"},{"comment":null,"isPropertyOfId":null,"label":null,"subjectId":"rdf~subject"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource/isObjectofs,expandSubjectsProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$expand=rdf_subjects,rdf_isPropertyOf&amp;$top=2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource('NWD~Employee-2')/rdf_isObjectOf(rdf_isPropertyOf(),rdf_subjects())","value":[{"comment":null,"isPropertyOfId":"northwind~reportsTo","label":"reports to employee","subjectId":"northwind~reportsTo","rdf_isPropertyOf":{"comment":null,"label":"reports to employee","subjectId":"northwind~reportsTo"},"rdf_subjects":[{"comment":null,"label":"Employee-1","subjectId":"NWD~Employee-1"},{"comment":null,"label":"Employee-8","subjectId":"NWD~Employee-8"}]}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource/isObjectof</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdfs_Resource('NWD~Employee-2')/rdf_isObjectOf('northwind~reportsTo')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource/$entity","comment":null,"isPropertyOfId":null,"label":"reports to employee","subjectId":"northwind~reportsTo"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource/isObjectof,expandSubjects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$expand=rdf_subjects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource(rdf_subjects())/$entity","comment":null,"isPropertyOfId":null,"label":"reports to employee","subjectId":"northwind~reportsTo","rdf_subjects":[{"comment":null,"label":"Employee-1","subjectId":"NWD~Employee-1"},{"comment":null,"label":"Employee-3","subjectId":"NWD~Employee-3"},{"comment":null,"label":"Employee-4","subjectId":"NWD~Employee-4"},{"comment":null,"label":"Employee-5","subjectId":"NWD~Employee-5"},{"comment":null,"label":"Employee-8","subjectId":"NWD~Employee-8"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource/isObjectof/subjects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdfs_Resource('NWD~Employee-2')/rdf_isObjectOf('northwind~reportsTo')/rdf_subjects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource('NWD~Employee-2')/rdf_isObjectOf('northwind~reportsTo')/rdf_subjects","value":[{"comment":null,"label":"Employee-1","subjectId":"NWD~Employee-1"},{"comment":null,"label":"Employee-3","subjectId":"NWD~Employee-3"},{"comment":null,"label":"Employee-4","subjectId":"NWD~Employee-4"},{"comment":null,"label":"Employee-5","subjectId":"NWD~Employee-5"},{"comment":null,"label":"Employee-8","subjectId":"NWD~Employee-8"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segmentpaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path1.EntitySet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$top=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee","value":[{"birthDate":"1968-12-08","comment":null,"employeeAddress":"507 - 20th Ave. E.\\nApt. 2A","employeeCity":"Seattle","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98122","employeeSalary":null,"employer":null,"extension":"5467","favorite":null,"firstName":"Nancy","hireDate":"2012-05-01","homePhone":"(206) 555-9857","label":"Employee-1","lastName":"Davolio","lat":47.6234778,"lat_long":"47.6234778,-122.3063220","long":-122.306322,"notes":"Education includes a BA in psychology from Colorado State University in 1970. She also completed The Art of the Cold Call. Nancy is a member of Toastmasters International.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-1","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Ms."},{"birthDate":"1972-02-19","comment":null,"employeeAddress":"908 W. Capital Way","employeeCity":"Tacoma","employeeCountry":"USA","employeeLinkedIn":"https://www.linkedin.com/in/peterjohnlawrence/","employeePostalCode":"98401","employeeSalary":null,"employer":null,"extension":"3457","favorite":null,"firstName":"Andrew","hireDate":"2012-08-14","homePhone":"(206) 555-9482","label":"Employee-2","lastName":"Fuller","lat":38.972057,"lat_long":"38.9720570,-77.0268860","long":-77.026886,"notes":"Andrew received his BTS commercial in 1974 and a Ph.D. in international marketing from the University of Dallas in 1981. He is fluent in French and Italian and reads German. He joined the company as a sales representative, was promoted to sales manager in January 1992 and to vice president of sales in March 1993. Andrew is a member of the Sales Management Roundtable, the Seattle Chamber of Commerce, and the Pacific Rim Importers Association.","photo":"http://accweb/emmployees/fuller.bmp","regionDescription":null,"reportsToId":null,"reportsToNotation":null,"subjectId":"NWD~Employee-2","territoryNotation":null,"title":"Vice President, Sales","titleOfCourtesy":"Dr."},{"birthDate":"1975-03-04","comment":null,"employeeAddress":"14 Garrett Hill","employeeCity":"London","employeeCountry":"UK","employeeLinkedIn":null,"employeePostalCode":"SW1 8JR","employeeSalary":null,"employer":null,"extension":"3453","favorite":null,"firstName":"Steven","hireDate":"2013-10-17","homePhone":"(71) 555-4848","label":"Employee-5","lastName":"Buchanan","lat":51.5239508,"lat_long":"51.5239508,-0.0944701","long":-0.0944701,"notes":"Steven Buchanan graduated from St. Andrews University, Scotland, with a BSC degree in 1976. Upon joining the company as a sales representative in 1992, he spent 6 months in an orientation program at the Seattle office and then returned to his permanent post in London. He was promoted to sales manager in March 1993. Mr. Buchanan has completed the courses Successful Telemarketing and International Sales Management. He is fluent in French.","photo":"http://accweb/emmployees/buchanan.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-5","territoryNotation":null,"title":"Sales Manager","titleOfCourtesy":"Mr."},{"birthDate":"1978-01-09","comment":null,"employeeAddress":"4726 - 11th Ave. N.E.","employeeCity":"Seattle","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98105","employeeSalary":null,"employer":null,"extension":"2344","favorite":null,"firstName":"Laura","hireDate":"2014-03-05","homePhone":"(206) 555-1189","label":"Employee-8","lastName":"Callahan","lat":47.6641642,"lat_long":"47.6641642,-122.3160149","long":-122.3160149,"notes":"Laura received a BA in psychology from the University of Washington. She has also completed a course in business French. She reads and writes French.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-8","territoryNotation":null,"title":"Inside Sales Coordinator","titleOfCourtesy":"Ms."},{"birthDate":"1986-01-27","comment":null,"employeeAddress":"7 Houndstooth Rd.","employeeCity":"London","employeeCountry":"UK","employeeLinkedIn":null,"employeePostalCode":"WG2 7LT","employeeSalary":null,"employer":null,"extension":"452","favorite":null,"firstName":"Anne","hireDate":"2014-11-15","homePhone":"(71) 555-4444","label":"Employee-9","lastName":"Dodsworth","lat":51.5073509,"lat_long":"51.5073509,-0.1277583","long":-0.1277583,"notes":"Anne has a BA degree in English from St. Lawrence College. She is fluent in French and German.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-5","reportsToNotation":null,"subjectId":"NWD~Employee-9","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Ms."}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path1.Entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee('NWD~Employee-2')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee/$entity","birthDate":"1972-02-19","comment":null,"employeeAddress":"908 W. Capital Way","employeeCity":"Tacoma","employeeCountry":"USA","employeeLinkedIn":"https://www.linkedin.com/in/peterjohnlawrence/","employeePostalCode":"98401","employeeSalary":null,"employer":null,"extension":"3457","favorite":null,"firstName":"Andrew","hireDate":"2012-08-14","homePhone":"(206) 555-9482","label":"Employee-2","lastName":"Fuller","lat":38.972057,"lat_long":"38.9720570,-77.0268860","long":-77.026886,"notes":"Andrew received his BTS commercial in 1974 and a Ph.D. in international marketing from the University of Dallas in 1981. He is fluent in French and Italian and reads German. He joined the company as a sales representative, was promoted to sales manager in January 1992 and to vice president of sales in March 1993. Andrew is a member of the Sales Management Roundtable, the Seattle Chamber of Commerce, and the Pacific Rim Importers Association.","photo":"http://accweb/emmployees/fuller.bmp","regionDescription":null,"reportsToId":null,"reportsToNotation":null,"subjectId":"NWD~Employee-2","territoryNotation":null,"title":"Vice President, Sales","titleOfCourtesy":"Dr."}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path2.EntitySet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$select=subjectId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~Employee-2')/managesOrder(subjectId)","value":[{"subjectId":"NWD~Order-10265"},{"subjectId":"NWD~Order-10277"},{"subjectId":"NWD~Order-10280"},{"subjectId":"NWD~Order-10295"},{"subjectId":"NWD~Order-10300"},{"subjectId":"NWD~Order-10307"},{"subjectId":"NWD~Order-10312"},{"subjectId":"NWD~Order-10313"},{"subjectId":"NWD~Order-10327"},{"subjectId":"NWD~Order-10339"},{"subjectId":"NWD~Order-10345"},{"subjectId":"NWD~Order-10368"},{"subjectId":"NWD~Order-10379"},{"subjectId":"NWD~Order-10388"},{"subjectId":"NWD~Order-10392"},{"subjectId":"NWD~Order-10398"},{"subjectId":"NWD~Order-10404"},{"subjectId":"NWD~Order-10407"},{"subjectId":"NWD~Order-10414"},{"subjectId":"NWD~Order-10422"},{"subjectId":"NWD~Order-10457"},{"subjectId":"NWD~Order-10462"},{"subjectId":"NWD~Order-10471"},{"subjectId":"NWD~Order-10478"},{"subjectId":"NWD~Order-10487"},{"subjectId":"NWD~Order-10502"},{"subjectId":"NWD~Order-10515"},{"subjectId":"NWD~Order-10516"},{"subjectId":"NWD~Order-10541"},{"subjectId":"NWD~Order-10552"},{"subjectId":"NWD~Order-10553"},{"subjectId":"NWD~Order-10556"},{"subjectId":"NWD~Order-10561"},{"subjectId":"NWD~Order-10563"},{"subjectId":"NWD~Order-10583"},{"subjectId":"NWD~Order-10588"},{"subjectId":"NWD~Order-10595"},{"subjectId":"NWD~Order-10615"},{"subjectId":"NWD~Order-10620"},{"subjectId":"NWD~Order-10657"},{"subjectId":"NWD~Order-10663"},{"subjectId":"NWD~Order-10669"},{"subjectId":"NWD~Order-10673"},{"subjectId":"NWD~Order-10676"},{"subjectId":"NWD~Order-10683"},{"subjectId":"NWD~Order-10686"},{"subjectId":"NWD~Order-10691"},{"subjectId":"NWD~Order-10727"},{"subjectId":"NWD~Order-10734"},{"subjectId":"NWD~Order-10737"},{"subjectId":"NWD~Order-10738"},{"subjectId":"NWD~Order-10752"},{"subjectId":"NWD~Order-10780"},{"subjectId":"NWD~Order-10781"},{"subjectId":"NWD~Order-10787"},{"subjectId":"NWD~Order-10798"},{"subjectId":"NWD~Order-10805"},{"subjectId":"NWD~Order-10808"},{"subjectId":"NWD~Order-10810"},{"subjectId":"NWD~Order-10815"},{"subjectId":"NWD~Order-10819"},{"subjectId":"NWD~Order-10832"},{"subjectId":"NWD~Order-10846"},{"subjectId":"NWD~Order-10858"},{"subjectId":"NWD~Order-10865"},{"subjectId":"NWD~Order-10912"},{"subjectId":"NWD~Order-10915"},{"subjectId":"NWD~Order-10919"},{"subjectId":"NWD~Order-10939"},{"subjectId":"NWD~Order-10949"},{"subjectId":"NWD~Order-10967"},{"subjectId":"NWD~Order-10971"},{"subjectId":"NWD~Order-10982"},{"subjectId":"NWD~Order-10983"},{"subjectId":"NWD~Order-10985"},{"subjectId":"NWD~Order-10989"},{"subjectId":"NWD~Order-10990"},{"subjectId":"NWD~Order-10994"},{"subjectId":"NWD~Order-11000"},{"subjectId":"NWD~Order-11001"},{"subjectId":"NWD~Order-11005"},{"subjectId":"NWD~Order-11009"},{"subjectId":"NWD~Order-11010"},{"subjectId":"NWD~Order-11013"},{"subjectId":"NWD~Order-11014"},{"subjectId":"NWD~Order-11015"},{"subjectId":"NWD~Order-11020"},{"subjectId":"NWD~Order-11028"},{"subjectId":"NWD~Order-11032"},{"subjectId":"NWD~Order-11035"},{"subjectId":"NWD~Order-11042"},{"subjectId":"NWD~Order-11053"},{"subjectId":"NWD~Order-11059"},{"subjectId":"NWD~Order-11060"},{"subjectId":"NWD~Order-11070"},{"subjectId":"NWD~Order-11073"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path2.Entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee('NWD~Employee-5')/reportsTo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~Employee-5')/reportsTo/$entity","birthDate":"1972-02-19","comment":null,"employeeAddress":"908 W. Capital Way","employeeCity":"Tacoma","employeeCountry":"USA","employeeLinkedIn":"https://www.linkedin.com/in/peterjohnlawrence/","employeePostalCode":"98401","employeeSalary":null,"employer":null,"extension":"3457","favorite":null,"firstName":"Andrew","hireDate":"2012-08-14","homePhone":"(206) 555-9482","label":"Employee-2","lastName":"Fuller","lat":38.972057,"lat_long":"38.9720570,-77.0268860","long":-77.026886,"notes":"Andrew received his BTS commercial in 1974 and a Ph.D. in international marketing from the University of Dallas in 1981. He is fluent in French and Italian and reads German. He joined the company as a sales representative, was promoted to sales manager in January 1992 and to vice president of sales in March 1993. Andrew is a member of the Sales Management Roundtable, the Seattle Chamber of Commerce, and the Pacific Rim Importers Association.","photo":"http://accweb/emmployees/fuller.bmp","regionDescription":null,"reportsToId":null,"reportsToNotation":null,"subjectId":"NWD~Employee-2","territoryNotation":null,"title":"Vice President, Sales","titleOfCourtesy":"Dr."}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee/$entity","comment":null,"customerId":"NWD~Customer-BLONP","customerNotation":null,"employeeId":"NWD~Employee-2","employeeNotation":null,"freight":55.279999,"label":"Order-10265","lat":48.5835085,"lat_long":"48.5835085,7.7446960","long":7.744696,"orderDate":"2016-07-25T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-08-22T00:00:00Z","shipAddress":"24, place Kléber","shipCity":"Strasbourg","shipCountry":"France","shipName":"Blondel père et fils","shipPostalCode":"67000","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2016-08-12T00:00:00Z","subjectId":"NWD~Order-10265"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path3.EntitySet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail","value":[{"comment":null,"discount":0.0,"label":"OrderDetail-10265-17","orderDetailUnitPrice":31.2,"orderId":"NWD~Order-10265","orderNotation":null,"productId":"NWD~Product-17","productNotation":null,"quantity":30,"subjectId":"NWD~OrderDetail-10265-17"},{"comment":null,"discount":0.0,"label":"OrderDetail-10265-70","orderDetailUnitPrice":12.0,"orderId":"NWD~Order-10265","orderNotation":null,"productId":"NWD~Product-70","productNotation":null,"quantity":20,"subjectId":"NWD~OrderDetail-10265-70"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path3.Entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/customer/$entity","comment":null,"customerAddress":"24, place Kléber","customerCity":"Strasbourg","customerCompanyName":"Blondesddsl père et fils","customerContactName":"Frédérique Citeaux","customerContactTitle":"Marketing Manager","customerCountry":"France","customerFax":"88.60.15.32","customerPhone":"88.60.15.31","customerPostalCode":"67000","customerWebsite":null,"label":"Blondesddsl père et fils","lat":48.5835085,"lat_long":"48.5835085,7.7446960","long":7.744696,"regionDescription":null,"subjectId":"NWD~Customer-BLONP"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail('NWD~OrderDetail-10265-17')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee/$entity","comment":null,"discount":0.0,"label":"OrderDetail-10265-17","orderDetailUnitPrice":31.2,"orderId":"NWD~Order-10265","orderNotation":null,"productId":"NWD~Product-17","productNotation":null,"quantity":30,"subjectId":"NWD~OrderDetail-10265-17"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path4.Entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail('NWD~OrderDetail-10265-17')/product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail('NWD~OrderDetail-10265-17')/product/$entity","categoryId":"NWD~Category-6","categoryNotation":null,"comment":null,"discontinued":true,"label":"Product-17","productName":"Alice Mutton","productUnitPrice":39.0,"quantityPerUnit":"20 - 1 kg tins","reorderLevel":0,"subjectId":"NWD~Product-17","supplierId":"NWD~Supplier-7","supplierNotation":null,"unitCommission":null,"unitsInStock":0,"unitsOnOrder":0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path5.Entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail('NWD~OrderDetail-10265-17')/product/supplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail('NWD~OrderDetail-10265-17')/product/supplier/$entity","comment":null,"homePage":null,"label":"Supplier-7","lat":-37.741888,"lat_long":"-37.7418880,144.9475730","long":144.947573,"regionDescription":null,"subjectId":"NWD~Supplier-7","supplierAddress":"74 Rose St. Moonie Ponds","supplierCity":"Melbourne","supplierCompanyName":"Pavlova, Ltd.","supplierContactName":"Ian Devling","supplierContactTitle":"Marketing Manager","supplierCountry":"Australia","supplierFax":null,"supplierHomePage":null,"supplierPhone":"(03) 444-2343","supplierPostalCode":"3058"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path6.Entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail('NWD~OrderDetail-10265-17')/product/supplier/suppliesProduct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~Employee-2')/managesOrder('NWD~Order-10265')/hasOrderDetail('NWD~OrderDetail-10265-17')/product/supplier/suppliesProduct","value":[{"categoryId":"NWD~Category-3","categoryNotation":null,"comment":null,"discontinued":false,"label":"Product-16","productName":"Pavlova","productUnitPrice":17.45,"quantityPerUnit":"32 - 500 g boxes","reorderLevel":10,"subjectId":"NWD~Product-16","supplierId":"NWD~Supplier-7","supplierNotation":null,"unitCommission":null,"unitsInStock":29,"unitsOnOrder":0},{"categoryId":"NWD~Category-6","categoryNotation":null,"comment":null,"discontinued":true,"label":"Product-17","productName":"Alice Mutton","productUnitPrice":39.0,"quantityPerUnit":"20 - 1 kg tins","reorderLevel":0,"subjectId":"NWD~Product-17","supplierId":"NWD~Supplier-7","supplierNotation":null,"unitCommission":null,"unitsInStock":0,"unitsOnOrder":0},{"categoryId":"NWD~Category-8","categoryNotation":null,"comment":null,"discontinued":false,"label":"Product-18","productName":"Carnarvon Tigers","productUnitPrice":62.5,"quantityPerUnit":"16 kg pkg.","reorderLevel":0,"subjectId":"NWD~Product-18","supplierId":"NWD~Supplier-7","supplierNotation":null,"unitCommission":null,"unitsInStock":42,"unitsOnOrder":0},{"categoryId":"NWD~Category-2","categoryNotation":null,"comment":null,"discontinued":false,"label":"Product-63","productName":"Vegie-spread","productUnitPrice":43.9,"quantityPerUnit":"15 - 625 g jars","reorderLevel":5,"subjectId":"NWD~Product-63","supplierId":"NWD~Supplier-7","supplierNotation":null,"unitCommission":null,"unitsInStock":24,"unitsOnOrder":0},{"categoryId":"NWD~Category-1","categoryNotation":null,"comment":null,"discontinued":false,"label":"Product-70","productName":"Outback Lager","productUnitPrice":15.0,"quantityPerUnit":"24 - 355 ml bottles","reorderLevel":30,"subjectId":"NWD~Product-70","supplierId":"NWD~Supplier-7","supplierNotation":null,"unitCommission":null,"unitsInStock":15,"unitsOnOrder":10}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProxyOLGAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">olgap_ShortestPath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODATA2SPARQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service=%27tfl%27&amp;start=londontube~Euston&amp;end=londontube~Baker_Street&amp;propertyPath=%27(tfl~connectsFrom)!(rdf~type%7Ctfl~connectsTo)%5E!(rdf~type%7Ctfl~hasStationInZone%7Ctfl~hasStationOnLine%7Ctfl~connectsFrom)%5E(rdf~type)%27&amp;maxPath=8&amp;$orderby=edge</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{"@odata.context":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_ShortestPath</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">","value":[{"direct":true,"edge":1,"maxPath":null,"object":"londontube~Kings_Cross_St._Pancras","property":"tfl~connectsFrom","propertyPath":null,"subject":"londontube~Euston"},{"direct":true,"edge":2,"maxPath":null,"object":"londontube~Euston_Square","property":"tfl~connectsFrom","propertyPath":null,"subject":"londontube~Kings_Cross_St._Pancras"},{"direct":true,"edge":3,"maxPath":null,"object":"londontube~Great_Portland_Street","property":"tfl~connectsFrom","propertyPath":null,"subject":"londontube~Euston_Square"},{"direct":true,"edge":4,"maxPath":null,"object":"londontube~Baker_Street","property":"tfl~connectsFrom","propertyPath":null,"subject":"londontube~Great_Portland_Street"}]}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">service=%22tfl%22&amp;start=londontube~Goldhawk_Road&amp;end=londontube~Tower_Hill&amp;propertyPath=%22!(rdf~type%7Ctfl~connectsFrom%7Ctfl~onLine%7Ctfl~inZone)%5E!(rdf~type%7Ctfl~hasStationInZone%7Ctfl~hasStationOnLine)%22&amp;maxPath=20&amp;$select=direct,object,property,subject&amp;$expand=olgap_object($select=label),olgap_subject($select=label),olgap_property($select=label,subjectId)&amp;$orderby=edge&amp;bidirectional=true&amp;$skip=0&amp;$top=20</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_ShortestPath(direct,object,property,subject,olgap_object(label,subjectId),olgap_property(label,subjectId),olgap_subject(label,subjectId))","value":[{"direct":true,"object":"londontube~Shepherds_Bush_Market","property":"tfl~connectsTo","subject":"londontube~Goldhawk_Road","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Shepherds_Bush_Market')","label":"Shepherds Bush Market","subjectId":"londontube~Shepherds_Bush_Market"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Goldhawk_Road')","label":"Goldhawk Road","subjectId":"londontube~Goldhawk_Road"}},{"direct":true,"object":"londontube~Wood_Lane","property":"tfl~connectsTo","subject":"londontube~Shepherds_Bush_Market","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Wood_Lane')","label":"Wood Lane","subjectId":"londontube~Wood_Lane"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Shepherds_Bush_Market')","label":"Shepherds Bush Market","subjectId":"londontube~Shepherds_Bush_Market"}},{"direct":true,"object":"londontube~Latimer_Road","property":"tfl~connectsTo","subject":"londontube~Wood_Lane","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Latimer_Road')","label":"Latimer Road","subjectId":"londontube~Latimer_Road"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Wood_Lane')","label":"Wood Lane","subjectId":"londontube~Wood_Lane"}},{"direct":true,"object":"londontube~Ladbroke_Grove","property":"tfl~connectsTo","subject":"londontube~Latimer_Road","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Ladbroke_Grove')","label":"Ladbroke Grove","subjectId":"londontube~Ladbroke_Grove"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Latimer_Road')","label":"Latimer Road","subjectId":"londontube~Latimer_Road"}},{"direct":true,"object":"londontube~Westbourne_Park","property":"tfl~connectsTo","subject":"londontube~Ladbroke_Grove","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Westbourne_Park')","label":"Westbourne Park","subjectId":"londontube~Westbourne_Park"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Ladbroke_Grove')","label":"Ladbroke Grove","subjectId":"londontube~Ladbroke_Grove"}},{"direct":true,"object":"londontube~Royal_Oak","property":"tfl~connectsTo","subject":"londontube~Westbourne_Park","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Royal_Oak')","label":"Royal Oak","subjectId":"londontube~Royal_Oak"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Westbourne_Park')","label":"Westbourne Park","subjectId":"londontube~Westbourne_Park"}},{"direct":true,"object":"londontube~Paddington","property":"tfl~connectsTo","subject":"londontube~Royal_Oak","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Paddington')","label":"Paddington","subjectId":"londontube~Paddington"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Royal_Oak')","label":"Royal Oak","subjectId":"londontube~Royal_Oak"}},{"direct":true,"object":"londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29","property":"tfl~connectsTo","subject":"londontube~Paddington","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29')","label":"Edgware Road (Circle/District/Hammersmith and City)","subjectId":"londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Paddington')","label":"Paddington","subjectId":"londontube~Paddington"}},{"direct":true,"object":"londontube~Baker_Street","property":"tfl~connectsTo","subject":"londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Baker_Street')","label":"Baker Street","subjectId":"londontube~Baker_Street"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29')","label":"Edgware Road (Circle/District/Hammersmith and City)","subjectId":"londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29"}},{"direct":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">false,"object":"londontube~Bond_Street","property":"tfl~connectsFrom","subject":"londontube~Baker_Street","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Bond_Street')","label":"Bond Street","subjectId":"londontube~Bond_Street"},"olgap_property":{"label":"Connects From","subjectId":"tfl~connectsFrom"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Baker_Street')","label":"Baker Street","subjectId":"londontube~Baker_Street"}},{"direct":false,"object":"londontube~Green_Park","property":"tfl~connectsFrom","subject":"londontube~Bond_Street","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Green_Park')","label":"Green Park","subjectId":"londontube~Green_Park"},"olgap_property":{"label":"Connects From","subjectId":"tfl~connectsFrom"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Bond_Street')","label":"Bond Street","subjectId":"londontube~Bond_Street"}},{"direct":false,"object":"londontube~Westminster","property":"tfl~connectsFrom","subject":"londontube~Green_Park","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Westminster')","label":"Westminster","subjectId":"londontube~Westminster"},"olgap_property":{"label":"Connects From","subjectId":"tfl~connectsFrom"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Green_Park')","label":"Green Park","subjectId":"londontube~Green_Park"}},{"direct":false,"object":"londontube~Waterloo","property":"tfl~connectsFrom","subject":"londontube~Westminster","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Waterloo')","label":"Waterloo","subjectId":"londontube~Waterloo"},"olgap_property":{"label":"Connects From","subjectId":"tfl~connectsFrom"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Westminster')","label":"Westminster","subjectId":"londontube~Westminster"}},{"direct":false,"object":"londontube~Bank","property":"tfl~connectsFrom","subject":"londontube~Waterloo","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Bank')","label":"Bank","subjectId":"londontube~Bank"},"olgap_property":{"label":"Connects From","subjectId":"tfl~connectsFrom"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Waterloo')","label":"Waterloo","subjectId":"londontube~Waterloo"}},{"direct":false,"object":"londontube~Liverpool_Street","property":"tfl~connectsTo","subject":"londontube~Bank","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Liverpool_Street')","label":"Liverpool Street","subjectId":"londontube~Liverpool_Street"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Bank')","label":"Bank","subjectId":"londontube~Bank"}},{"direct":false,"object":"londontube~Aldgate","property":"tfl~connectsFrom","subject":"londontube~Liverpool_Street","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Aldgate')","label":"Aldgate","subjectId":"londontube~Aldgate"},"olgap_property":{"label":"Connects From","subjectId":"tfl~connectsFrom"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Liverpool_Street')","label":"Liverpool Street","subjectId":"londontube~Liverpool_Street"}},{"direct":false,"object":"londontube~Tower_Hill","property":"tfl~connectsFrom","subject":"londontube~Aldgate","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Tower_Hill')","label":"Tower Hill","subjectId":"londontube~Tower_Hill"},"olgap_property":{"label":"Connects From","subjectId":"tfl~connectsFrom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Aldgate')","label":"Aldgate","subjectId":"londontube~Aldgate"}}]}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">service=%27northwind%27&amp;start=NWD~Customer-PRINI&amp;end=NWD~Product-29&amp;propertyPath=%27!(rdf~type)%5E!(rdf~type)%27&amp;maxPath=15&amp;$orderby=edge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_ShortestPath","value":[{"direct":false,"edge":1,"maxPath":null,"object":"NWD~Order-11007","property":"northwind~customer","propertyPath":null,"subject":"NWD~Customer-PRINI"},{"direct":false,"edge":2,"maxPath":null,"object":"NWD~OrderDetail-11007-29","property":"northwind~order","propertyPath":null,"subject":"NWD~Order-11007"},{"direct":true,"edge":3,"maxPath":null,"object":"NWD~Product-29","property":"northwind~product","propertyPath":null,"subject":"NWD~OrderDetail-11007-29"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service=%27northwind%27&amp;start=NWD~Order-10477&amp;end=NWD~Order-10491&amp;propertyPath=%27!(rdf~type)%5E!(rdf~type)%27&amp;maxPath=15&amp;$orderby=edge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_ShortestPath","value":[{"direct":true,"edge":1,"maxPath":null,"object":"NWD~Employee-5","property":"northwind~employee","propertyPath":null,"subject":"NWD~Order-10477"},{"direct":true,"edge":2,"maxPath":null,"object":"NWD~Employee-2","property":"northwind~reportsTo","propertyPath":null,"subject":"NWD~Employee-5"},{"direct":false,"edge":3,"maxPath":null,"object":"NWD~Employee-8","property":"northwind~reportsTo","propertyPath":null,"subject":"NWD~Employee-2"},{"direct":false,"edge":4,"maxPath":null,"object":"NWD~Order-10491","property":"northwind~employee","propertyPath":null,"subject":"NWD~Employee-8"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">olgap_Triangles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service=%27tfl%27</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_Triangles","value":[{"triangles":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">555</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">,"trianglesService":"j0~tfl"}]}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">olgap_DegreeDistribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service=%27tfl%27&amp;$orderby=degree</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_DegreeDistribution","value":[{"count":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">901,"degree":1,"degreeDistributionService":"UNDEF"},{"count":701,"degree":2,"degreeDistributionService":"UNDEF"},{"count":4,"degree":3,"degreeDistributionService":"UNDEF"},{"count":17,"degree":4,"degreeDistributionService":"UNDEF"},{"count":11,"degree":5,"degreeDistributionService":"UNDEF"},{"count":17,"degree":6,"degreeDistributionService":"UNDEF"},{"count":5,"degree":7,"degreeDistributionService":"UNDEF"},{"count":2,"degree":8,"degreeDistributionService":"UNDEF"},{"count":5,"degree":9,"degreeDistributionService":"UNDEF"},{"count":4,"degree":11,"degreeDistributionService":"UNDEF"},{"count":1,"degree":13,"degreeDistributionService":"UNDEF"},{"count":1,"degree":14,"degreeDistributionService":"UNDEF"},{"count":37,"degree":16,"degreeDistributionService":"UNDEF"},{"count":335,"degree":18,"degreeDistributionService":"UNDEF"},{"count":76,"degree":20,"degreeDistributionService":"UNDEF"},{"count":2,"degree":21,"degreeDistributionService":"UNDEF"},{"count":34,"degree":22,"degreeDistributionService":"UNDEF"},{"count":1,"degree":23,"degreeDistributionService":"UNDEF"},{"count":80,"degree":24,"degreeDistributionService":"UNDEF"},{"count":1,"degree":25,"degreeDistributionService":"UNDEF"},{"count":31</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">,"degree":26,"degreeDistributionService":"UNDEF"},{"count":2,"degree":27,"degreeDistributionService":"UNDEF"},{"count":13,"degree":28,"degreeDistributionService":"UNDEF"},{"count":2,"degree":29,"degreeDistributionService":"UNDEF"},{"count":12,"degree":30,"degreeDistributionService":"UNDEF"},{"count":7,"degree":32,"degreeDistributionService":"UNDEF"},{"count":5,"degree":34,"degreeDistributionService":"UNDEF"},{"count":3,"degree":36,"degreeDistributionService":"UNDEF"},{"count":3,"degree":38,"degreeDistributionService":"UNDEF"},{"count":2,"degree":42,"degreeDistributionService":"UNDEF"},{"count":1,"degree":44,"degreeDistributionService":"UNDEF"},{"count":2,"degree":45,"degreeDistributionService":"UNDEF"},{"count":1,"degree":48,"degreeDistributionService":"UNDEF"},{"count":1,"degree":49,"degreeDistributionService":"UNDEF"},{"count":1,"degree":50,"degreeDistributionService":"UNDEF"},{"count":1,"degree":52,"degreeDistributionService":"UNDEF"},{"count":1,"degree":53,"degreeDistributionService":"UNDEF"},{"count":1,"degree":57,"degreeDistributionService":"UNDEF"},{"count":1,"degree":61,"degreeDistributionService":"UNDEF"},{"count":1,"degree":67,"degreeDistributionService":"UNDEF"},{"count":1,"degree":69,"degreeDistributionService":"UNDEF"},{"count":1,"degree":73,"degreeDistributionService":"UNDEF"},{"count":1,"degree":81,"degreeDistributionService":"UNDEF"},{"count":1,"degree":91,"degreeDistributionService":"UNDEF"},{"count":1,"degree":93,"degreeDistributionService":"UNDEF"},{"count":1,"degree":101,"degreeDistributionService":"UNDEF"},{"count":1,"degree":103,"degreeDistributionService":"UNDEF"},{"count":1,"degree":107,"degreeDistributionService":"UNDEF"},{"count":1,"degree":109,"degreeDistributionService":"UNDEF"},{"count":1,"degree":123,"degreeDistributionService":"UNDEF"},{"count":1,"degree":137,"degreeDistributionService":"UNDEF"},{"count":1,"degree":145,"degreeDistributionService":"UNDEF"},{"count":1,"degree":163,"degreeDistributionService":"UNDEF"},{"count":1,"degree":203,"degreeDistributionService":"UNDEF"},{"count":1,"degree":215,"degreeDistributionService":"UNDEF"},{"count":1,"degree":225,"degreeDistributionService":"UNDEF"},{"count":1,"degree":299,"degreeDistributionService":"UNDEF"},{"count":1,"degree":305,"degreeDistributionService":"UNDEF"},{"count":1,"degree":353,"degreeDistributionService":"UNDEF"},{"count":1,"degree":1295,"degreeDistributionService":"UNDEF"}]}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">olgap_Eccentricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service=%27tfl%27&amp;subject=londontube~Baker_Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_Eccentricity","value":[{"eccentricity":2,"eccentricitySubject":"londontube~Baker_Street"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">olgap_ConnectedComponents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">olgap_PageRank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProxySearch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search_EntitySearch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service=%22northwind%22&amp;string=%22isabel%20AND%20portugal%22&amp;$orderby=entity&amp;$select=entity,formattedValue,type&amp;$expand=search_entity($select=label,subjectId)&amp;$skip=0&amp;$top=20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#search_EntitySearch(entity,formattedValue,type,search_entity(label,subjectId))","value":[{"entity":"NWD~Customer-PRINI","formattedValue":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;company name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;label:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;contact name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Isabel&lt;/B&gt; de Castro&lt;/td&gt;&lt;/tr&gt;","type":"northwind~Customer","search_entity":{"label":"Princesa Isabel Vinhos","subjectId":"NWD~Customer-PRINI"}},{"entity":"NWD~Order-10336","formattedValue":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;ship name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","type":"northwind~Order","search_entity":{"label":"Order-10336","subjectId":"NWD~Order-10336"}},{"entity":"NWD~Order-10397","formattedValue":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;ship name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","type":"northwind~Order","search_entity":{"label":"Order-10397","subjectId":"NWD~Order-10397"}},{"entity":"NWD~Order-10433","formattedValue":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;ship name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","type":"northwind~Order","search_entity":{"label":"Order-10433","subjectId":"NWD~Order-10433"}},{"entity":"NWD~Order-10477","formattedValue":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;ship name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","type":"northwind~Order","search_entity":{"label":"Order-10477","subjectId":"NWD~Order-10477"}},{"entity":"NWD~Order-11007","formattedValue":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt; &lt;tr&gt;&lt;td&gt;&lt;i&gt;ship name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","type":"northwind~Order","search_entity":{"label":"Order-11007","subjectId":"NWD~Order-11007"}}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search_LinkedSearch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service=%22northwind%22&amp;subjectA=NWD~Customer-ANTON&amp;stringB=%22Geitost%22&amp;$select=entityA,entityB,formattedValueB,i10,i21,i32,i43,i54,i65,node1,node2,node3,node4,node5,p01,p12,p23,p34,p45,p56,type1,type2,type3,type4,type5,typeA,typeB&amp;$skip=0&amp;$top=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#search_LinkedSearch(entityA,entityB,formattedValueB,i10,i21,i32,i43,i54,i65,node1,node2,node3,node4,node5,p01,p12,p23,p34,p45,p56,type1,type2,type3,type4,type5,typeA,typeB)","value":[{"entityA":"NWD~Customer-ANTON","entityB":"NWD~Product-33","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;product name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Geitost&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","i10":"northwind~customer","i21":"UNDEF","i32":"northwind~customer","i43":"northwind~order","i54":"UNDEF","i65":"UNDEF","node1":"NWD~Order-10365","node2":"NWD~Customer-ANTON","node3":"NWD~Order-10677","node4":"NWD~OrderDetail-10677-33","node5":"UNDEF","p01":"UNDEF","p12":"northwind~customer","p23":"UNDEF","p34":"UNDEF","p45":"northwind~product","p56":"UNDEF","type1":"northwind~Order","type2":"northwind~Customer","type3":"northwind~Order","type4":"northwind~OrderDetail","type5":"UNDEF","typeA":"UNDEF","typeB":"northwind~Product"},{"entityA":"NWD~Customer-ANTON","entityB":"NWD~Product-33","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;product name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Geitost&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","i10":"northwind~customer","i21":"UNDEF","i32":"northwind~customer","i43":"northwind~order","i54":"UNDEF","i65":"UNDEF","node1":"NWD~Order-10365","node2":"NWD~Customer-ANTON","node3":"NWD~Order-10682","node4":"NWD~OrderDetail-10682-33","node5":"UNDEF","p01":"UNDEF","p12":"northwind~customer","p23":"UNDEF","p34":"UNDEF","p45":"northwind~product","p56":"UNDEF","type1":"northwind~Order","type2":"northwind~Customer","type3":"northwind~Order","type4":"northwind~OrderDetail","type5":"UNDEF","typeA":"UNDEF","typeB":"northwind~Product"},{"entityA":"NWD~Customer-ANTON","entityB":"NWD~Product-33","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;product name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Geitost&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","i10":"northwind~customer","i21":"UNDEF","i32":"UNDEF","i43":"northwind~orderRegion","i54":"northwind~order","i65":"UNDEF","node1":"NWD~Order-10365","node2":"NWD~Employee-3","node3":"NWD~Region-4306a04670067b5b27e766335d3d40fa","node4":"NWD~Order-10269","node5":"NWD~OrderDetail-10269-33","p01":"UNDEF","p12":"northwind~employee","p23":"northwind~employeeRegion","p34":"UNDEF","p45":"UNDEF","p56":"northwind~product","type1":"northwind~Order","type2":"northwind~Employee","type3":"northwind~Region","type4":"northwind~Order","type5":"northwind~OrderDetail","typeA":"UNDEF","typeB":"northwind~Product"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search_PathSearch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service=%22northwind%22&amp;subjectA=NWD~Customer-ANTON&amp;stringB=%22Geitost%22&amp;propertyPath=%27!(rdf~type)%5E!(rdf~type)%27&amp;maxPath=20&amp;$select=entityA,entityB,formattedValueB,edge,subject,property,direct,object&amp;$top=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search_LinkedEntitySearch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service=%22northwind%22&amp;stringA=%22isabel%22&amp;stringB=%22portugal%22&amp;$select=entityA,entityB,formattedValueA,formattedValueB,i10,i21,i32,i43,i54,i65,node1,node2,node3,node4,node5,p01,p12,p23,p34,p45,p56,type1,type2,type3,type4,type5,typeA,typeB&amp;$skip=0&amp;$top=3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#search_LinkedEntitySearch(entityA,entityB,formattedValueA,formattedValueB,i10,i21,i32,i43,i54,i65,node1,node2,node3,node4,node5,p01,p12,p23,p34,p45,p56,type1,type2,type3,type4,type5,typeA,typeB)","value":[{"entityA":"NWD~Customer-PRINI","entityB":"NWD~Order-11007","formattedValueA":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;company name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","i10":"northwind~customer","i21":"UNDEF","i32":"northwind~customer","i43":"UNDEF","i54":"northwind~customer","i65":"UNDEF","node1":"NWD~Order-10336","node2":"NWD~Customer-PRINI","node3":"NWD~Order-10336","node4":"NWD~Customer-PRINI","node5":"UNDEF","p01":"UNDEF","p12":"northwind~customer","p23":"UNDEF","p34":"northwind~customer","p45":"UNDEF","p56":"UNDEF","type1":"northwind~Order","type2":"northwind~Customer","type3":"northwind~Order","type4":"northwind~Customer","type5":"UNDEF","typeA":"northwind~Customer","typeB":"northwind~Order"},{"entityA":"NWD~Customer-PRINI","entityB":"NWD~Order-11007","formattedValueA":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;company name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","i10":"northwind~customer","i21":"UNDEF","i32":"northwind~customer","i43":"UNDEF","i54":"UNDEF","i65":"UNDEF","node1":"NWD~Order-10336","node2":"NWD~Customer-PRINI","node3":"UNDEF","node4":"UNDEF","node5":"UNDEF","p01":"UNDEF","p12":"northwind~customer","p23":"UNDEF","p34":"UNDEF","p45":"UNDEF","p56":"UNDEF","type1":"northwind~Order","type2":"northwind~Customer","type3":"UNDEF","type4":"UNDEF","type5":"UNDEF","typeA":"northwind~Customer","typeB":"northwind~Order"},{"entityA":"NWD~Customer-PRINI","entityB":"NWD~Order-11007","formattedValueA":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;company name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","i10":"northwind~customer","i21":"UNDEF","i32":"UNDEF","i43":"UNDEF","i54":"UNDEF","i65":"UNDEF","node1":"UNDEF","node2":"UNDEF","node3":"UNDEF","node4":"UNDEF","node5":"UNDEF","p01":"UNDEF","p12":"UNDEF","p23":"UNDEF","p34":"UNDEF","p45":"UNDEF","p56":"UNDEF","type1":"UNDEF","type2":"UNDEF","type3":"UNDEF","type4":"UNDEF","type5":"UNDEF","typeA":"northwind~Customer","typeB":"northwind~Order"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search_PathEntitySearch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service=%22northwind%22&amp;stringA=%22isabel%22&amp;stringB=%22portugal%22&amp;propertyPath=%27!(rdf~type)%5E!(rdf~type)%27&amp;maxPath=20&amp;$select=entityA,formattedValueA,entityB,formattedValueB,edge,subject,property,direct,object&amp;$top=1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#search_PathEntitySearch(direct,edge,entityA,entityB,formattedValueA,formattedValueB,object,property,subject,typeA,typeB)","value":[{"@odata.id":"search_PathEntitySearch(entityA='NWD~Order-10477',entityB='NWD~Order-10491',object='NWD~</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Order-10366',property='northwind~shipVia',subject='NWD~Shipper-2',typeA='northwind~Order',typeB='northwind~Order')","direct":false,"edge":2,"entityA":"NWD~Order-10477","entityB":"NWD~Order-10491","formattedValueA":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","object":"NWD~Order-10366","property":"northwind~shipVia","subject":"NWD~Shipper-2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">","typeA":"northwind~Order","typeB":"northwind~Order"}]}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ProxyContextmenu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contextmenu_Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service=%22northwind%22&amp;subject=NWD~OrderDetail-10255-16&amp;$select=count,property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#contextmenu_Count(count,entity,property)","value":[{"@odata.id":"contextmenu_Count(entity='NWD~OrderDetail-10255-16',property='northwind~product')","count":1,"entity":"NWD~OrderDetail-10255-16","property":"northwind~product"},{"@odata.id":"contextmenu_Count(entity='NWD~OrderDetail-10255-16',property='northwind~order')","count":1,"entity":"NWD~OrderDetail-10255-16","property":"northwind~order"},{"@odata.id":"contextmenu_Count(entity='NWD~OrderDetail-10255-16',property='rdf~type')","count":1,"entity":"NWD~OrderDetail-10255-16","property":"rdf~type"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contextmenu_Types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service=%22northwind%22&amp;subject=NWD~OrderDetail-10255-16</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#contextmenu_Types","value":[{"entity":"NWD~OrderDetail-10255-16","type":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">northwind~OrderDetail"},{"entity":"UNDEF","type":"rdfs~Resource</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
       </rPr>
       <t xml:space="preserve">"}]}</t>
     </r>
@@ -793,7 +1011,32 @@
     <t xml:space="preserve">Employee('NWD~SystemAEmployee-1')/reportsTo/employeeSalary</t>
   </si>
   <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~SystemAEmployee-1')/reportsTo/employeeSalary","systemAEmployeeSalary":42.0,"systemBEmployeeAnnualSalary":null,"systemBEmployeeMonthlySalary":null}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~SystemAEmployee-1')/reportsTo/employeeSalary","systemAEmployeeSalary":</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">null,"systemBEmployeeAnnualSalary":48.0,"systemBEmployeeMonthlySalary":4.199999809265137</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">URI4</t>
@@ -1255,7 +1498,32 @@
     <t xml:space="preserve">$expand=employee($expand=reportsTo)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order(employee(reportsTo()))/$entity","comment":null,"customerId":"NWD~Customer-TOMSP","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":11.61,"label":"Order-10249","lat":51.6566,"lat_long":"51.6566000,7.0904400","long":7.09044,"orderDate":"2016-07-05T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-08-16T00:00:00Z","shipAddress":"Luisenstr. 48","shipCity":"Münster","shipCountry":"Germany","shipName":"Toms Spezialitäten","shipPostalCode":"44087","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2016-07-10T00:00:00Z","subjectId":"NWD~Order-10249","employee":{"birthDate":null,"comment":null,"employeeAddress":null,"employeeCity":null,"employeeCountry":null,"employeeLinkedIn":null,"employeePostalCode":null,"employeeSalary":null,"employer":null,"extension":null,"favorite":null,"firstName":null,"hireDate":null,"homePhone":null,"label":null,"lastName":null,"lat":null,"lat_long":null,"long":null,"notes":null,"photo":null,"regionDescription":null,"reportsToId":"NWD~SystemBEmployee-2","reportsToNotation":null,"subjectId":"NWD~SystemAEmployee-1","territoryNotation":null,"title":null,"titleOfCourtesy":null,"reportsTo":{"birthDate":null,"comment":null,"employeeAddress":null,"employeeCity":null,"employeeCountry":null,"employeeLinkedIn":null,"employeePostalCode":"98401","employeeSalary":{"systemAEmployeeSalary":null,"systemBEmployeeAnnualSalary":48.0,"systemBEmployeeMonthlySalary":4.199999809265137},"employer":{},"extension":null,"favorite":{},"firstName":null,"hireDate":null,"homePhone":null,"label":"SystemB employee-2","lastName":null,"lat":null,"lat_long":null,"long":null,"notes":null,"photo":null,"regionDescription":null,"reportsToId":null,"reportsToNotation":null,"subjectId":"NWD~SystemBEmployee-2","territoryNotation":null,"title":null,"titleOfCourtesy":null}}}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order(employee(reportsTo()))/$entity","comment":null,"customerId":"NWD~Customer-TOMSP","customerNotation":null,"employeeId":"NWD~Employee-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">6","employeeNotation":null,"freight":11.61,"label":"Order-10249","lat":51.6566,"lat_long":"51.6566000,7.0904400","long":7.09044,"orderDate":"2016-07-05T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-08-16T00:00:00Z","shipAddress":"Luisenstr. 48","shipCity":"Münster","shipCountry":"Germany","shipName":"Toms Spezialitäten","shipPostalCode":"44087","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2016-07-10T00:00:00Z","subjectId":"NWD~Order-10249","employee":{"birthDate":"1983-07-02","comment":null,"employeeAddress":"Coventry House\\nMiner Rd.","employeeCity":"London","employeeCountry":"UK","employeeLinkedIn":null,"employeePostalCode":"EC2 7JR","employeeSalary":null,"employer":null,"extension":"428","favorite":null,"firstName":"Michael","hireDate":"2013-10-17","homePhone":"(71) 555-7773","label":"Employee-6","lastName":"Suyama","lat":51.5100082,"lat_long":"51.5100082,-0.1329494","long":-0.1329494,"notes":"Michael is a graduate of Sussex University (MA, economics, 1983) and the University of California at Los Angeles (MBA, marketing, 1986). He has also taken the courses Multi-Cultural Selling and Time Management for the Sales Professional. He is fluent in Japanese and can read and write French, Portuguese, and Spanish.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-5","reportsToNotation":null,"subjectId":"NWD~Employee-6","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Mr.","reportsTo":{"birthDate":"1972-02-19","comment":null,"employeeAddress":"908 W. Capital Way","employeeCity":"Tacoma","employeeCountry":"USA","employeeLinkedIn":"https://www.linkedin.com/in/peterjohnlawrence/","employeePostalCode":"98401","employeeSalary":null,"employer":null,"extension":"3457","favorite":null,"firstName":"Andrew","hireDate":"2012-08-14","homePhone":"(206) 555-9482","label":"MatchingEmployee-2","lastName":"Fuller","lat":null,"lat_long":null,"long":null,"notes":"Andrew received his BTS commercial in 1974 and a Ph.D. in international marketing from the University of Dallas in 1981. He is fluent in French and Italian and reads German. He joined the company as a sales representative, was promoted to sales manager in January 1992 and to vice president of sales in March 1993. Andrew is a member of the Sales Management Roundtable, the Seattle Chamber of Commerce, and the Pacific Rim Importers Association.","photo":"http://accweb/emmployees/fuller.bmp","regionDescription":null,"reportsToId":"NWD~Employee-5","reportsToNotation":null,"subjectId":"NWD~MatchingEmployee-2","territoryNotation":null,"title":"Vice President, Sales","titleOfCourtesy":"Doctor"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">}}}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">URI2.12</t>
@@ -1273,7 +1541,32 @@
     <t xml:space="preserve">$expand=shipVia,employee($expand=reportsTo)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order(employee(reportsTo()),shipVia())/$entity","comment":null,"customerId":"NWD~Customer-TOMSP","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":11.61,"label":"Order-10249","lat":51.6566,"lat_long":"51.6566000,7.0904400","long":7.09044,"orderDate":"2016-07-05T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-08-16T00:00:00Z","shipAddress":"Luisenstr. 48","shipCity":"Münster","shipCountry":"Germany","shipName":"Toms Spezialitäten","shipPostalCode":"44087","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2016-07-10T00:00:00Z","subjectId":"NWD~Order-10249","employee":{"birthDate":null,"comment":null,"employeeAddress":null,"employeeCity":null,"employeeCountry":null,"employeeLinkedIn":null,"employeePostalCode":null,"employeeSalary":null,"employer":null,"extension":null,"favorite":null,"firstName":null,"hireDate":null,"homePhone":null,"label":null,"lastName":null,"lat":null,"lat_long":null,"long":null,"notes":null,"photo":null,"regionDescription":null,"reportsToId":"NWD~SystemBEmployee-2","reportsToNotation":null,"subjectId":"NWD~SystemAEmployee-1","territoryNotation":null,"title":null,"titleOfCourtesy":null,"reportsTo":{"birthDate":null,"comment":null,"employeeAddress":null,"employeeCity":null,"employeeCountry":null,"employeeLinkedIn":null,"employeePostalCode":"98401","employeeSalary":{"systemAEmployeeSalary":null,"systemBEmployeeAnnualSalary":48.0,"systemBEmployeeMonthlySalary":4.199999809265137},"employer":{},"extension":null,"favorite":{},"firstName":null,"hireDate":null,"homePhone":null,"label":"SystemB employee-2","lastName":null,"lat":null,"lat_long":null,"long":null,"notes":null,"photo":null,"regionDescription":null,"reportsToId":null,"reportsToNotation":null,"subjectId":"NWD~SystemBEmployee-2","territoryNotation":null,"title":null,"titleOfCourtesy":null}},"shipVia":{"comment":null,"label":"Shipper-1","shipperCompanyName":"Speedy Express","shipperPhone":"(503) 555-9831","subjectId":"NWD~Shipper-1"}}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order(employee(reportsTo()),shipVia())/$entity","comment":null,"customerId":"NWD~Customer-TOMSP","customerNotation":null,"employeeId":"NWD~Employee-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">6","employeeNotation":null,"freight":11.61,"label":"Order-10249","lat":51.6566,"lat_long":"51.6566000,7.0904400","long":7.09044,"orderDate":"2016-07-05T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-08-16T00:00:00Z","shipAddress":"Luisenstr. 48","shipCity":"Münster","shipCountry":"Germany","shipName":"Toms Spezialitäten","shipPostalCode":"44087","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2016-07-10T00:00:00Z","subjectId":"NWD~Order-10249","employee":{"birthDate":"1983-07-02","comment":null,"employeeAddress":"Coventry House\\nMiner Rd.","employeeCity":"London","employeeCountry":"UK","employeeLinkedIn":null,"employeePostalCode":"EC2 7JR","employeeSalary":null,"employer":null,"extension":"428","favorite":null,"firstName":"Michael","hireDate":"2013-10-17","homePhone":"(71) 555-7773","label":"Employee-6","lastName":"Suyama","lat":51.5100082,"lat_long":"51.5100082,-0.1329494","long":-0.1329494,"notes":"Michael is a graduate of Sussex University (MA, economics, 1983) and the University of California at Los Angeles (MBA, marketing, 1986). He has also taken the courses Multi-Cultural Selling and Time Management for the Sales Professional. He is fluent in Japanese and can read and write French, Portuguese, and Spanish.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-5","reportsToNotation":null,"subjectId":"NWD~Employee-6","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Mr.","reportsTo":{"birthDate":"1972-02-19","comment":null,"employeeAddress":"908 W. Capital Way","employeeCity":"Tacoma","employeeCountry":"USA","employeeLinkedIn":"https://www.linkedin.com/in/peterjohnlawrence/","employeePostalCode":"98401","employeeSalary":null,"employer":null,"extension":"3457","favorite":null,"firstName":"Andrew","hireDate":"2012-08-14","homePhone":"(206) 555-9482","label":"MatchingEmployee-2","lastName":"Fuller","lat":null,"lat_long":null,"long":null,"notes":"Andrew received his BTS commercial in 1974 and a Ph.D. in international marketing from the University of Dallas in 1981. He is fluent in French and Italian and reads German. He joined the company as a sales representative, was promoted to sales manager in January 1992 and to vice president of sales in March 1993. Andrew is a member of the Sales Management Roundtable, the Seattle Chamber of Commerce, and the Pacific Rim Importers Association.","photo":"http://accweb/emmployees/fuller.bmp","regionDescription":null,"reportsToId":"NWD~Employee-5","reportsToNotation":null,"subjectId":"NWD~MatchingEmployee-2","territoryNotation":null,"title":"Vice President, Sales","titleOfCourtesy":"Doctor"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">}},"shipVia":{"comment":null,"label":"Shipper-1","shipperCompanyName":"Speedy Express","shipperPhone":"(503) 555-9831","subjectId":"NWD~Shipper-1"}}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">URI2.14</t>
@@ -1282,7 +1575,33 @@
     <t xml:space="preserve">$expand=employee($expand=reportsTo($expand=reportsTo))</t>
   </si>
   <si>
-    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order(employee(reportsTo(reportsTo())))/$entity","comment":null,"customerId":"NWD~Customer-TOMSP","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":11.61,"label":"Order-10249","lat":51.6566,"lat_long":"51.6566000,7.0904400","long":7.09044,"orderDate":"2016-07-05T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-08-16T00:00:00Z","shipAddress":"Luisenstr. 48","shipCity":"Münster","shipCountry":"Germany","shipName":"Toms Spezialitäten","shipPostalCode":"44087","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2016-07-10T00:00:00Z","subjectId":"NWD~Order-10249","employee":{"birthDate":null,"comment":null,"employeeAddress":null,"employeeCity":null,"employeeCountry":null,"employeeLinkedIn":null,"employeePostalCode":null,"employeeSalary":null,"employer":null,"extension":null,"favorite":null,"firstName":null,"hireDate":null,"homePhone":null,"label":null,"lastName":null,"lat":null,"lat_long":null,"long":null,"notes":null,"photo":null,"regionDescription":null,"reportsToId":"NWD~SystemBEmployee-2","reportsToNotation":null,"subjectId":"NWD~SystemAEmployee-1","territoryNotation":null,"title":null,"titleOfCourtesy":null,"reportsTo":{"birthDate":null,"comment":null,"employeeAddress":null,"employeeCity":null,"employeeCountry":null,"employeeLinkedIn":null,"employeePostalCode":"98401","employeeSalary":{"systemAEmployeeSalary":null,"systemBEmployeeAnnualSalary":48.0,"systemBEmployeeMonthlySalary":4.199999809265137},"employer":{},"extension":null,"favorite":{},"firstName":null,"hireDate":null,"homePhone":null,"label":"SystemB employee-2","lastName":null,"lat":null,"lat_long":null,"long":null,"notes":null,"photo":null,"regionDescription":null,"reportsToId":null,"reportsToNotation":null,"subjectId":"NWD~SystemBEmployee-2","territoryNotation":null,"title":null,"titleOfCourtesy":null,"reportsTo":null}}}</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order(employee(reportsTo(reportsTo())))/$entity","comment":null,"customerId":"NWD~Customer-TOMSP","customerNotation":null,"employeeId":"NWD~Employee-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">6","employeeNotation":null,"freight":11.61,"label":"Order-10249","lat":51.6566,"lat_long":"51.6566000,7.0904400","long":7.09044,"orderDate":"2016-07-05T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-08-16T00:00:00Z","shipAddress":"Luisenstr. 48","shipCity":"Münster","shipCountry":"Germany","shipName":"Toms Spezialitäten","shipPostalCode":"44087","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2016-07-10T00:00:00Z","subjectId":"NWD~Order-10249","employee":{"birthDate":"1983-07-02","comment":null,"employeeAddress":"Coventry House\\nMiner Rd.","employeeCity":"London","employeeCountry":"UK","employeeLinkedIn":null,"employeePostalCode":"EC2 7JR","employeeSalary":null,"employer":null,"extension":"428","favorite":null,"firstName":"Michael","hireDate":"2013-10-17","homePhone":"(71) 555-7773","label":"Employee-6","lastName":"Suyama","lat":51.5100082,"lat_long":"51.5100082,-0.1329494","long":-0.1329494,"notes":"Michael is a graduate of Sussex University (MA, economics, 1983) and the University of California at Los Angeles (MBA, marketing, 1986). He has also taken the courses Multi-Cultural Selling and Time Management for the Sales Professional. He is fluent in Japanese and can read and write French, Portuguese, and Spanish.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-5","reportsToNotation":null,"subjectId":"NWD~Employee-6","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Mr.","reportsTo":{"birthDate":"1972-02-19","comment":null,"employeeAddress":"908 W. Capital Way","employeeCity":"Tacoma","employeeCountry":"USA","employeeLinkedIn":"https://www.linkedin.com/in/peterjohnlawrence/","employeePostalCode":"98401","employeeSalary":null,"employer":null,"extension":"3457","favorite":null,"firstName":"Andrew","hireDate":"2012-08-14","homePhone":"(206) 555-9482","label":"MatchingEmployee-2","lastName":"Fuller","lat":null,"lat_long":null,"long":null,"notes":"Andrew received his BTS commercial in 1974 and a Ph.D. in international marketing from the University of Dallas in 1981. He is fluent in French and Italian and reads German. He joined the company as a sales representative, was promoted to sales manager in January 1992 and to vice president of sales in March 1993. Andrew is a member of the Sales Management Roundtable, the Seattle Chamber of Commerce, and the Pacific Rim Importers Association.","photo":"http://accweb/emmployees/fuller.bmp","regionDescription":null,"reportsToId":"NWD~Employee-5","reportsToNotation":null,"subjectId":"NWD~MatchingEmployee-2","territoryNotation":null,"title":"Vice President, Sales","titleOfCourtesy":"Doctor","reportsTo":{"birthDate":"1975-03-04","comment":null,"employeeAddress":"14 Garrett Hill","employeeCity":"London","employeeCountry":"UK","employeeLinkedIn":null,"employeePostalCode":"SW1 8JR","employeeSalary":null,"employer":null,"extension":"3453","favorite":null,"firstName":"Steven","hireDate":"2013-10-17","homePhone":"(71) 555-4848","label":"Employee-5","lastName":"Buchanan","lat":51.5239508,"lat_long":"51.5239508,-0.0944701","long":-0.0944701,"notes":"Steven Buchanan graduated from St. Andrews University, Scotland, with a BSC degree in 1976. Upon joining the company as a sales representative in 1992, he spent 6 months in an orientation program at the Seattle office and then returned to his permanent post in London. He was promoted to sales manager in March 1993. Mr. Buchanan has completed the courses Successful Telemarketing and International Sales Management. He is fluent in French.","photo":"http://accweb/emmployees/buchanan.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-5","territoryNotation":null,"title":"Sales Manager","titleOfCourtesy":"Mr."}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">}}}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">URI2.15</t>
@@ -1561,6 +1880,26 @@
     <t xml:space="preserve">Employee('NWD~SystemAEmployee-1')/employeeSalary/systemAEmployeeSalary/$value</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">42</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.0</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">URI4 Simple property of a complex property of an entity</t>
   </si>
   <si>
@@ -2152,16 +2491,93 @@
     <t xml:space="preserve">$filter= (shipCountry eq 'France') or (shipCountry eq 'Germany')&amp;$skip=0&amp;$top=10</t>
   </si>
   <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order","value":[{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-4","employeeNotation":null,"freight":108.26,"label":"Order-10337","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2016-10-24T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-11-21T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2016-10-29T00:00:00Z","subjectId":"NWD~Order-10337"},{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-7","employeeNotation":null,"freight":105.65,"label":"Order-10513","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2017-04-22T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-06-03T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-04-28T00:00:00Z","subjectId":"NWD~Order-10513"},{"comment":null,"customerId":"NWD~Customer-QUICK","customerNotation":null,"employeeId":"NWD~Employee-3","employeeNotation":null,"freight":1007.64,"label":"Order-10540","lat":51.1799698,"lat_long":"51.1799698,14.4370284","long":14.4370284,"orderDate":"2017-05-19T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-06-16T00:00:00Z","shipAddress":"Taucherstraße 10","shipCity":"Cunewalde","shipCountry":"Germany","shipName":"QUICK-Stop","shipPostalCode":"01307","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2017-06-13T00:00:00Z","subjectId":"NWD~Order-10540"},{"comment":null,"customerId":"NWD~Customer-BONAP","customerNotation":null,"employeeId":"NWD~Employee-2","employeeNotation":null,"freight":113.15,"label":"Order-10663","lat":43.2611295,"lat_long":"43.2611295,5.3886613","long":5.3886613,"orderDate":"2017-09-10T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-24T00:00:00Z","shipAddress":"12, rue des Bouchers","shipCity":"Marseille","shipCountry":"France","shipName":"Bon app'","shipPostalCode":"13008","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2017-10-03T00:00:00Z","subjectId":"NWD~Order-10663"},{"comment":null,"customerId":"NWD~Customer-BONAP","customerNotation":null,"employeeId":"NWD~Employee-4","employeeNotation":null,"freight":16.709999,"label":"Order-10755","lat":43.2611295,"lat_long":"43.2611295,5.3886613","long":5.3886613,"orderDate":"2017-11-26T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-12-24T00:00:00Z","shipAddress":"12, rue des Bouchers","shipCity":"Marseille","shipCountry":"France","shipName":"Bon app'","shipPostalCode":"13008","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2017-11-28T00:00:00Z","subjectId":"NWD~Order-10755"},{"comment":null,"customerId":"NWD~Customer-FOLIG","customerNotation":null,"employeeId":"NWD~Employee-3","employeeNotation":null,"freight":37.349998,"label":"Order-10763","lat":50.5690579,"lat_long":"50.5690579,3.2223336","long":3.2223336,"orderDate":"2017-12-03T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-12-31T00:00:00Z","shipAddress":"184, chaussée de Tournai","shipCity":"Lille","shipCountry":"France","shipName":"Folies gourmandes","shipPostalCode":"59000","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2017-12-08T00:00:00Z","subjectId":"NWD~Order-10763"},{"comment":null,"customerId":"NWD~Customer-MORGK","customerNotation":null,"employeeId":"NWD~Employee-3","employeeNotation":null,"freight":58.130001,"label":"Order-10779","lat":51.2200438,"lat_long":"51.2200438,12.1401173","long":12.1401173,"orderDate":"2017-12-16T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2008-01-13T00:00:00Z","shipAddress":"Heerstr. 22","shipCity":"Leipzig","shipCountry":"Germany","shipName":"Morgenstern Gesundkost","shipPostalCode":"04179","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2008-01-14T00:00:00Z","subjectId":"NWD~Order-10779"},{"comment":null,"customerId":"NWD~Customer-LAMAI","customerNotation":null,"employeeId":"NWD~Employee-7","employeeNotation":null,"freight":68.260002,"label":"Order-10923","lat":43.5996235,"lat_long":"43.5996235,1.4454683","long":1.4454683,"orderDate":"2008-03-03T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2008-04-14T00:00:00Z","shipAddress":"1 rue Alsace-Lorraine","shipCity":"Toulouse","shipCountry":"France","shipName":"La maison d'Asie","shipPostalCode":"31000","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2008-03-13T00:00:00Z","subjectId":"NWD~Order-10923"},{"comment":null,"customerId":"NWD~Customer-QUICK","customerNotation":null,"employeeId":"NWD~Employee-8","employeeNotation":null,"freight":275.79001,"label":"Order-10962","lat":51.1799698,"lat_long":"51.1799698,14.4370284","long":14.4370284,"orderDate":"2008-03-19T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2008-04-16T00:00:00Z","shipAddress":"Taucherstraße 10","shipCity":"Cunewalde","shipCountry":"Germany","shipName":"QUICK-Stop","shipPostalCode":"01307","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2008-03-23T00:00:00Z","subjectId":"NWD~Order-10962"},{"comment":null,"customerId":"NWD~Customer-QUICK","customerNotation":null,"employeeId":"NWD~Employee-3","employeeNotation":null,"freight":297.17999,"label":"Order-11021","lat":51.1799698,"lat_long":"51.1799698,14.4370284","long":14.4370284,"orderDate":"2008-04-14T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2008-05-12T00:00:00Z","shipAddress":"Taucherstraße 10","shipCity":"Cunewalde","shipCountry":"Germany","shipName":"QUICK-Stop","shipPostalCode":"01307","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2008-04-21T00:00:00Z","subjectId":"NWD~Order-11021"}]}</t>
+  </si>
+  <si>
     <t xml:space="preserve">$filter= (shipCountry eq 'France') or (shipCountry eq 'Germany')&amp;$expand=customer&amp;$skip=0&amp;$top=10</t>
   </si>
   <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order(customer())","value":[{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-4","employeeNotation":null,"freight":108.26,"label":"Order-10337","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2016-10-24T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-11-21T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2016-10-29T00:00:00Z","subjectId":"NWD~Order-10337","customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-7","employeeNotation":null,"freight":105.65,"label":"Order-10513","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2017-04-22T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-06-03T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-04-28T00:00:00Z","subjectId":"NWD~Order-10513","customer":{"comment":null,"customerAddress":"Adenauerallee 900","customerCity":"Stuttgart","customerCompanyName":"Die Wandernde Kuh","customerContactName":"Rita Müller","customerContactTitle":"Sales Representative","customerCountry":"Germany","customerFax":"0711-035428","customerPhone":"0711-020361","customerPostalCode":"70563","customerWebsite":null,"label":"Die Wandernde Kuh","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"regionDescription":null,"subjectId":"NWD~Customer-WANDK"}},{"comment":null,"customerId":"NWD~Customer-QUICK","customerNotation":null,"employeeId":"NWD~Employee-3","employeeNotation":null,"freight":1007.64,"label":"Order-10540","lat":51.1799698,"lat_long":"51.1799698,14.4370284","long":14.4370284,"orderDate":"2017-05-19T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-06-16T00:00:00Z","shipAddress":"Taucherstraße 10","shipCity":"Cunewalde","shipCountry":"Germany","shipName":"QUICK-Stop","shipPostalCode":"01307","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2017-06-13T00:00:00Z","subjectId":"NWD~Order-10540","customer":{"comment":null,"customerAddress":"Taucherstraße 10","customerCity":"Cunewalde","customerCompanyName":"QUICK-Stop","customerContactName":"Horst Kloss","customerContactTitle":"Accounting Manager","customerCountry":"Germany","customerFax":null,"customerPhone":"0372-035188","customerPostalCode":"01307","customerWebsite":null,"label":"QUICK-Stop","lat":51.1799698,"lat_long":"51.1799698,14.4370284","long":14.4370284,"regionDescription":null,"subjectId":"NWD~Customer-QUICK"}},{"comment":null,"customerId":"NWD~Customer-BONAP","customerNotation":null,"employeeId":"NWD~Employee-2","employeeNotation":null,"freight":113.15,"label":"Order-10663","lat":43.2611295,"lat_long":"43.2611295,5.3886613","long":5.3886613,"orderDate":"2017-09-10T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-24T00:00:00Z","shipAddress":"12, rue des Bouchers","shipCity":"Marseille","shipCountry":"France","shipName":"Bon app'","shipPostalCode":"13008","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2017-10-03T00:00:00Z","subjectId":"NWD~Order-10663","customer":{"comment":null,"customerAddress":"12, rue des Bouchers","customerCity":"Marseille","customerCompanyName":"Bon app'","customerContactName":"Laurence Lebihan","customerContactTitle":"Owner","customerCountry":"France","customerFax":"91.24.45.41","customerPhone":"91.24.45.40","customerPostalCode":"13008","customerWebsite":null,"label":"Bon app'","lat":43.2611295,"lat_long":"43.2611295,5.3886613","long":5.3886613,"regionDescription":null,"subjectId":"NWD~Customer-BONAP"}},{"comment":null,"customerId":"NWD~Customer-BONAP","customerNotation":null,"employeeId":"NWD~Employee-4","employeeNotation":null,"freight":16.709999,"label":"Order-10755","lat":43.2611295,"lat_long":"43.2611295,5.3886613","long":5.3886613,"orderDate":"2017-11-26T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-12-24T00:00:00Z","shipAddress":"12, rue des Bouchers","shipCity":"Marseille","shipCountry":"France","shipName":"Bon app'","shipPostalCode":"13008","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2017-11-28T00:00:00Z","subjectId":"NWD~Order-10755","customer":{"comment":null,"customerAddress":"12, rue des Bouchers","customerCity":"Marseille","customerCompanyName":"Bon app'","customerContactName":"Laurence Lebihan","customerContactTitle":"Owner","customerCountry":"France","customerFax":"91.24.45.41","customerPhone":"91.24.45.40","customerPostalCode":"13008","customerWebsite":null,"label":"Bon app'","lat":43.2611295,"lat_long":"43.2611295,5.3886613","long":5.3886613,"regionDescription":null,"subjectId":"NWD~Customer-BONAP"}},{"comment":null,"customerId":"NWD~Customer-FOLIG","customerNotation":null,"employeeId":"NWD~Employee-3","employeeNotation":null,"freight":37.349998,"label":"Order-10763","lat":50.5690579,"lat_long":"50.5690579,3.2223336","long":3.2223336,"orderDate":"2017-12-03T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-12-31T00:00:00Z","shipAddress":"184, chaussée de Tournai","shipCity":"Lille","shipCountry":"France","shipName":"Folies gourmandes","shipPostalCode":"59000","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2017-12-08T00:00:00Z","subjectId":"NWD~Order-10763","customer":{"comment":null,"customerAddress":"184, chaussée de Tournai","customerCity":"Lille","customerCompanyName":"Folies gourmandes","customerContactName":"Martine Rancé","customerContactTitle":"Assistant Sales Agent","customerCountry":"France","customerFax":"20.16.10.17","customerPhone":"20.16.10.16","customerPostalCode":"59000","customerWebsite":null,"label":"Folies gourmandes","lat":50.5690579,"lat_long":"50.5690579,3.2223336","long":3.2223336,"regionDescription":null,"subjectId":"NWD~Customer-FOLIG"}},{"comment":null,"customerId":"NWD~Customer-MORGK","customerNotation":null,"employeeId":"NWD~Employee-3","employeeNotation":null,"freight":58.130001,"label":"Order-10779","lat":51.2200438,"lat_long":"51.2200438,12.1401173","long":12.1401173,"orderDate":"2017-12-16T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2008-01-13T00:00:00Z","shipAddress":"Heerstr. 22","shipCity":"Leipzig","shipCountry":"Germany","shipName":"Morgenstern Gesundkost","shipPostalCode":"04179","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2008-01-14T00:00:00Z","subjectId":"NWD~Order-10779","customer":{"comment":null,"customerAddress":"Heerstr. 22","customerCity":"Leipzig","customerCompanyName":"Morgenstern Gesundkost","customerContactName":"Alexander Feuer","customerContactTitle":"Marketing Assistant","customerCountry":"Germany","customerFax":null,"customerPhone":"0342-023176","customerPostalCode":"04179","customerWebsite":null,"label":"Morgenstern Gesundkost","lat":51.2200438,"lat_long":"51.2200438,12.1401173","long":12.1401173,"regionDescription":null,"subjectId":"NWD~Customer-MORGK"}},{"comment":null,"customerId":"NWD~Customer-LAMAI","customerNotation":null,"employeeId":"NWD~Employee-7","employeeNotation":null,"freight":68.260002,"label":"Order-10923","lat":43.5996235,"lat_long":"43.5996235,1.4454683","long":1.4454683,"orderDate":"2008-03-03T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2008-04-14T00:00:00Z","shipAddress":"1 rue Alsace-Lorraine","shipCity":"Toulouse","shipCountry":"France","shipName":"La maison d'Asie","shipPostalCode":"31000","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2008-03-13T00:00:00Z","subjectId":"NWD~Order-10923","customer":{"comment":null,"customerAddress":"1 rue Alsace-Lorraine","customerCity":"Toulouse","customerCompanyName":"La maison d'Asie","customerContactName":"Annette Roulet","customerContactTitle":"Sales Manager","customerCountry":"France","customerFax":"61.77.61.11","customerPhone":"61.77.61.10","customerPostalCode":"31000","customerWebsite":null,"label":"La maison d'Asie","lat":43.5996235,"lat_long":"43.5996235,1.4454683","long":1.4454683,"regionDescription":null,"subjectId":"NWD~Customer-LAMAI"}},{"comment":null,"customerId":"NWD~Customer-QUICK","customerNotation":null,"employeeId":"NWD~Employee-8","employeeNotation":null,"freight":275.79001,"label":"Order-10962","lat":51.1799698,"lat_long":"51.1799698,14.4370284","long":14.4370284,"orderDate":"2008-03-19T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2008-04-16T00:00:00Z","shipAddress":"Taucherstraße 10","shipCity":"Cunewalde","shipCountry":"Germany","shipName":"QUICK-Stop","shipPostalCode":"01307","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2008-03-23T00:00:00Z","subjectId":"NWD~Order-10962","customer":{"comment":null,"customerAddress":"Taucherstraße 10","customerCity":"Cunewalde","customerCompanyName":"QUICK-Stop","customerContactName":"Horst Kloss","customerContactTitle":"Accounting Manager","customerCountry":"Germany","customerFax":null,"customerPhone":"0372-035188","customerPostalCode":"01307","customerWebsite":null,"label":"QUICK-Stop","lat":51.1799698,"lat_long":"51.1799698,14.4370284","long":14.4370284,"regionDescription":null,"subjectId":"NWD~Customer-QUICK"}},{"comment":null,"customerId":"NWD~Customer-QUICK","customerNotation":null,"employeeId":"NWD~Employee-3","employeeNotation":null,"freight":297.17999,"label":"Order-11021","lat":51.1799698,"lat_long":"51.1799698,14.4370284","long":14.4370284,"orderDate":"2008-04-14T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2008-05-12T00:00:00Z","shipAddress":"Taucherstraße 10","shipCity":"Cunewalde","shipCountry":"Germany","shipName":"QUICK-Stop","shipPostalCode":"01307","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2008-04-21T00:00:00Z","subjectId":"NWD~Order-11021","customer":{"comment":null,"customerAddress":"Taucherstraße 10","customerCity":"Cunewalde","customerCompanyName":"QUICK-Stop","customerContactName":"Horst Kloss","customerContactTitle":"Accounting Manager","customerCountry":"Germany","customerFax":null,"customerPhone":"0372-035188","customerPostalCode":"01307","customerWebsite":null,"label":"QUICK-Stop","lat":51.1799698,"lat_long":"51.1799698,14.4370284","long":14.4370284,"regionDescription":null,"subjectId":"NWD~Customer-QUICK"}}]}</t>
+  </si>
+  <si>
     <t xml:space="preserve">$filter= (shipCountry eq 'France') or (shipCountry eq 'Germany')&amp;$expand=customer($filter=(customerCompanyName eq 'Frankenversand'))&amp;$skip=0&amp;$top=10</t>
   </si>
   <si>
-    <t xml:space="preserve">$filter= (shipCountry eq 'France') or (shipCountry eq 'Germany')&amp;$expand=customer($filter=(customerCompanyName eq 'Frankenversand')),employee&amp;$skip=0&amp;$top=10</t>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order(customer())","value":[{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-4","employeeNotation":null,"freight":108.26,"label":"Order-10337","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2016-10-24T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-11-21T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2016-10-29T00:00:00Z","subjectId":"NWD~Order-10337","customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":135.35001,"label":"Order-10396","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2016-12-27T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-01-10T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2017-01-06T00:00:00Z","subjectId":"NWD~Order-10396","customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-8","employeeNotation":null,"freight":4.9299998,"label":"Order-10488","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2017-03-27T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-04-24T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2017-04-02T00:00:00Z","subjectId":"NWD~Order-10488","customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-8","employeeNotation":null,"freight":36.650002,"label":"Order-10560","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2017-06-06T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-07-04T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-06-09T00:00:00Z","subjectId":"NWD~Order-10560","customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-8","employeeNotation":null,"freight":97.18,"label":"Order-10623","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2017-08-07T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-04T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2017-08-12T00:00:00Z","subjectId":"NWD~Order-10623","customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":93.25,"label":"Order-10653","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2017-09-02T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-30T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-09-19T00:00:00Z","subjectId":"NWD~Order-10653","customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":59.25,"label":"Order-10717","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2017-10-24T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-11-21T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2017-10-29T00:00:00Z","subjectId":"NWD~Order-10717","customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-6","employeeNotation":null,"freight":16.85,"label":"Order-10791","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2017-12-23T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2018-01-20T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2018-01-01T00:00:00Z","subjectId":"NWD~Order-10791","customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":76.099998,"label":"Order-10859","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2018-01-29T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2018-02-26T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2018-02-02T00:00:00Z","subjectId":"NWD~Order-10859","customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":242.95,"label":"Order-11012","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2018-04-09T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2018-04-23T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2018-04-17T00:00:00Z","subjectId":"NWD~Order-11012","customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$filter= (shipCountry eq 'France') or (shipCountry eq 'Germany')&amp;$expand=customer($filter=(customerCompanyName eq 'Frankenversand')),employee&amp;$skip=0&amp;$top=5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order(employee(),customer())","value":[{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-4","employeeNotation":null,"freight":108.26,"label":"Order-10337","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2016-10-24T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-11-21T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2016-10-29T00:00:00Z","subjectId":"NWD~Order-10337","employee":{"birthDate":"1957-09-19","comment":null,"employeeAddress":"4110 Old Redmond Rd.","employeeCity":"Redmond","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98052","employeeSalary":null,"employer":null,"extension":"5176","favorite":null,"firstName":"Margaret","hireDate":"2013-05-03","homePhone":"(206) 555-8122","label":"Employee-4","lastName":"Peacock","lat":47.6679429,"lat_long":"47.6679429,-122.1334222","long":-122.1334222,"notes":"Margaret holds a BA in English literature from Concordia College (1958) and an MA from the American Institute of Culinary Arts (1966). She was assigned to the London office temporarily from July through November 1992.","photo":"http://accweb/emmployees/peacock.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-4","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Mrs."},"customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">8","employeeNotation":null,"freight":97.18,"label":"Order-10623","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2017-08-07T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-04T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2017-08-12T00:00:00Z","subjectId":"NWD~Order-10623","employee":{"birthDate":"1978-01-09","comment":null,"employeeAddress":"4726 - 11th Ave. N.E.","employeeCity":"Seattle","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98105","employeeSalary":null,"employer":null,"extension":"2344","favorite":null,"firstName":"Laura","hireDate":"2014-03-05","homePhone":"(206) 555-1189","label":"Employee-8","lastName":"Callahan","lat":47.6641642,"lat_long":"47.6641642,-122.3160149","long":-122.3160149,"notes":"Laura received a BA in psychology from the University of Washington. She has also completed a course in business French. She reads and writes French.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-8","territoryNotation":null,"title":"Inside Sales Coordinator","titleOfCourtesy":"Ms."},"customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":93.25,"label":"Order-10653","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2017-09-02T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-30T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-09-19T00:00:00Z","subjectId":"NWD~Order-10653","employee":{"birthDate":"1968-12-08","comment":null,"employeeAddress":"507 - 20th Ave. E.\\nApt. 2A","employeeCity":"Seattle","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98122","employeeSalary":null,"employer":null,"extension":"5467","favorite":null,"firstName":"Nancy","hireDate":"2012-05-01","homePhone":"(206) 555-9857","label":"Employee-1","lastName":"Davolio","lat":47.6234778,"lat_long":"47.6234778,-122.3063220","long":-122.306322,"notes":"Education includes a BA in psychology from Colorado State University in 1970. She also completed The Art of the Cold Call. Nancy is a member of Toastmasters International.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-1","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Ms."},"customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-6","employeeNotation":null,"freight":16.85,"label":"Order-10791","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2017-12-23T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2018-01-20T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2018-01-01T00:00:00Z","subjectId":"NWD~Order-10791","employee":{"birthDate":"1983-07-02","comment":null,"employeeAddress":"Coventry House\\nMiner Rd.","employeeCity":"London","employeeCountry":"UK","employeeLinkedIn":null,"employeePostalCode":"EC2 7JR","employeeSalary":null,"employer":null,"extension":"428","favorite":null,"firstName":"Michael","hireDate":"2013-10-17","homePhone":"(71) 555-7773","label":"Employee-6","lastName":"Suyama","lat":51.5100082,"lat_long":"51.5100082,-0.1329494","long":-0.1329494,"notes":"Michael is a graduate of Sussex University (MA, economics, 1983) and the University of California at Los Angeles (MBA, marketing, 1986). He has also taken the courses Multi-Cultural Selling and Time Management for the Sales Professional. He is fluent in Japanese and can read and write French, Portuguese, and Spanish.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-5","reportsToNotation":null,"subjectId":"NWD~Employee-6","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Mr."},"customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":242.95,"label":"Order-11012","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2018-04-09T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2018-04-23T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2018-04-17T00:00:00Z","subjectId":"NWD~Order-11012","employee":{"birthDate":"1968-12-08","comment":null,"employeeAddress":"507 - 20th Ave. E.\\nApt. 2A","employeeCity":"Seattle","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98122","employeeSalary":null,"employer":null,"extension":"5467","favorite":null,"firstName":"Nancy","hireDate":"2012-05-01","homePhone":"(206) 555-9857","label":"Employee-1","lastName":"Davolio","lat":47.6234778,"lat_long":"47.6234778,-122.3063220","long":-122.306322,"notes":"Education includes a BA in psychology from Colorado State University in 1970. She also completed The Art of the Cold Call. Nancy is a member of Toastmasters International.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-1","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Ms."},"customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}}]}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">$filter= (shipCountry eq 'France') or (shipCountry eq 'Germany')&amp;$expand=customer($filter=(customerCompanyName eq 'Frankenversand')),employee($filter=(firstName eq 'Nancy'))&amp;$skip=0&amp;$top=10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order(employee(),customer())","value":[{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":135.35001,"label":"Order-10396","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2016-12-27T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-01-10T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2017-01-06T00:00:00Z","subjectId":"NWD~Order-10396","employee":{"birthDate":"1968-12-08","comment":null,"employeeAddress":"507 - 20th Ave. E.\\nApt. 2A","employeeCity":"Seattle","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98122","employeeSalary":null,"employer":null,"extension":"5467","favorite":null,"firstName":"Nancy","hireDate":"2012-05-01","homePhone":"(206) 555-9857","label":"Employee-1","lastName":"Davolio","lat":47.6234778,"lat_long":"47.6234778,-122.3063220","long":-122.306322,"notes":"Education includes a BA in psychology from Colorado State University in 1970. She also completed The Art of the Cold Call. Nancy is a member of Toastmasters International.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-1","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Ms."},"customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":93.25,"label":"Order-10653","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2017-09-02T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-30T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-09-19T00:00:00Z","subjectId":"NWD~Order-10653","employee":{"birthDate":"1968-12-08","comment":null,"employeeAddress":"507 - 20th Ave. E.\\nApt. 2A","employeeCity":"Seattle","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98122","employeeSalary":null,"employer":null,"extension":"5467","favorite":null,"firstName":"Nancy","hireDate":"2012-05-01","homePhone":"(206) 555-9857","label":"Employee-1","lastName":"Davolio","lat":47.6234778,"lat_long":"47.6234778,-122.3063220","long":-122.306322,"notes":"Education includes a BA in psychology from Colorado State University in 1970. She also completed The Art of the Cold Call. Nancy is a member of Toastmasters International.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-1","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Ms."},"customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":59.25,"label":"Order-10717","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2017-10-24T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-11-21T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2017-10-29T00:00:00Z","subjectId":"NWD~Order-10717","employee":{"birthDate":"1968-12-08","comment":null,"employeeAddress":"507 - 20th Ave. E.\\nApt. 2A","employeeCity":"Seattle","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98122","employeeSalary":null,"employer":null,"extension":"5467","favorite":null,"firstName":"Nancy","hireDate":"2012-05-01","homePhone":"(206) 555-9857","label":"Employee-1","lastName":"Davolio","lat":47.6234778,"lat_long":"47.6234778,-122.3063220","long":-122.306322,"notes":"Education includes a BA in psychology from Colorado State University in 1970. She also completed The Art of the Cold Call. Nancy is a member of Toastmasters International.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-1","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Ms."},"customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":76.099998,"label":"Order-10859","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2018-01-29T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2018-02-26T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2018-02-02T00:00:00Z","subjectId":"NWD~Order-10859","employee":{"birthDate":"1968-12-08","comment":null,"employeeAddress":"507 - 20th Ave. E.\\nApt. 2A","employeeCity":"Seattle","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98122","employeeSalary":null,"employer":null,"extension":"5467","favorite":null,"firstName":"Nancy","hireDate":"2012-05-01","homePhone":"(206) 555-9857","label":"Employee-1","lastName":"Davolio","lat":47.6234778,"lat_long":"47.6234778,-122.3063220","long":-122.306322,"notes":"Education includes a BA in psychology from Colorado State University in 1970. She also completed The Art of the Cold Call. Nancy is a member of Toastmasters International.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-1","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Ms."},"customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":242.95,"label":"Order-11012","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2018-04-09T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2018-04-23T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2018-04-17T00:00:00Z","subjectId":"NWD~Order-11012","employee":{"birthDate":"1968-12-08","comment":null,"employeeAddress":"507 - 20th Ave. E.\\nApt. 2A","employeeCity":"Seattle","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98122","employeeSalary":null,"employer":null,"extension":"5467","favorite":null,"firstName":"Nancy","hireDate":"2012-05-01","homePhone":"(206) 555-9857","label":"Employee-1","lastName":"Davolio","lat":47.6234778,"lat_long":"47.6234778,-122.3063220","long":-122.306322,"notes":"Education includes a BA in psychology from Colorado State University in 1970. She also completed The Art of the Cold Call. Nancy is a member of Toastmasters International.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-1","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Ms."},"customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$filter=(customer/customerCity eq 'Stuttgart') and (hasOrderDetail/any(od:od/productId eq 'NWD~Product-21')) &amp;$expand=hasOrderDetail&amp;$top=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order(hasOrderDetail())","value":[{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-7","employeeNotation":null,"freight":105.65,"label":"Order-10513","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2017-04-22T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-06-03T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-04-28T00:00:00Z","subjectId":"NWD~Order-10513","hasOrderDetail":[{"comment":null,"discount":0.2,"label":"OrderDetail-10513-21","orderDetailUnitPrice":10.0,"orderId":"NWD~Order-10513","orderNotation":null,"productId":"NWD~Product-21","productNotation":null,"quantity":40,"subjectId":"NWD~OrderDetail-10513-21"},{"comment":null,"discount":0.2,"label":"OrderDetail-10513-32","orderDetailUnitPrice":32.0,"orderId":"NWD~Order-10513","orderNotation":null,"productId":"NWD~Product-32","productNotation":null,"quantity":50,"subjectId":"NWD~OrderDetail-10513-32"},{"comment":null,"discount":0.2,"label":"OrderDetail-10513-61","orderDetailUnitPrice":28.5,"orderId":"NWD~Order-10513","orderNotation":null,"productId":"NWD~Product-61","productNotation":null,"quantity":15,"subjectId":"NWD~OrderDetail-10513-61"}]}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$filter=(hasOrderDetail/quantity eq 15)&amp;$top=5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"error":{"code":null,"message":"The URI is malformed."}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$filter=(hasOrderDetail/any(od:od/quantity eq 15))&amp;$top=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order","value":[{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-7","employeeNotation":null,"freight":105.65,"label":"Order-10513","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2017-04-22T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-06-03T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-04-28T00:00:00Z","subjectId":"NWD~Order-10513"},{"comment":null,"customerId":"NWD~Customer-WARTH","customerNotation":null,"employeeId":"NWD~Employee-2","employeeNotation":null,"freight":149.49001,"label":"Order-10553","lat":65.010279,"lat_long":"65.0102790,25.4650189","long":25.4650189,"orderDate":"2017-05-30T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-06-27T00:00:00Z","shipAddress":"Torikatu 38","shipCity":"Oulu","shipCountry":"Finland","shipName":"Wartian Herkku","shipPostalCode":"90110","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2017-06-03T00:00:00Z","subjectId":"NWD~Order-10553"},{"comment":null,"customerId":"NWD~Customer-FURIB","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":1.27,"label":"Order-10664","lat":38.7639293,"lat_long":"38.7639293,-9.1995368","long":-9.1995368,"orderDate":"2017-09-10T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-10-08T00:00:00Z","shipAddress":"Jardim das rosas n. 32","shipCity":"Lisboa","shipCountry":"Portugal","shipName":"Furia Bacalhau e Frutos do Mar","shipPostalCode":"1675","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2017-09-19T00:00:00Z","subjectId":"NWD~Order-10664"},{"comment":null,"customerId":"NWD~Customer-OCEAN","customerNotation":null,"employeeId":"NWD~Employee-8","employeeNotation":null,"freight":217.86,"label":"Order-10986","lat":-34.6030312,"lat_long":"-34.6030312,-58.3707695","long":-58.3707695,"orderDate":"2008-03-30T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2008-04-27T00:00:00Z","shipAddress":"Ing. Gustavo Moncada 8585 Piso 20-A","shipCity":"Buenos Aires","shipCountry":"Argentina","shipName":"Océano Atlántico Ltda.","shipPostalCode":"1010","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2008-04-21T00:00:00Z","subjectId":"NWD~Order-10986"},{"comment":null,"customerId":"NWD~Customer-QUICK","customerNotation":null,"employeeId":"NWD~Employee-3","employeeNotation":null,"freight":297.17999,"label":"Order-11021","lat":51.1799698,"lat_long":"51.1799698,14.4370284","long":14.4370284,"orderDate":"2008-04-14T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2008-05-12T00:00:00Z","shipAddress":"Taucherstraße 10","shipCity":"Cunewalde","shipCountry":"Germany","shipName":"QUICK-Stop","shipPostalCode":"01307","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2008-04-21T00:00:00Z","subjectId":"NWD~Order-11021"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$filter=(customer/customerCity eq 'Stuttgart')  &amp;$top=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order","value":[{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-2","employeeNotation":null,"freight":40.259998,"label":"Order-10312","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2016-09-23T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-10-21T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2016-10-03T00:00:00Z","subjectId":"NWD~Order-10312"},{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-6","employeeNotation":null,"freight":36.709999,"label":"Order-10356","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2016-11-18T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-12-16T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2016-11-27T00:00:00Z","subjectId":"NWD~Order-10356"},{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-7","employeeNotation":null,"freight":105.65,"label":"Order-10513","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2017-04-22T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-06-03T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-04-28T00:00:00Z","subjectId":"NWD~Order-10513"},{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-8","employeeNotation":null,"freight":41.380001,"label":"Order-10632","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2017-08-14T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-11T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-08-19T00:00:00Z","subjectId":"NWD~Order-10632"},{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-4","employeeNotation":null,"freight":23.549999,"label":"Order-10640","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2017-08-21T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-18T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-08-28T00:00:00Z","subjectId":"NWD~Order-10640"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$filter= (shipCountry eq 'France')&amp;$top=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order","value":[{"comment":null,"customerId":"NWD~Customer-BONAP","customerNotation":null,"employeeId":"NWD~Employee-2","employeeNotation":null,"freight":113.15,"label":"Order-10663","lat":43.2611295,"lat_long":"43.2611295,5.3886613","long":5.3886613,"orderDate":"2017-09-10T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-24T00:00:00Z","shipAddress":"12, rue des Bouchers","shipCity":"Marseille","shipCountry":"France","shipName":"Bon app'","shipPostalCode":"13008","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2017-10-03T00:00:00Z","subjectId":"NWD~Order-10663"},{"comment":null,"customerId":"NWD~Customer-BONAP","customerNotation":null,"employeeId":"NWD~Employee-4","employeeNotation":null,"freight":16.709999,"label":"Order-10755","lat":43.2611295,"lat_long":"43.2611295,5.3886613","long":5.3886613,"orderDate":"2017-11-26T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-12-24T00:00:00Z","shipAddress":"12, rue des Bouchers","shipCity":"Marseille","shipCountry":"France","shipName":"Bon app'","shipPostalCode":"13008","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2017-11-28T00:00:00Z","subjectId":"NWD~Order-10755"},{"comment":null,"customerId":"NWD~Customer-FOLIG","customerNotation":null,"employeeId":"NWD~Employee-3","employeeNotation":null,"freight":37.349998,"label":"Order-10763","lat":50.5690579,"lat_long":"50.5690579,3.2223336","long":3.2223336,"orderDate":"2017-12-03T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-12-31T00:00:00Z","shipAddress":"184, chaussée de Tournai","shipCity":"Lille","shipCountry":"France","shipName":"Folies gourmandes","shipPostalCode":"59000","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2017-12-08T00:00:00Z","subjectId":"NWD~Order-10763"},{"comment":null,"customerId":"NWD~Customer-LAMAI","customerNotation":null,"employeeId":"NWD~Employee-7","employeeNotation":null,"freight":68.260002,"label":"Order-10923","lat":43.5996235,"lat_long":"43.5996235,1.4454683","long":1.4454683,"orderDate":"2008-03-03T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2008-04-14T00:00:00Z","shipAddress":"1 rue Alsace-Lorraine","shipCity":"Toulouse","shipCountry":"France","shipName":"La maison d'Asie","shipPostalCode":"31000","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2008-03-13T00:00:00Z","subjectId":"NWD~Order-10923"},{"comment":null,"customerId":"NWD~Customer-SPECD","customerNotation":null,"employeeId":"NWD~Employee-3","employeeNotation":null,"freight":87.379997,"label":"Order-10964","lat":48.8711159,"lat_long":"48.8711159,2.2919884","long":2.2919884,"orderDate":"2008-03-20T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2008-04-17T00:00:00Z","shipAddress":"25, rue Lauriston","shipCity":"Paris","shipCountry":"France","shipName":"Spécialités du monde","shipPostalCode":"75016","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2008-03-24T00:00:00Z","subjectId":"NWD~Order-10964"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$filter=(customer/customerCity eq 'Stuttgart') and (shipCountry eq 'Germany') &amp;$top=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$filter=(customer/customerCity eq 'Stuttgart') and (shipCountry eq 'Germany') and (employee/firstName eq 'Laura') &amp;$top=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order","value":[{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-8","employeeNotation":null,"freight":45.080002,"label":"Order-10301","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2016-09-09T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-10-07T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2016-09-17T00:00:00Z","subjectId":"NWD~Order-10301"},{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-8","employeeNotation":null,"freight":41.380001,"label":"Order-10632","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2017-08-14T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-11T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-08-19T00:00:00Z","subjectId":"NWD~Order-10632"},{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-8","employeeNotation":null,"freight":20.6,"label":"Order-10651","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2017-09-01T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-29T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2017-09-11T00:00:00Z","subjectId":"NWD~Order-10651"},{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-8","employeeNotation":null,"freight":71.639999,"label":"Order-11046","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2018-04-23T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2018-05-21T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2018-04-24T00:00:00Z","subjectId":"NWD~Order-11046"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$filter=(customer/customerCity eq 'Stuttgart') and (employee/reportsTo/firstName eq 'Andrew') &amp;$top=5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order","value":[{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-8","employeeNotation":null,"freight":45.080002,"label":"Order-10301","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2016-09-09T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-10-07T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2016-09-17T00:00:00Z","subjectId":"NWD~Order-10301"},{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-6","employeeNotation":null,"freight":36.709999,"label":"Order-10356","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2016-11-18T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-12-16T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2016-11-27T00:00:00Z","subjectId":"NWD~Order-10356"},{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-7","employeeNotation":null,"freight":105.65,"label":"Order-10513","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2017-04-22T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-06-03T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-04-28T00:00:00Z","subjectId":"NWD~Order-10513"},{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-8","employeeNotation":null,"freight":41.380001,"label":"Order-10632","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2017-08-14T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-11T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-08-19T00:00:00Z","subjectId":"NWD~Order-10632"},{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-4","employeeNotation":null,"freight":23.549999,"label":"Order-10640","lat":48.7794494,"lat_long":"48.7794494,9.1852878","long":9.1852878,"orderDate":"2017-08-21T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-18T00:00:00Z","shipAddress":"Adenauerallee 900","shipCity":"Stuttgart","shipCountry":"Germany","shipName":"Die Wandernde Kuh","shipPostalCode":"70563","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-08-28T00:00:00Z","subjectId":"NWD~Order-10640"}]}</t>
   </si>
 </sst>
 </file>
@@ -2171,7 +2587,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2192,6 +2608,37 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2249,16 +2696,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2279,13 +2730,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K234"/>
+  <dimension ref="A1:K242"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A160" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K236" activeCellId="0" sqref="K236"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J161" activeCellId="0" sqref="J161"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.86"/>
@@ -2294,7 +2745,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="55.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="121.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="89.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="36.84"/>
@@ -2429,7 +2880,7 @@
       <c r="I5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2478,7 +2929,7 @@
       <c r="I7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2527,7 +2978,7 @@
       <c r="I9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="J9" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3037,11 +3488,11 @@
       <c r="I30" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J30" s="0" t="s">
+      <c r="J30" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>98</v>
       </c>
@@ -3063,7 +3514,7 @@
       <c r="I31" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J31" s="0" t="s">
+      <c r="J31" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3141,7 +3592,7 @@
       <c r="I34" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J34" s="0" t="s">
+      <c r="J34" s="1" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3167,7 +3618,7 @@
       <c r="I35" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J35" s="0" t="s">
+      <c r="J35" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -3193,13 +3644,16 @@
       <c r="I36" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="J36" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>98</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>46</v>
@@ -3211,7 +3665,7 @@
         <v>100</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H37" s="0" t="s">
         <v>110</v>
@@ -3225,7 +3679,7 @@
         <v>98</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>46</v>
@@ -3237,7 +3691,7 @@
         <v>100</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H38" s="0" t="s">
         <v>110</v>
@@ -3248,10 +3702,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>12</v>
@@ -3260,24 +3714,24 @@
         <v>100</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I39" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>122</v>
+      <c r="J39" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>46</v>
@@ -3289,24 +3743,27 @@
         <v>100</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I40" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>12</v>
@@ -3315,21 +3772,18 @@
         <v>100</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I41" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="J41" s="0" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>129</v>
@@ -3358,7 +3812,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>132</v>
@@ -3378,7 +3832,7 @@
       <c r="I43" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J43" s="0" t="s">
+      <c r="J43" s="1" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3430,7 +3884,7 @@
       <c r="I45" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J45" s="2" t="s">
+      <c r="J45" s="1" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3456,7 +3910,7 @@
       <c r="I46" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J46" s="2" t="s">
+      <c r="J46" s="1" t="s">
         <v>144</v>
       </c>
     </row>
@@ -3465,7 +3919,7 @@
         <v>145</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>146</v>
@@ -3477,7 +3931,7 @@
         <v>13</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H47" s="0" t="s">
         <v>147</v>
@@ -3494,7 +3948,7 @@
         <v>145</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>146</v>
@@ -3506,7 +3960,7 @@
         <v>13</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H48" s="0" t="s">
         <v>149</v>
@@ -4277,7 +4731,7 @@
       <c r="I77" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J77" s="0" t="s">
+      <c r="J77" s="1" t="s">
         <v>239</v>
       </c>
     </row>
@@ -5670,7 +6124,7 @@
       <c r="I127" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J127" s="0" t="s">
+      <c r="J127" s="1" t="s">
         <v>393</v>
       </c>
     </row>
@@ -5728,7 +6182,7 @@
       <c r="I129" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J129" s="0" t="s">
+      <c r="J129" s="1" t="s">
         <v>399</v>
       </c>
     </row>
@@ -5757,7 +6211,7 @@
       <c r="I130" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="J130" s="0" t="s">
+      <c r="J130" s="1" t="s">
         <v>402</v>
       </c>
     </row>
@@ -6620,19 +7074,19 @@
       <c r="G161" s="0" t="s">
         <v>494</v>
       </c>
-      <c r="J161" s="0" t="n">
-        <v>42</v>
+      <c r="J161" s="1" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B162" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E162" s="0" t="s">
         <v>12</v>
@@ -6652,13 +7106,13 @@
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B163" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E163" s="0" t="s">
         <v>12</v>
@@ -6667,24 +7121,24 @@
         <v>13</v>
       </c>
       <c r="G163" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="I163" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J163" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B164" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C164" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="E164" s="0" t="s">
         <v>12</v>
@@ -6693,21 +7147,21 @@
         <v>13</v>
       </c>
       <c r="G164" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="J164" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B165" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C165" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="E165" s="0" t="s">
         <v>12</v>
@@ -6716,24 +7170,24 @@
         <v>13</v>
       </c>
       <c r="G165" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="I165" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J165" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B166" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C166" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="E166" s="0" t="s">
         <v>12</v>
@@ -6742,21 +7196,21 @@
         <v>13</v>
       </c>
       <c r="G166" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="J166" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B167" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="E167" s="0" t="s">
         <v>12</v>
@@ -6765,24 +7219,24 @@
         <v>13</v>
       </c>
       <c r="G167" s="0" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="I167" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J167" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B168" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E168" s="0" t="s">
         <v>12</v>
@@ -6791,21 +7245,21 @@
         <v>13</v>
       </c>
       <c r="G168" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="J168" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B169" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E169" s="0" t="s">
         <v>12</v>
@@ -6814,24 +7268,24 @@
         <v>13</v>
       </c>
       <c r="G169" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="I169" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J169" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B170" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C170" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E170" s="0" t="s">
         <v>12</v>
@@ -6840,21 +7294,21 @@
         <v>13</v>
       </c>
       <c r="G170" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="J170" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B171" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="E171" s="0" t="s">
         <v>12</v>
@@ -6863,24 +7317,24 @@
         <v>13</v>
       </c>
       <c r="G171" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="I171" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J171" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B172" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C172" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D172" s="0" t="s">
         <v>146</v>
@@ -6892,24 +7346,24 @@
         <v>13</v>
       </c>
       <c r="G172" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="I172" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J172" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B173" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="E173" s="0" t="s">
         <v>12</v>
@@ -6918,24 +7372,24 @@
         <v>13</v>
       </c>
       <c r="G173" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="I173" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J173" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B174" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E174" s="0" t="s">
         <v>12</v>
@@ -6944,24 +7398,24 @@
         <v>13</v>
       </c>
       <c r="G174" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="I174" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J174" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B175" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="E175" s="0" t="s">
         <v>12</v>
@@ -6970,27 +7424,27 @@
         <v>13</v>
       </c>
       <c r="G175" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="H175" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="I175" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J175" s="0" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B176" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C176" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="E176" s="0" t="s">
         <v>12</v>
@@ -6999,24 +7453,24 @@
         <v>13</v>
       </c>
       <c r="G176" s="0" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="I176" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J176" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B177" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C177" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E177" s="0" t="s">
         <v>12</v>
@@ -7025,27 +7479,27 @@
         <v>13</v>
       </c>
       <c r="G177" s="0" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="H177" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="I177" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J177" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B178" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C178" s="0" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E178" s="0" t="s">
         <v>12</v>
@@ -7065,13 +7519,13 @@
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B179" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C179" s="0" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E179" s="0" t="s">
         <v>12</v>
@@ -7080,24 +7534,24 @@
         <v>13</v>
       </c>
       <c r="G179" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="I179" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J179" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B180" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C180" s="0" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E180" s="0" t="s">
         <v>12</v>
@@ -7106,24 +7560,24 @@
         <v>13</v>
       </c>
       <c r="G180" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="I180" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J180" s="0" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B181" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C181" s="0" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E181" s="0" t="s">
         <v>12</v>
@@ -7132,24 +7586,24 @@
         <v>13</v>
       </c>
       <c r="G181" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="I181" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J181" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B182" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C182" s="0" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E182" s="0" t="s">
         <v>12</v>
@@ -7158,24 +7612,24 @@
         <v>13</v>
       </c>
       <c r="G182" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="I182" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J182" s="0" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B183" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C183" s="0" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E183" s="0" t="s">
         <v>12</v>
@@ -7184,7 +7638,7 @@
         <v>13</v>
       </c>
       <c r="G183" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="H183" s="0" t="s">
         <v>15</v>
@@ -7193,18 +7647,18 @@
         <v>16</v>
       </c>
       <c r="J183" s="0" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B184" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C184" s="0" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="E184" s="0" t="s">
         <v>12</v>
@@ -7213,7 +7667,7 @@
         <v>13</v>
       </c>
       <c r="G184" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="H184" s="0" t="s">
         <v>304</v>
@@ -7222,18 +7676,18 @@
         <v>16</v>
       </c>
       <c r="J184" s="0" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B185" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C185" s="0" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="E185" s="0" t="s">
         <v>12</v>
@@ -7242,27 +7696,27 @@
         <v>13</v>
       </c>
       <c r="G185" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="H185" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="I185" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J185" s="0" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B186" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C186" s="0" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="E186" s="0" t="s">
         <v>12</v>
@@ -7271,27 +7725,27 @@
         <v>13</v>
       </c>
       <c r="G186" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="H186" s="0" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="I186" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J186" s="0" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B187" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C187" s="0" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E187" s="0" t="s">
         <v>12</v>
@@ -7300,24 +7754,24 @@
         <v>13</v>
       </c>
       <c r="G187" s="0" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="I187" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J187" s="0" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B188" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C188" s="0" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="E188" s="0" t="s">
         <v>12</v>
@@ -7326,24 +7780,24 @@
         <v>13</v>
       </c>
       <c r="G188" s="0" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="I188" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J188" s="0" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B189" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C189" s="0" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="E189" s="0" t="s">
         <v>12</v>
@@ -7352,24 +7806,24 @@
         <v>13</v>
       </c>
       <c r="G189" s="0" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="I189" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J189" s="0" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B190" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C190" s="0" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="E190" s="0" t="s">
         <v>12</v>
@@ -7378,27 +7832,27 @@
         <v>13</v>
       </c>
       <c r="G190" s="0" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="H190" s="0" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="I190" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J190" s="0" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B191" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C191" s="0" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="E191" s="0" t="s">
         <v>12</v>
@@ -7418,13 +7872,13 @@
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C192" s="0" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="E192" s="0" t="s">
         <v>12</v>
@@ -7433,7 +7887,7 @@
         <v>13</v>
       </c>
       <c r="G192" s="0" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="H192" s="0" t="s">
         <v>203</v>
@@ -7442,18 +7896,18 @@
         <v>16</v>
       </c>
       <c r="J192" s="0" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B193" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C193" s="0" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="E193" s="0" t="s">
         <v>12</v>
@@ -7462,21 +7916,21 @@
         <v>13</v>
       </c>
       <c r="G193" s="0" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="J193" s="0" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B194" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C194" s="0" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="E194" s="0" t="s">
         <v>12</v>
@@ -7485,27 +7939,27 @@
         <v>13</v>
       </c>
       <c r="G194" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="I194" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J194" s="0" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="K194" s="0" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B195" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C195" s="0" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E195" s="0" t="s">
         <v>12</v>
@@ -7514,21 +7968,21 @@
         <v>13</v>
       </c>
       <c r="G195" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="J195" s="0" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B196" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C196" s="0" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="E196" s="0" t="s">
         <v>12</v>
@@ -7537,27 +7991,27 @@
         <v>13</v>
       </c>
       <c r="G196" s="0" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="I196" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J196" s="0" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="K196" s="0" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C197" s="0" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D197" s="0" t="s">
         <v>46</v>
@@ -7569,30 +8023,30 @@
         <v>13</v>
       </c>
       <c r="G197" s="0" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="I197" s="0" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C198" s="0" t="s">
+        <v>603</v>
+      </c>
+      <c r="E198" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F198" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I198" s="0" t="s">
         <v>602</v>
-      </c>
-      <c r="E198" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F198" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I198" s="0" t="s">
-        <v>601</v>
       </c>
       <c r="J198" s="0" t="s">
         <v>284</v>
@@ -7600,10 +8054,10 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="C199" s="0" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="D199" s="0" t="s">
         <v>46</v>
@@ -7620,10 +8074,10 @@
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C200" s="0" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="D200" s="0" t="s">
         <v>46</v>
@@ -7640,10 +8094,10 @@
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C201" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="D201" s="0" t="s">
         <v>146</v>
@@ -7655,21 +8109,21 @@
         <v>13</v>
       </c>
       <c r="G201" s="0" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="I201" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J201" s="0" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C202" s="0" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D202" s="0" t="s">
         <v>146</v>
@@ -7681,24 +8135,24 @@
         <v>13</v>
       </c>
       <c r="G202" s="0" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="H202" s="0" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="I202" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J202" s="0" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C203" s="0" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D203" s="0" t="s">
         <v>46</v>
@@ -7715,10 +8169,10 @@
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="C204" s="0" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D204" s="0" t="s">
         <v>46</v>
@@ -7735,10 +8189,10 @@
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C205" s="0" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="D205" s="0" t="s">
         <v>46</v>
@@ -7755,13 +8209,13 @@
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B206" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C206" s="0" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="E206" s="0" t="s">
         <v>12</v>
@@ -7770,7 +8224,7 @@
         <v>13</v>
       </c>
       <c r="G206" s="0" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="J206" s="0" t="n">
         <v>91</v>
@@ -7778,13 +8232,13 @@
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B207" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C207" s="0" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="E207" s="0" t="s">
         <v>12</v>
@@ -7793,7 +8247,7 @@
         <v>13</v>
       </c>
       <c r="G207" s="0" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="J207" s="0" t="n">
         <v>10</v>
@@ -7801,13 +8255,13 @@
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B208" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C208" s="0" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="E208" s="0" t="s">
         <v>12</v>
@@ -7816,7 +8270,7 @@
         <v>13</v>
       </c>
       <c r="G208" s="0" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="J208" s="0" t="n">
         <v>3511</v>
@@ -7824,13 +8278,13 @@
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B209" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C209" s="0" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="E209" s="0" t="s">
         <v>12</v>
@@ -7839,7 +8293,7 @@
         <v>13</v>
       </c>
       <c r="G209" s="0" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="J209" s="0" t="n">
         <v>3348</v>
@@ -7847,13 +8301,13 @@
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B210" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C210" s="0" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="E210" s="0" t="s">
         <v>12</v>
@@ -7862,7 +8316,7 @@
         <v>13</v>
       </c>
       <c r="G210" s="0" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="J210" s="0" t="n">
         <v>2155</v>
@@ -7870,13 +8324,13 @@
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B211" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C211" s="0" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="E211" s="0" t="s">
         <v>12</v>
@@ -7885,53 +8339,53 @@
         <v>13</v>
       </c>
       <c r="G211" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="I211" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J211" s="0" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="K211" s="0" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B212" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C212" s="0" t="s">
+        <v>636</v>
+      </c>
+      <c r="E212" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F212" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G212" s="0" t="s">
+        <v>637</v>
+      </c>
+      <c r="I212" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J212" s="0" t="s">
         <v>635</v>
       </c>
-      <c r="E212" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F212" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G212" s="0" t="s">
-        <v>636</v>
-      </c>
-      <c r="I212" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J212" s="0" t="s">
-        <v>634</v>
-      </c>
       <c r="K212" s="0" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="D213" s="0" t="s">
         <v>46</v>
@@ -7948,10 +8402,10 @@
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="D214" s="0" t="s">
         <v>46</v>
@@ -7968,10 +8422,10 @@
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C215" s="0" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="D215" s="0" t="s">
         <v>46</v>
@@ -7988,13 +8442,13 @@
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B216" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C216" s="0" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="E216" s="0" t="s">
         <v>12</v>
@@ -8003,30 +8457,30 @@
         <v>13</v>
       </c>
       <c r="G216" s="0" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="H216" s="0" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="I216" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J216" s="0" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="K216" s="0" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B217" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C217" s="0" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D217" s="0" t="s">
         <v>46</v>
@@ -8038,30 +8492,30 @@
         <v>13</v>
       </c>
       <c r="G217" s="0" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="H217" s="0" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="I217" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J217" s="0" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="K217" s="0" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B218" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="E218" s="0" t="s">
         <v>12</v>
@@ -8070,30 +8524,30 @@
         <v>13</v>
       </c>
       <c r="G218" s="0" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="H218" s="0" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="I218" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J218" s="0" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="K218" s="0" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B219" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C219" s="0" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="D219" s="0" t="s">
         <v>46</v>
@@ -8108,24 +8562,24 @@
         <v>311</v>
       </c>
       <c r="H219" s="0" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="I219" s="0" t="s">
         <v>16</v>
       </c>
       <c r="K219" s="0" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B220" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C220" s="0" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="D220" s="0" t="s">
         <v>46</v>
@@ -8140,24 +8594,24 @@
         <v>311</v>
       </c>
       <c r="H220" s="0" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="I220" s="0" t="s">
         <v>16</v>
       </c>
       <c r="K220" s="0" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B221" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C221" s="0" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D221" s="0" t="s">
         <v>46</v>
@@ -8172,24 +8626,24 @@
         <v>413</v>
       </c>
       <c r="H221" s="0" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="I221" s="0" t="s">
         <v>16</v>
       </c>
       <c r="K221" s="0" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B222" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C222" s="0" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D222" s="0" t="s">
         <v>46</v>
@@ -8204,24 +8658,24 @@
         <v>413</v>
       </c>
       <c r="H222" s="0" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="I222" s="0" t="s">
         <v>16</v>
       </c>
       <c r="K222" s="0" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B223" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C223" s="0" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D223" s="0" t="s">
         <v>46</v>
@@ -8236,24 +8690,24 @@
         <v>388</v>
       </c>
       <c r="H223" s="0" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="I223" s="0" t="s">
         <v>16</v>
       </c>
       <c r="K223" s="0" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B224" s="0" t="s">
         <v>286</v>
       </c>
       <c r="C224" s="0" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D224" s="0" t="s">
         <v>46</v>
@@ -8268,24 +8722,24 @@
         <v>300</v>
       </c>
       <c r="H224" s="0" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="I224" s="0" t="s">
         <v>16</v>
       </c>
       <c r="K224" s="0" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B225" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C225" s="0" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="D225" s="0" t="s">
         <v>46</v>
@@ -8300,24 +8754,24 @@
         <v>311</v>
       </c>
       <c r="H225" s="0" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="I225" s="0" t="s">
         <v>16</v>
       </c>
       <c r="K225" s="0" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B226" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C226" s="0" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D226" s="0" t="s">
         <v>46</v>
@@ -8332,24 +8786,24 @@
         <v>370</v>
       </c>
       <c r="H226" s="0" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="I226" s="0" t="s">
         <v>16</v>
       </c>
       <c r="K226" s="0" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B227" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C227" s="0" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="E227" s="0" t="s">
         <v>12</v>
@@ -8361,24 +8815,24 @@
         <v>370</v>
       </c>
       <c r="H227" s="0" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="I227" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J227" s="0" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B228" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C228" s="0" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D228" s="0" t="s">
         <v>46</v>
@@ -8393,24 +8847,24 @@
         <v>311</v>
       </c>
       <c r="H228" s="0" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="I228" s="0" t="s">
         <v>16</v>
       </c>
       <c r="K228" s="0" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B229" s="0" t="s">
         <v>339</v>
       </c>
       <c r="C229" s="0" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="D229" s="0" t="s">
         <v>46</v>
@@ -8425,21 +8879,21 @@
         <v>311</v>
       </c>
       <c r="H229" s="0" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="I229" s="0" t="s">
         <v>16</v>
       </c>
       <c r="K229" s="0" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B230" s="0" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E230" s="0" t="s">
         <v>12</v>
@@ -8451,18 +8905,21 @@
         <v>311</v>
       </c>
       <c r="H230" s="0" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="I230" s="0" t="s">
         <v>16</v>
+      </c>
+      <c r="J230" s="2" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B231" s="0" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E231" s="0" t="s">
         <v>12</v>
@@ -8474,18 +8931,21 @@
         <v>311</v>
       </c>
       <c r="H231" s="0" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="I231" s="0" t="s">
         <v>16</v>
+      </c>
+      <c r="J231" s="2" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B232" s="0" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E232" s="0" t="s">
         <v>12</v>
@@ -8497,18 +8957,21 @@
         <v>311</v>
       </c>
       <c r="H232" s="0" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="I232" s="0" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J232" s="2" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B233" s="0" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E233" s="0" t="s">
         <v>12</v>
@@ -8520,18 +8983,21 @@
         <v>311</v>
       </c>
       <c r="H233" s="0" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
       <c r="I233" s="0" t="s">
         <v>16</v>
+      </c>
+      <c r="J233" s="1" t="s">
+        <v>699</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B234" s="0" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E234" s="0" t="s">
         <v>12</v>
@@ -8543,13 +9009,227 @@
         <v>311</v>
       </c>
       <c r="H234" s="0" t="s">
-        <v>695</v>
+        <v>700</v>
       </c>
       <c r="I234" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="J234" s="2" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="B235" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="E235" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F235" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G235" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="H235" s="0" t="s">
+        <v>702</v>
+      </c>
+      <c r="I235" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J235" s="2" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="B236" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="E236" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F236" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G236" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="H236" s="0" t="s">
+        <v>704</v>
+      </c>
+      <c r="I236" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J236" s="2" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="B237" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="E237" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F237" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G237" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="H237" s="0" t="s">
+        <v>706</v>
+      </c>
+      <c r="I237" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J237" s="2" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="B238" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="E238" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F238" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G238" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="H238" s="0" t="s">
+        <v>708</v>
+      </c>
+      <c r="I238" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J238" s="2" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="B239" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="E239" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F239" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G239" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="H239" s="0" t="s">
+        <v>710</v>
+      </c>
+      <c r="I239" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J239" s="2" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="B240" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="E240" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F240" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G240" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="H240" s="0" t="s">
+        <v>712</v>
+      </c>
+      <c r="I240" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J240" s="2" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="B241" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="E241" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F241" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G241" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="H241" s="0" t="s">
+        <v>713</v>
+      </c>
+      <c r="I241" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J241" s="2" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="B242" s="0" t="s">
+        <v>691</v>
+      </c>
+      <c r="E242" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F242" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G242" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="H242" s="0" t="s">
+        <v>715</v>
+      </c>
+      <c r="I242" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J242" s="2" t="s">
+        <v>716</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J30" r:id="rId1" location="olgap_ShortestPath" display="http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_ShortestPath"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Updated WAR. Also fixed missing OLGAP functions
</commit_message>
<xml_diff>
--- a/odata2sparql.v4/src/test/resources/GetTests.xlsx
+++ b/odata2sparql.v4/src/test/resources/GetTests.xlsx
@@ -102,7 +102,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource(rdf_facts(rdf_property(),rdf_terms()))/$entity","comment":null,"label":"OrderDetail-10250-51","subjectId":"NWD~OrderDetail-10250-51","rdf_facts":[{"comment":null,"label":null,"propertyId":"rdfs~label","subjectId":"NWD~OrderDetail-10250-51-4f75ce12336ab89a4edebd807cd62265","rdf_property":{"comment":"","label":"label","subjectId":"rdfs~label"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":</t>
     </r>
@@ -112,7 +111,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"OrderDetail-10250-51","rdf_object":"OrderDetail-10250-51","resourceId":null,"subjectId":"NWD~OrderDetail-10250-51-4f75ce12336ab89a4edebd807cd62265-311f0cc52cba0a21070961879f9173c8"}]},{"comment":null,"label":null,"propertyId":"northwind~discount","subjectId":"NWD~OrderDetail-10250-51-560ff6ef546ba93e36c161c0d4dce072","rdf_property":{"comment":"","label":"discount","subjectId":"northwind~discount"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":"0.15","rdf_object":"0.15","resourceId":null,"subjectId":"NWD~OrderDetail-10250-51-560ff6ef546ba93e36c161c0d4dce072-9ffc7a03c1959674fa8c0a7369460097"}]},{"comment":null,"label":null,"propertyId":"northwind~order","subjectId":"NWD~OrderDetail-10250-51-7849cdb0ec5319c5c3c71d9bff0672b0","rdf_property":{"comment":"","label":"is part of order","subjectId":"northwind~order"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/Order-10250","resourceId":"NWD~Order-10250","subjectId":"NWD~OrderDetail-10250-51-7849cdb0ec5319c5c3c71d9bff0672b0-b6b2d84f8259c3db3fb89c10ce920509"}]},{"comment":null,"label":null,"propertyId":"northwind~product","subjectId":"NWD~OrderDetail-10250-51-9f79a810fc71f8d74ecbb8bb013bed9c","rdf_property":{"comment":"","label":"includes product","subjectId":"northwind~product"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/Product-51","resourceId":"NWD~Product-51","subjectId":"NWD~OrderDetail-10250-51-9f79a810fc71f8d74ecbb8bb013bed9c-46a5bfba2bbe33d1a6e41ac2f23216b1"}]},{"comment":null,"label":null,"propertyId":"northwind~quantity","subjectId":"NWD~OrderDetail-10250-51-9fc1ed06938066abace0a241064b728b","rdf_property":{"comment":"","label":"quantity","subjectId":"northwind~quantity"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":"35","rdf_object":"35","resourceId":null,"subjectId":"NWD~OrderDetail-10250-51-9fc1ed06938066abace0a241064b728b-1c383cd30b7c298ab50293adfecb7b18"}]},{"comment":null,"label":null,"propertyId":"rdf~type","subjectId":"NWD~OrderDetail-10250-51-c74e2b735dd8dc85ad0ee3510c33925f","rdf_property":{"comment":"","label":"type","subjectId":"rdf~type"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/model/OrderDetail","resourceId":"northwind~OrderDetail","subjectId":"NWD~OrderDetail-10250-51-c74e2b735dd8dc85ad0ee3510c33925f-1c1c9eee9ed5045311df73136e39de22"}]},{"comment":null,"label":null,"propertyId":"northwind~orderDetailUnitPrice","subjectId":"NWD~OrderDetail-10250-51-f42cdd44e43333f6f7b46b4988d2a2f6","rdf_property":{"comment":"","label":"unit price","subjectId":"northwind~orderDetailUnitPrice"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":"42.4"</t>
     </r>
@@ -121,7 +119,6 @@
         <sz val="10"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,"rdf_object":"42.4","resourceId":null,"subjectId":"NWD~OrderDetail-10250-51-f42cdd44e43333f6f7b46b4988d2a2f6-8a622231ebe8e6ec3b0e654c589717d3"}]}]}</t>
     </r>
@@ -147,7 +144,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource('NWD~OrderDetail-10250-51')/rdf_facts(rdf_property(),rdf_terms())","value":[{"comment":"","label":"discount","propertyId":"northwind~discount","subjectId":"northwind~discount","rdf_property":{"comment":"","label":"discount","subjectId":"northwind~discount"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":</t>
     </r>
@@ -157,7 +153,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"0.15","rdf_object":"0.15","resourceId":null,"subjectId":"northwind~discount-9ffc7a03c1959674fa8c0a7369460097"}]},{"comment":"","label":"is part of order","propertyId":"northwind~order","subjectId":"northwind~order","rdf_property":{"comment":"","label":"is part of order","subjectId":"northwind~order"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/Order-10250","resourceId":"NWD~Order-10250","subjectId":"northwind~order-b6b2d84f8259c3db3fb89c10ce920509"}]},{"comment":"","label":"unit price","propertyId":"northwind~orderDetailUnitPrice","subjectId":"northwind~orderDetailUnitPrice","rdf_property":{"comment":"","label":"unit price","subjectId":"northwind~orderDetailUnitPrice"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":"42.4","rdf_object":"42.4","resourceId":null,"subjectId":"northwind~orderDetailUnitPrice-8a622231ebe8e6ec3b0e654c589717d3"}]},{"comment":"","label":"includes product","propertyId":"northwind~product","subjectId":"northwind~product","rdf_property":{"comment":"","label":"includes product","subjectId":"northwind~product"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/Product-51","resourceId":"NWD~Product-51","subjectId":"northwind~product-46a5bfba2bbe33d1a6e41ac2f23216b1"}]},{"comment":"","label":"quantity","propertyId":"northwind~quantity","subjectId":"northwind~quantity","rdf_property":{"comment":"","label":"quantity","subjectId":"northwind~quantity"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":"35","rdf_object":"35","resourceId":null,"subjectId":"northwind~quantity-1c383cd30b7c298ab50293adfecb7b18"}]},{"comment":"","label":"label","propertyId":"rdfs~label","subjectId":"rdfs~label","rdf_property":{"comment":"","label":"label","subjectId":"rdfs~label"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":"OrderDetail-10250-51","rdf_object":"OrderDetail-10250-51","resourceId":null,"subjectId":"rdfs~label-311f0cc52cba0a21070961879f9173c8"}]},{"comment":"","label":"type","propertyId":"rdf~type","subjectId":"rdf~type","rdf_property":{"comment":"","label":"type","subjectId":"rdf~type"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/model/OrderDetail","resourceId":"northwind~OrderDetail"</t>
     </r>
@@ -166,7 +161,6 @@
         <sz val="10"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,"subjectId":"rdf~type-1c1c9eee9ed5045311df73136e39de22"}]}]}</t>
     </r>
@@ -189,7 +183,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#rdfs_Resource(rdf_property(),rdf_terms())/$entity","comment":"","label":"includes product","propertyId":"northwind~product","subjectId":"northwind~product","rdf_property":{"comment":"","label":"includes product","subjectId":"northwind~product"},"rdf_terms":[{"comment":null,"label":null,"rdf_literal":null,"rdf_object":"http://northwind.com/Product-51","resourceId":</t>
     </r>
@@ -199,7 +192,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"NWD~Product-51"</t>
     </r>
@@ -208,7 +200,6 @@
         <sz val="10"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,"subjectId":"northwind~product-46a5bfba2bbe33d1a6e41ac2f23216b1"}]}</t>
     </r>
@@ -423,7 +414,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_ShortestPath(direct,object,property,subject,olgap_object(label,subjectId),olgap_property(label,subjectId),olgap_subject(label,subjectId))","value":[{"direct":true,"object":"londontube~Shepherds_Bush_Market","property":"tfl~connectsTo","subject":"londontube~Goldhawk_Road","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Shepherds_Bush_Market')","label":"Shepherds Bush Market","subjectId":"londontube~Shepherds_Bush_Market"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Goldhawk_Road')","label":"Goldhawk Road","subjectId":"londontube~Goldhawk_Road"}},{"direct":true,"object":"londontube~Wood_Lane","property":"tfl~connectsTo","subject":"londontube~Shepherds_Bush_Market","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Wood_Lane')","label":"Wood Lane","subjectId":"londontube~Wood_Lane"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Shepherds_Bush_Market')","label":"Shepherds Bush Market","subjectId":"londontube~Shepherds_Bush_Market"}},{"direct":true,"object":"londontube~Latimer_Road","property":"tfl~connectsTo","subject":"londontube~Wood_Lane","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Latimer_Road')","label":"Latimer Road","subjectId":"londontube~Latimer_Road"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Wood_Lane')","label":"Wood Lane","subjectId":"londontube~Wood_Lane"}},{"direct":true,"object":"londontube~Ladbroke_Grove","property":"tfl~connectsTo","subject":"londontube~Latimer_Road","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Ladbroke_Grove')","label":"Ladbroke Grove","subjectId":"londontube~Ladbroke_Grove"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Latimer_Road')","label":"Latimer Road","subjectId":"londontube~Latimer_Road"}},{"direct":true,"object":"londontube~Westbourne_Park","property":"tfl~connectsTo","subject":"londontube~Ladbroke_Grove","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Westbourne_Park')","label":"Westbourne Park","subjectId":"londontube~Westbourne_Park"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Ladbroke_Grove')","label":"Ladbroke Grove","subjectId":"londontube~Ladbroke_Grove"}},{"direct":true,"object":"londontube~Royal_Oak","property":"tfl~connectsTo","subject":"londontube~Westbourne_Park","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Royal_Oak')","label":"Royal Oak","subjectId":"londontube~Royal_Oak"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Westbourne_Park')","label":"Westbourne Park","subjectId":"londontube~Westbourne_Park"}},{"direct":true,"object":"londontube~Paddington","property":"tfl~connectsTo","subject":"londontube~Royal_Oak","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Paddington')","label":"Paddington","subjectId":"londontube~Paddington"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Royal_Oak')","label":"Royal Oak","subjectId":"londontube~Royal_Oak"}},{"direct":true,"object":"londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29","property":"tfl~connectsTo","subject":"londontube~Paddington","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29')","label":"Edgware Road (Circle/District/Hammersmith and City)","subjectId":"londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Paddington')","label":"Paddington","subjectId":"londontube~Paddington"}},{"direct":true,"object":"londontube~Baker_Street","property":"tfl~connectsTo","subject":"londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Baker_Street')","label":"Baker Street","subjectId":"londontube~Baker_Street"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29')","label":"Edgware Road (Circle/District/Hammersmith and City)","subjectId":"londontube~Edgware_Road_%28Circle%2FDistrict%2FHammersmith_and_City%29"}},{"direct":</t>
     </r>
@@ -433,7 +423,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">false,"object":"londontube~Bond_Street","property":"tfl~connectsFrom","subject":"londontube~Baker_Street","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Bond_Street')","label":"Bond Street","subjectId":"londontube~Bond_Street"},"olgap_property":{"label":"Connects From","subjectId":"tfl~connectsFrom"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Baker_Street')","label":"Baker Street","subjectId":"londontube~Baker_Street"}},{"direct":false,"object":"londontube~Green_Park","property":"tfl~connectsFrom","subject":"londontube~Bond_Street","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Green_Park')","label":"Green Park","subjectId":"londontube~Green_Park"},"olgap_property":{"label":"Connects From","subjectId":"tfl~connectsFrom"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Bond_Street')","label":"Bond Street","subjectId":"londontube~Bond_Street"}},{"direct":false,"object":"londontube~Westminster","property":"tfl~connectsFrom","subject":"londontube~Green_Park","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Westminster')","label":"Westminster","subjectId":"londontube~Westminster"},"olgap_property":{"label":"Connects From","subjectId":"tfl~connectsFrom"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Green_Park')","label":"Green Park","subjectId":"londontube~Green_Park"}},{"direct":false,"object":"londontube~Waterloo","property":"tfl~connectsFrom","subject":"londontube~Westminster","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Waterloo')","label":"Waterloo","subjectId":"londontube~Waterloo"},"olgap_property":{"label":"Connects From","subjectId":"tfl~connectsFrom"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Westminster')","label":"Westminster","subjectId":"londontube~Westminster"}},{"direct":false,"object":"londontube~Bank","property":"tfl~connectsFrom","subject":"londontube~Waterloo","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Bank')","label":"Bank","subjectId":"londontube~Bank"},"olgap_property":{"label":"Connects From","subjectId":"tfl~connectsFrom"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Waterloo')","label":"Waterloo","subjectId":"londontube~Waterloo"}},{"direct":false,"object":"londontube~Liverpool_Street","property":"tfl~connectsTo","subject":"londontube~Bank","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Liverpool_Street')","label":"Liverpool Street","subjectId":"londontube~Liverpool_Street"},"olgap_property":{"label":"Connects To","subjectId":"tfl~connectsTo"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Bank')","label":"Bank","subjectId":"londontube~Bank"}},{"direct":false,"object":"londontube~Aldgate","property":"tfl~connectsFrom","subject":"londontube~Liverpool_Street","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Aldgate')","label":"Aldgate","subjectId":"londontube~Aldgate"},"olgap_property":{"label":"Connects From","subjectId":"tfl~connectsFrom"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Liverpool_Street')","label":"Liverpool Street","subjectId":"londontube~Liverpool_Street"}},{"direct":false,"object":"londontube~Tower_Hill","property":"tfl~connectsFrom","subject":"londontube~Aldgate","olgap_object":{"@odata.id":"rdfs_Resource('londontube~Tower_Hill')","label":"Tower Hill","subjectId":"londontube~Tower_Hill"},"olgap_property":{"label":"Connects From","subjectId":"tfl~connectsFrom</t>
     </r>
@@ -442,7 +431,6 @@
         <sz val="10"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"},"olgap_subject":{"@odata.id":"rdfs_Resource('londontube~Aldgate')","label":"Aldgate","subjectId":"londontube~Aldgate"}}]}</t>
     </r>
@@ -471,7 +459,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_Triangles","value":[{"triangles":</t>
     </r>
@@ -481,7 +468,6 @@
         <color rgb="FF000000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -491,7 +477,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">555</t>
     </r>
@@ -500,7 +485,6 @@
         <sz val="10"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,"trianglesService":"j0~tfl"}]}</t>
     </r>
@@ -517,7 +501,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#olgap_DegreeDistribution","value":[{"count":</t>
     </r>
@@ -527,7 +510,6 @@
         <color rgb="FF000000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
     </r>
@@ -537,7 +519,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">901,"degree":1,"degreeDistributionService":"UNDEF"},{"count":701,"degree":2,"degreeDistributionService":"UNDEF"},{"count":4,"degree":3,"degreeDistributionService":"UNDEF"},{"count":17,"degree":4,"degreeDistributionService":"UNDEF"},{"count":11,"degree":5,"degreeDistributionService":"UNDEF"},{"count":17,"degree":6,"degreeDistributionService":"UNDEF"},{"count":5,"degree":7,"degreeDistributionService":"UNDEF"},{"count":2,"degree":8,"degreeDistributionService":"UNDEF"},{"count":5,"degree":9,"degreeDistributionService":"UNDEF"},{"count":4,"degree":11,"degreeDistributionService":"UNDEF"},{"count":1,"degree":13,"degreeDistributionService":"UNDEF"},{"count":1,"degree":14,"degreeDistributionService":"UNDEF"},{"count":37,"degree":16,"degreeDistributionService":"UNDEF"},{"count":335,"degree":18,"degreeDistributionService":"UNDEF"},{"count":76,"degree":20,"degreeDistributionService":"UNDEF"},{"count":2,"degree":21,"degreeDistributionService":"UNDEF"},{"count":34,"degree":22,"degreeDistributionService":"UNDEF"},{"count":1,"degree":23,"degreeDistributionService":"UNDEF"},{"count":80,"degree":24,"degreeDistributionService":"UNDEF"},{"count":1,"degree":25,"degreeDistributionService":"UNDEF"},{"count":31</t>
     </r>
@@ -546,7 +527,6 @@
         <sz val="10"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,"degree":26,"degreeDistributionService":"UNDEF"},{"count":2,"degree":27,"degreeDistributionService":"UNDEF"},{"count":13,"degree":28,"degreeDistributionService":"UNDEF"},{"count":2,"degree":29,"degreeDistributionService":"UNDEF"},{"count":12,"degree":30,"degreeDistributionService":"UNDEF"},{"count":7,"degree":32,"degreeDistributionService":"UNDEF"},{"count":5,"degree":34,"degreeDistributionService":"UNDEF"},{"count":3,"degree":36,"degreeDistributionService":"UNDEF"},{"count":3,"degree":38,"degreeDistributionService":"UNDEF"},{"count":2,"degree":42,"degreeDistributionService":"UNDEF"},{"count":1,"degree":44,"degreeDistributionService":"UNDEF"},{"count":2,"degree":45,"degreeDistributionService":"UNDEF"},{"count":1,"degree":48,"degreeDistributionService":"UNDEF"},{"count":1,"degree":49,"degreeDistributionService":"UNDEF"},{"count":1,"degree":50,"degreeDistributionService":"UNDEF"},{"count":1,"degree":52,"degreeDistributionService":"UNDEF"},{"count":1,"degree":53,"degreeDistributionService":"UNDEF"},{"count":1,"degree":57,"degreeDistributionService":"UNDEF"},{"count":1,"degree":61,"degreeDistributionService":"UNDEF"},{"count":1,"degree":67,"degreeDistributionService":"UNDEF"},{"count":1,"degree":69,"degreeDistributionService":"UNDEF"},{"count":1,"degree":73,"degreeDistributionService":"UNDEF"},{"count":1,"degree":81,"degreeDistributionService":"UNDEF"},{"count":1,"degree":91,"degreeDistributionService":"UNDEF"},{"count":1,"degree":93,"degreeDistributionService":"UNDEF"},{"count":1,"degree":101,"degreeDistributionService":"UNDEF"},{"count":1,"degree":103,"degreeDistributionService":"UNDEF"},{"count":1,"degree":107,"degreeDistributionService":"UNDEF"},{"count":1,"degree":109,"degreeDistributionService":"UNDEF"},{"count":1,"degree":123,"degreeDistributionService":"UNDEF"},{"count":1,"degree":137,"degreeDistributionService":"UNDEF"},{"count":1,"degree":145,"degreeDistributionService":"UNDEF"},{"count":1,"degree":163,"degreeDistributionService":"UNDEF"},{"count":1,"degree":203,"degreeDistributionService":"UNDEF"},{"count":1,"degree":215,"degreeDistributionService":"UNDEF"},{"count":1,"degree":225,"degreeDistributionService":"UNDEF"},{"count":1,"degree":299,"degreeDistributionService":"UNDEF"},{"count":1,"degree":305,"degreeDistributionService":"UNDEF"},{"count":1,"degree":353,"degreeDistributionService":"UNDEF"},{"count":1,"degree":1295,"degreeDistributionService":"UNDEF"}]}</t>
     </r>
@@ -614,7 +594,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#search_PathEntitySearch(direct,edge,entityA,entityB,formattedValueA,formattedValueB,object,property,subject,typeA,typeB)","value":[{"@odata.id":"search_PathEntitySearch(entityA='NWD~Order-10477',entityB='NWD~Order-10491',object='NWD~</t>
     </r>
@@ -624,7 +603,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Order-10366',property='northwind~shipVia',subject='NWD~Shipper-2',typeA='northwind~Order',typeB='northwind~Order')","direct":false,"edge":2,"entityA":"NWD~Order-10477","entityB":"NWD~Order-10491","formattedValueA":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship name:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;Princesa &lt;B&gt;Isabel&lt;/B&gt; Vinhos&lt;/td&gt;&lt;/tr&gt;","formattedValueB":"&lt;tr&gt;&lt;td&gt;&lt;i&gt;ship country:&lt;/i&gt;&lt;/td&gt;&lt;td&gt;&lt;B&gt;Portugal&lt;/B&gt;&lt;/td&gt;&lt;/tr&gt;","object":"NWD~Order-10366","property":"northwind~shipVia","subject":"NWD~Shipper-2</t>
     </r>
@@ -633,7 +611,6 @@
         <sz val="10"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">","typeA":"northwind~Order","typeB":"northwind~Order"}]}</t>
     </r>
@@ -662,7 +639,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#contextmenu_Types","value":[{"entity":"NWD~OrderDetail-10255-16","type":"</t>
     </r>
@@ -672,7 +648,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">northwind~OrderDetail"},{"entity":"UNDEF","type":"rdfs~Resource</t>
     </r>
@@ -681,7 +656,6 @@
         <sz val="10"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"}]}</t>
     </r>
@@ -698,7 +672,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/ODATA2SPARQL/$metadata#contextmenu_</t>
     </r>
@@ -708,7 +681,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ClassNextIndex","value":[{"class":"northwind~Product","indexPrefix":null,"nextIndex":78,"prefix":"Product-</t>
     </r>
@@ -717,7 +689,6 @@
         <sz val="10"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"}]}</t>
     </r>
@@ -890,7 +861,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee(employer,label,subjectId)/$entity","@odata.id":"Employee('NWD~SystemBEmployee-2')","employer"</t>
     </r>
@@ -981,7 +951,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee/$entity","birthDate":"1972-02-19","comment":null,"employeeAddress":"908 W. Capital Way","employeeCity":"Tacoma","employeeCountry":"USA","employeeLinkedIn":"https://www.linkedin.com/in/peterjohnlawrence/","employeePostalCode":</t>
     </r>
@@ -1078,7 +1047,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~SystemAEmployee-1')/reportsTo/employeeSalary","systemAEmployeeSalary":</t>
     </r>
@@ -1196,7 +1164,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Employee('NWD~SystemAEmployee-1')/reportsTo/$entity","birthDate":"1972-02-19","comment":null,"employeeAddress":"908 W. Capital Way","employeeCity":"Tacoma","employeeCountry":"USA","employeeLinkedIn":"https://www.linkedin.com/in/peterjohnlawrence/","employeePostalCode":"98401","employeeSalary"</t>
     </r>
@@ -1608,7 +1575,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order(employee(reportsTo()))/$entity","comment":null,"customerId":"NWD~Customer-TOMSP","customerNotation":null,"employeeId":"NWD~Employee-6","employeeNotation":null,"freight":11.61,"label":"Order-10249","lat":51.6566,"lat_long":"51.6566000,7.0904400","long":7.09044,"orderDate":"2016-07-05T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-08-16T00:00:00Z","shipAddress":"Luisenstr. 48","shipCity":"Münster","shipCountry":"Germany","shipName":"Toms Spezialitäten","shipPostalCode":"44087","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2016-07-10T00:00:00Z","subjectId":"NWD~Order-10249","employee":{"birthDate":"1983-07-02","comment":null,"employeeAddress":"Coventry House\\nMiner Rd.","employeeCity":"London","employeeCountry":"UK","employeeLinkedIn":null,"employeePostalCode":"EC2 7JR","employeeSalary":null,"employer":null,"extension":"428","favorite":null,"firstName":"Michael","hireDate":"2013-10-17","homePhone":"(71) 555-7773","label":"Employee-6","lastName":"Suyama","lat":51.5100082,"lat_long":"51.5100082,-0.1329494","long":-0.1329494,"notes":"Michael is a graduate of Sussex University (MA, economics, 1983) and the University of California at Los Angeles (MBA, marketing, 1986). He has also taken the courses Multi-Cultural Selling and Time Management for the Sales Professional. He is fluent in Japanese and can read and write French, Portuguese, and Spanish.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-5","reportsToNotation":null,"subjectId":"NWD~Employee-6","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Mr.","reportsTo":{"birthDate":</t>
     </r>
@@ -1651,7 +1617,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order(employee(reportsTo()),shipVia())/$entity","comment":null,"customerId":"NWD~Customer-TOMSP","customerNotation":null,"employeeId":"NWD~Employee-6","employeeNotation":null,"freight":11.61,"label":"Order-10249","lat":51.6566,"lat_long":"51.6566000,7.0904400","long":7.09044,"orderDate":"2016-07-05T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-08-16T00:00:00Z","shipAddress":"Luisenstr. 48","shipCity":"Münster","shipCountry":"Germany","shipName":"Toms Spezialitäten","shipPostalCode":"44087","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2016-07-10T00:00:00Z","subjectId":"NWD~Order-10249","employee":{"birthDate":"1983-07-02","comment":null,"employeeAddress":"Coventry House\\nMiner Rd.","employeeCity":"London","employeeCountry":"UK","employeeLinkedIn":null,"employeePostalCode":"EC2 7JR","employeeSalary":null,"employer":null,"extension":"428","favorite":null,"firstName":"Michael","hireDate":"2013-10-17","homePhone":"(71) 555-7773","label":"Employee-6","lastName":"Suyama","lat":51.5100082,"lat_long":"51.5100082,-0.1329494","long":-0.1329494,"notes":"Michael is a graduate of Sussex University (MA, economics, 1983) and the University of California at Los Angeles (MBA, marketing, 1986). He has also taken the courses Multi-Cultural Selling and Time Management for the Sales Professional. He is fluent in Japanese and can read and write French, Portuguese, and Spanish.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-5","reportsToNotation":null,"subjectId":"NWD~Employee-6","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Mr.","reportsTo":{"birthDate":</t>
     </r>
@@ -1685,7 +1650,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order(employee(reportsTo(reportsTo())))/$entity","comment":null,"customerId":"NWD~Customer-TOMSP","customerNotation":null,"employeeId":"NWD~Employee-</t>
     </r>
@@ -1695,7 +1659,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">6","employeeNotation":null,"freight":11.61,"label":"Order-10249","lat":51.6566,"lat_long":"51.6566000,7.0904400","long":7.09044,"orderDate":"2016-07-05T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-08-16T00:00:00Z","shipAddress":"Luisenstr. 48","shipCity":"Münster","shipCountry":"Germany","shipName":"Toms Spezialitäten","shipPostalCode":"44087","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2016-07-10T00:00:00Z","subjectId":"NWD~Order-10249","employee":{"birthDate":"1983-07-02","comment":null,"employeeAddress":"Coventry House\\nMiner Rd.","employeeCity":"London","employeeCountry":"UK","employeeLinkedIn":null,"employeePostalCode":"EC2 7JR","employeeSalary":null,"employer":null,"extension":"428","favorite":null,"firstName":"Michael","hireDate":"2013-10-17","homePhone":"(71) 555-7773","label":"Employee-6","lastName":"Suyama","lat":51.5100082,"lat_long":"51.5100082,-0.1329494","long":-0.1329494,"notes":"Michael is a graduate of Sussex University (MA, economics, 1983) and the University of California at Los Angeles (MBA, marketing, 1986). He has also taken the courses Multi-Cultural Selling and Time Management for the Sales Professional. He is fluent in Japanese and can read and write French, Portuguese, and Spanish.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-5","reportsToNotation":null,"subjectId":"NWD~Employee-6","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Mr.","reportsTo":{"birthDate":"1972-02-19","comment":null,"employeeAddress":"908 W. Capital Way","employeeCity":"Tacoma","employeeCountry":"USA","employeeLinkedIn":"https://www.linkedin.com/in/peterjohnlawrence/","employeePostalCode":"98401","employeeSalary":null,"employer":null,"extension":"3457","favorite":null,"firstName":"Andrew","hireDate":"2012-08-14","homePhone":"(206) 555-9482","label":"MatchingEmployee-2","lastName":"Fuller","lat":null,"lat_long":null,"long":null,"notes":"Andrew received his BTS commercial in 1974 and a Ph.D. in international marketing from the University of Dallas in 1981. He is fluent in French and Italian and reads German. He joined the company as a sales representative, was promoted to sales manager in January 1992 and to vice president of sales in March 1993. Andrew is a member of the Sales Management Roundtable, the Seattle Chamber of Commerce, and the Pacific Rim Importers Association.","photo":"http://accweb/emmployees/fuller.bmp","regionDescription":null,"reportsToId":"NWD~Employee-5","reportsToNotation":null,"subjectId":"NWD~MatchingEmployee-2","territoryNotation":null,"title":"Vice President, Sales","titleOfCourtesy":"Doctor","reportsTo":{"birthDate":"1975-03-04","comment":null,"employeeAddress":"14 Garrett Hill","employeeCity":"London","employeeCountry":"UK","employeeLinkedIn":null,"employeePostalCode":"SW1 8JR","employeeSalary":null,"employer":null,"extension":"3453","favorite":null,"firstName":"Steven","hireDate":"2013-10-17","homePhone":"(71) 555-4848","label":"Employee-5","lastName":"Buchanan","lat":51.5239508,"lat_long":"51.5239508,-0.0944701","long":-0.0944701,"notes":"Steven Buchanan graduated from St. Andrews University, Scotland, with a BSC degree in 1976. Upon joining the company as a sales representative in 1992, he spent 6 months in an orientation program at the Seattle office and then returned to his permanent post in London. He was promoted to sales manager in March 1993. Mr. Buchanan has completed the courses Successful Telemarketing and International Sales Management. He is fluent in French.","photo":"http://accweb/emmployees/buchanan.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-5","territoryNotation":null,"title":"Sales Manager","titleOfCourtesy":"Mr."}</t>
     </r>
@@ -1705,7 +1668,6 @@
         <color rgb="FF000000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">}}}</t>
     </r>
@@ -1992,7 +1954,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">42</t>
     </r>
@@ -2002,7 +1963,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.0</t>
     </r>
@@ -2622,7 +2582,6 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order(employee(),customer())","value":[{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-4","employeeNotation":null,"freight":108.26,"label":"Order-10337","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2016-10-24T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2016-11-21T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2016-10-29T00:00:00Z","subjectId":"NWD~Order-10337","employee":{"birthDate":"1957-09-19","comment":null,"employeeAddress":"4110 Old Redmond Rd.","employeeCity":"Redmond","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98052","employeeSalary":null,"employer":null,"extension":"5176","favorite":null,"firstName":"Margaret","hireDate":"2013-05-03","homePhone":"(206) 555-8122","label":"Employee-4","lastName":"Peacock","lat":47.6679429,"lat_long":"47.6679429,-122.1334222","long":-122.1334222,"notes":"Margaret holds a BA in English literature from Concordia College (1958) and an MA from the American Institute of Culinary Arts (1966). She was assigned to the London office temporarily from July through November 1992.","photo":"http://accweb/emmployees/peacock.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-4","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Mrs."},"customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-</t>
     </r>
@@ -2632,7 +2591,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Consolas"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">8","employeeNotation":null,"freight":97.18,"label":"Order-10623","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2017-08-07T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-04T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2017-08-12T00:00:00Z","subjectId":"NWD~Order-10623","employee":{"birthDate":"1978-01-09","comment":null,"employeeAddress":"4726 - 11th Ave. N.E.","employeeCity":"Seattle","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98105","employeeSalary":null,"employer":null,"extension":"2344","favorite":null,"firstName":"Laura","hireDate":"2014-03-05","homePhone":"(206) 555-1189","label":"Employee-8","lastName":"Callahan","lat":47.6641642,"lat_long":"47.6641642,-122.3160149","long":-122.3160149,"notes":"Laura received a BA in psychology from the University of Washington. She has also completed a course in business French. She reads and writes French.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-8","territoryNotation":null,"title":"Inside Sales Coordinator","titleOfCourtesy":"Ms."},"customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":93.25,"label":"Order-10653","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2017-09-02T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2017-09-30T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-1","shipViaNotation":null,"shippedDate":"2017-09-19T00:00:00Z","subjectId":"NWD~Order-10653","employee":{"birthDate":"1968-12-08","comment":null,"employeeAddress":"507 - 20th Ave. E.\\nApt. 2A","employeeCity":"Seattle","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98122","employeeSalary":null,"employer":null,"extension":"5467","favorite":null,"firstName":"Nancy","hireDate":"2012-05-01","homePhone":"(206) 555-9857","label":"Employee-1","lastName":"Davolio","lat":47.6234778,"lat_long":"47.6234778,-122.3063220","long":-122.306322,"notes":"Education includes a BA in psychology from Colorado State University in 1970. She also completed The Art of the Cold Call. Nancy is a member of Toastmasters International.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-1","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Ms."},"customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-6","employeeNotation":null,"freight":16.85,"label":"Order-10791","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2017-12-23T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2018-01-20T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-2","shipViaNotation":null,"shippedDate":"2018-01-01T00:00:00Z","subjectId":"NWD~Order-10791","employee":{"birthDate":"1983-07-02","comment":null,"employeeAddress":"Coventry House\\nMiner Rd.","employeeCity":"London","employeeCountry":"UK","employeeLinkedIn":null,"employeePostalCode":"EC2 7JR","employeeSalary":null,"employer":null,"extension":"428","favorite":null,"firstName":"Michael","hireDate":"2013-10-17","homePhone":"(71) 555-7773","label":"Employee-6","lastName":"Suyama","lat":51.5100082,"lat_long":"51.5100082,-0.1329494","long":-0.1329494,"notes":"Michael is a graduate of Sussex University (MA, economics, 1983) and the University of California at Los Angeles (MBA, marketing, 1986). He has also taken the courses Multi-Cultural Selling and Time Management for the Sales Professional. He is fluent in Japanese and can read and write French, Portuguese, and Spanish.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-5","reportsToNotation":null,"subjectId":"NWD~Employee-6","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Mr."},"customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}},{"comment":null,"customerId":"NWD~Customer-FRANK","customerNotation":null,"employeeId":"NWD~Employee-1","employeeNotation":null,"freight":242.95,"label":"Order-11012","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"orderDate":"2018-04-09T00:00:00Z","orderRegionId":null,"regionDescription":null,"requiredDate":"2018-04-23T00:00:00Z","shipAddress":"Berliner Platz 43","shipCity":"München","shipCountry":"Germany","shipName":"Frankenversand","shipPostalCode":"80805","shipViaId":"NWD~Shipper-3","shipViaNotation":null,"shippedDate":"2018-04-17T00:00:00Z","subjectId":"NWD~Order-11012","employee":{"birthDate":"1968-12-08","comment":null,"employeeAddress":"507 - 20th Ave. E.\\nApt. 2A","employeeCity":"Seattle","employeeCountry":"USA","employeeLinkedIn":null,"employeePostalCode":"98122","employeeSalary":null,"employer":null,"extension":"5467","favorite":null,"firstName":"Nancy","hireDate":"2012-05-01","homePhone":"(206) 555-9857","label":"Employee-1","lastName":"Davolio","lat":47.6234778,"lat_long":"47.6234778,-122.3063220","long":-122.306322,"notes":"Education includes a BA in psychology from Colorado State University in 1970. She also completed The Art of the Cold Call. Nancy is a member of Toastmasters International.","photo":"http://accweb/emmployees/davolio.bmp","regionDescription":null,"reportsToId":"NWD~Employee-2","reportsToNotation":null,"subjectId":"NWD~Employee-1","territoryNotation":null,"title":"Sales Representative","titleOfCourtesy":"Ms."},"customer":{"comment":null,"customerAddress":"Berliner Platz 43","customerCity":"München","customerCompanyName":"Frankenversand","customerContactName":"Peter Franken","customerContactTitle":"Marketing Manager","customerCountry":"Germany","customerFax":"089-0877451","customerPhone":"089-0877310","customerPostalCode":"80805","customerWebsite":null,"label":"Frankenversand","lat":48.1730861,"lat_long":"48.1730861,11.5879194","long":11.5879194,"regionDescription":null,"subjectId":"NWD~Customer-FRANK"}}]}</t>
     </r>
@@ -2671,7 +2629,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order","value":[{"comment":null,"customerId":"NWD~Customer-</t>
     </r>
@@ -2704,7 +2661,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"</t>
     </r>
@@ -2724,7 +2680,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">","value":[{"comment":null,"customerId":"NWD~Customer-WANDK","customerNotation":null,"employeeId":"NWD~Employee-</t>
     </r>
@@ -2757,7 +2712,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order","value":[{"comment":null,"customerId":"NWD~Customer-</t>
     </r>
@@ -2790,7 +2744,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order","value":[{"comment":null,"customerId":"NWD~Customer-</t>
     </r>
@@ -2823,7 +2776,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{"@odata.context":"http://localhost:8080/odata2sparql/northwind/$metadata#Order","value"</t>
     </r>
@@ -2872,12 +2824,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2899,33 +2850,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Consolas"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Consolas"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2935,6 +2859,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="0"/>
     </font>
@@ -3034,11 +2964,11 @@
   </sheetPr>
   <dimension ref="A1:K249"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G89" activeCellId="0" sqref="G89"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H45" activeCellId="0" sqref="H45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.86"/>
@@ -3046,8 +2976,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="50.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="121.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="50.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="68.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="89.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="36.84"/>

</xml_diff>